<commit_message>
Moved hard coded parameters to spreadsheet
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.palmer/Documents/GitHub/covasim-australia/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anna.palmer/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B166517-943D-AD44-9363-737BEE7CB166}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{218098B0-849A-2D4F-87F8-C814B4F01D68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18360" yWindow="3100" windowWidth="28040" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22780" yWindow="13600" windowWidth="25600" windowHeight="15540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data" sheetId="1" r:id="rId1"/>
     <sheet name="contact matrices-home" sheetId="2" r:id="rId2"/>
     <sheet name="age_sex" sheetId="3" r:id="rId3"/>
     <sheet name="households" sheetId="4" r:id="rId4"/>
+    <sheet name="layers" sheetId="5" r:id="rId5"/>
+    <sheet name="other_par" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="209">
   <si>
     <t>date</t>
   </si>
@@ -522,6 +524,144 @@
   </si>
   <si>
     <t>6+ persons</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>contacts</t>
+  </si>
+  <si>
+    <t>beta_layer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>quar_eff</t>
+  </si>
+  <si>
+    <t>proportion</t>
+  </si>
+  <si>
+    <t>age_lb</t>
+  </si>
+  <si>
+    <t>age_ub</t>
+  </si>
+  <si>
+    <t>cluster_type</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>Church</t>
+  </si>
+  <si>
+    <t>church</t>
+  </si>
+  <si>
+    <t>pSport</t>
+  </si>
+  <si>
+    <t>beach_goer</t>
+  </si>
+  <si>
+    <t>beach goers</t>
+  </si>
+  <si>
+    <t>professional sports players</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>general community</t>
+  </si>
+  <si>
+    <t>complete</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>pop_size</t>
+  </si>
+  <si>
+    <t>pop_scale</t>
+  </si>
+  <si>
+    <t>rescale</t>
+  </si>
+  <si>
+    <t>rescale_threshold</t>
+  </si>
+  <si>
+    <t>pop_infected</t>
+  </si>
+  <si>
+    <t>population size (this will be scaled)</t>
+  </si>
+  <si>
+    <t>scale factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fraction of susceptible population that will trigger rescaling </t>
+  </si>
+  <si>
+    <t>Number of initial infections</t>
+  </si>
+  <si>
+    <t>rescale_factor</t>
+  </si>
+  <si>
+    <t>start_day</t>
+  </si>
+  <si>
+    <t>end_day</t>
+  </si>
+  <si>
+    <t>start date of simulation</t>
+  </si>
+  <si>
+    <t>end date of simulation</t>
+  </si>
+  <si>
+    <t>n_runs</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>trace_probs</t>
+  </si>
+  <si>
+    <t>trace_time</t>
+  </si>
+  <si>
+    <t>undiag</t>
+  </si>
+  <si>
+    <t>Proportion of cases that are undiagnosed</t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1268,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1164,6 +1304,9 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1525,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -6007,4 +6150,434 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98290782-EDB5-8E49-BAFB-76C1B5158EA7}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="K1" s="19" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>110</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>110</v>
+      </c>
+      <c r="J3">
+        <v>0.8</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>0.5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>110</v>
+      </c>
+      <c r="J4">
+        <v>0.5</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>110</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>178</v>
+      </c>
+      <c r="B6" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>0.5</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.1</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>110</v>
+      </c>
+      <c r="I6" t="s">
+        <v>186</v>
+      </c>
+      <c r="J6">
+        <v>0.05</v>
+      </c>
+      <c r="K6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.01</v>
+      </c>
+      <c r="G7">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>186</v>
+      </c>
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.3</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>110</v>
+      </c>
+      <c r="I8" t="s">
+        <v>187</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>188</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="24">
+        <v>43891</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="24">
+        <v>44105</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="23" t="s">
+        <v>203</v>
+      </c>
+      <c r="B4" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B5">
+        <v>20000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>192</v>
+      </c>
+      <c r="B8">
+        <v>0.8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11">
+        <v>3.5000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B12">
+        <v>0.3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>208</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
WIP creating policies from input sheet
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dominic.delport\Documents\GitHub\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164FE0F0-0E60-4679-9C0F-EEACF52334D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61153C6-91AA-439A-9B63-165CC34A430A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,14 @@
     <sheet name="policies" sheetId="7" r:id="rId6"/>
     <sheet name="other_par" sheetId="6" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -825,7 +827,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="270">
   <si>
     <t>date</t>
   </si>
@@ -1632,14 +1634,18 @@
   </si>
   <si>
     <t>Change in baseline transmission risk for each network, relative to baseline</t>
+  </si>
+  <si>
+    <t>Date ended/replaced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="34" x14ac:knownFonts="1">
     <font>
@@ -2344,7 +2350,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2492,6 +2498,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2501,7 +2510,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2553,28 +2565,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b val="0"/>
@@ -2913,24 +2904,24 @@
       <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.796875" style="22"/>
+    <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="2" max="2" width="14.5" style="7" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="14.19921875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="13" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.796875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="14.19921875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="7" customWidth="1"/>
     <col min="8" max="8" width="14.5" style="7" customWidth="1"/>
     <col min="9" max="9" width="16" style="7" customWidth="1"/>
     <col min="10" max="10" width="14" style="7" customWidth="1"/>
-    <col min="11" max="11" width="14.69921875" style="7" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" style="7" customWidth="1"/>
     <col min="12" max="12" width="20" style="7" customWidth="1"/>
-    <col min="13" max="16384" width="10.796875" style="7"/>
+    <col min="13" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +2959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="21">
         <v>43891</v>
       </c>
@@ -2988,7 +2979,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="21">
         <v>43892</v>
       </c>
@@ -3008,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="21">
         <v>43893</v>
       </c>
@@ -3028,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="21">
         <v>43894</v>
       </c>
@@ -3048,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="21">
         <v>43895</v>
       </c>
@@ -3068,7 +3059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="21">
         <v>43896</v>
       </c>
@@ -3088,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="21">
         <v>43897</v>
       </c>
@@ -3108,7 +3099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="21">
         <v>43898</v>
       </c>
@@ -3128,7 +3119,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="21">
         <v>43899</v>
       </c>
@@ -3148,7 +3139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="21">
         <v>43900</v>
       </c>
@@ -3168,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="21">
         <v>43901</v>
       </c>
@@ -3188,7 +3179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="21">
         <v>43902</v>
       </c>
@@ -3208,7 +3199,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="21">
         <v>43903</v>
       </c>
@@ -3228,7 +3219,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="21">
         <v>43904</v>
       </c>
@@ -3248,7 +3239,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="21">
         <v>43905</v>
       </c>
@@ -3268,7 +3259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="21">
         <v>43906</v>
       </c>
@@ -3294,7 +3285,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="21">
         <v>43907</v>
       </c>
@@ -3323,7 +3314,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="21">
         <v>43908</v>
       </c>
@@ -3352,7 +3343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="21">
         <v>43909</v>
       </c>
@@ -3381,7 +3372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="21">
         <v>43910</v>
       </c>
@@ -3410,7 +3401,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="21">
         <v>43911</v>
       </c>
@@ -3439,7 +3430,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="21">
         <v>43912</v>
       </c>
@@ -3468,7 +3459,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="21">
         <v>43913</v>
       </c>
@@ -3503,7 +3494,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="21">
         <v>43914</v>
       </c>
@@ -3535,7 +3526,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="21">
         <v>43915</v>
       </c>
@@ -3567,7 +3558,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="21">
         <v>43916</v>
       </c>
@@ -3599,7 +3590,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="21">
         <v>43917</v>
       </c>
@@ -3631,7 +3622,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="21">
         <v>43918</v>
       </c>
@@ -3663,7 +3654,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="21">
         <v>43919</v>
       </c>
@@ -3701,7 +3692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="21">
         <v>43920</v>
       </c>
@@ -3736,7 +3727,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="21">
         <v>43921</v>
       </c>
@@ -3774,7 +3765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="21">
         <v>43922</v>
       </c>
@@ -3812,7 +3803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="21">
         <v>43923</v>
       </c>
@@ -3850,7 +3841,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="21">
         <v>43924</v>
       </c>
@@ -3888,7 +3879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="21">
         <v>43925</v>
       </c>
@@ -3926,7 +3917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="21">
         <v>43926</v>
       </c>
@@ -3964,7 +3955,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="21">
         <v>43927</v>
       </c>
@@ -4002,7 +3993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="21">
         <v>43928</v>
       </c>
@@ -4040,7 +4031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="21">
         <v>43929</v>
       </c>
@@ -4078,7 +4069,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="21">
         <v>43930</v>
       </c>
@@ -4116,7 +4107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="21">
         <v>43931</v>
       </c>
@@ -4154,7 +4145,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="21">
         <v>43932</v>
       </c>
@@ -4192,7 +4183,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="21">
         <v>43933</v>
       </c>
@@ -4230,7 +4221,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="21">
         <v>43934</v>
       </c>
@@ -4268,7 +4259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="21">
         <v>43935</v>
       </c>
@@ -4306,7 +4297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="21">
         <v>43936</v>
       </c>
@@ -4344,7 +4335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="21">
         <v>43937</v>
       </c>
@@ -4382,7 +4373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="21">
         <v>43938</v>
       </c>
@@ -4420,7 +4411,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="21">
         <v>43939</v>
       </c>
@@ -4458,7 +4449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="21">
         <v>43940</v>
       </c>
@@ -4496,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="21">
         <v>43941</v>
       </c>
@@ -4534,7 +4525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="21">
         <v>43942</v>
       </c>
@@ -4585,9 +4576,9 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -4643,7 +4634,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -4699,7 +4690,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -4752,7 +4743,7 @@
         <v>4.3559999999999996E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -4805,7 +4796,7 @@
         <v>4.1580000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -4858,7 +4849,7 @@
         <v>3.0739999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -4911,7 +4902,7 @@
         <v>3.6970000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -4964,7 +4955,7 @@
         <v>6.8170000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -5017,7 +5008,7 @@
         <v>3.594E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -5070,7 +5061,7 @@
         <v>2.7920000000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -5123,7 +5114,7 @@
         <v>6.6759999999999996E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -5176,7 +5167,7 @@
         <v>1.2394000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -5229,7 +5220,7 @@
         <v>2.0105999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -5282,7 +5273,7 @@
         <v>2.0524000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -5335,7 +5326,7 @@
         <v>5.2319999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -5388,7 +5379,7 @@
         <v>1.4578000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -5441,7 +5432,7 @@
         <v>9.6379000000000006E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -5529,12 +5520,12 @@
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="10.796875" style="8"/>
+    <col min="1" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>153</v>
       </c>
@@ -5551,7 +5542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
@@ -5569,7 +5560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -5587,7 +5578,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>38</v>
       </c>
@@ -5602,7 +5593,7 @@
         <v>53807</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>39</v>
       </c>
@@ -5617,7 +5608,7 @@
         <v>54603</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>40</v>
       </c>
@@ -5632,7 +5623,7 @@
         <v>53380</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -5647,7 +5638,7 @@
         <v>52236</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
@@ -5662,7 +5653,7 @@
         <v>52696</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>43</v>
       </c>
@@ -5677,7 +5668,7 @@
         <v>51199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
@@ -5692,7 +5683,7 @@
         <v>51198</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>45</v>
       </c>
@@ -5707,7 +5698,7 @@
         <v>50836</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
@@ -5722,7 +5713,7 @@
         <v>49144</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
@@ -5737,7 +5728,7 @@
         <v>47266</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
@@ -5752,7 +5743,7 @@
         <v>46880</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>49</v>
       </c>
@@ -5767,7 +5758,7 @@
         <v>46060</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
@@ -5782,7 +5773,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>51</v>
       </c>
@@ -5797,7 +5788,7 @@
         <v>45958</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -5812,7 +5803,7 @@
         <v>47505</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>53</v>
       </c>
@@ -5827,7 +5818,7 @@
         <v>47748</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>54</v>
       </c>
@@ -5842,7 +5833,7 @@
         <v>51641</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>55</v>
       </c>
@@ -5857,7 +5848,7 @@
         <v>57079</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
         <v>56</v>
       </c>
@@ -5872,7 +5863,7 @@
         <v>60111</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>57</v>
       </c>
@@ -5887,7 +5878,7 @@
         <v>62268</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>58</v>
       </c>
@@ -5902,7 +5893,7 @@
         <v>62979</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
         <v>59</v>
       </c>
@@ -5917,7 +5908,7 @@
         <v>65013</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="9" t="s">
         <v>60</v>
       </c>
@@ -5932,7 +5923,7 @@
         <v>65746</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="9" t="s">
         <v>61</v>
       </c>
@@ -5947,7 +5938,7 @@
         <v>67618</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="9" t="s">
         <v>62</v>
       </c>
@@ -5962,7 +5953,7 @@
         <v>69532</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="9" t="s">
         <v>63</v>
       </c>
@@ -5977,7 +5968,7 @@
         <v>68855</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="9" t="s">
         <v>64</v>
       </c>
@@ -5992,7 +5983,7 @@
         <v>70345</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="9" t="s">
         <v>65</v>
       </c>
@@ -6007,7 +5998,7 @@
         <v>69062</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="9" t="s">
         <v>66</v>
       </c>
@@ -6022,7 +6013,7 @@
         <v>70909</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="9" t="s">
         <v>67</v>
       </c>
@@ -6037,7 +6028,7 @@
         <v>70590</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="9" t="s">
         <v>68</v>
       </c>
@@ -6052,7 +6043,7 @@
         <v>70286</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="9" t="s">
         <v>69</v>
       </c>
@@ -6067,7 +6058,7 @@
         <v>70326</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>70</v>
       </c>
@@ -6082,7 +6073,7 @@
         <v>68170</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>71</v>
       </c>
@@ -6097,7 +6088,7 @@
         <v>66194</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>72</v>
       </c>
@@ -6112,7 +6103,7 @@
         <v>63654</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>73</v>
       </c>
@@ -6127,7 +6118,7 @@
         <v>61073</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>74</v>
       </c>
@@ -6142,7 +6133,7 @@
         <v>58823</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="9" t="s">
         <v>75</v>
       </c>
@@ -6157,7 +6148,7 @@
         <v>57759</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="9" t="s">
         <v>76</v>
       </c>
@@ -6172,7 +6163,7 @@
         <v>57893</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="9" t="s">
         <v>77</v>
       </c>
@@ -6187,7 +6178,7 @@
         <v>57469</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="9" t="s">
         <v>78</v>
       </c>
@@ -6202,7 +6193,7 @@
         <v>58949</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="9" t="s">
         <v>79</v>
       </c>
@@ -6217,7 +6208,7 @@
         <v>58767</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="9" t="s">
         <v>80</v>
       </c>
@@ -6232,7 +6223,7 @@
         <v>60562</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="9" t="s">
         <v>81</v>
       </c>
@@ -6247,7 +6238,7 @@
         <v>62190</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="9" t="s">
         <v>82</v>
       </c>
@@ -6262,7 +6253,7 @@
         <v>58515</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>83</v>
       </c>
@@ -6277,7 +6268,7 @@
         <v>57148</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>84</v>
       </c>
@@ -6292,7 +6283,7 @@
         <v>55722</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="s">
         <v>85</v>
       </c>
@@ -6307,7 +6298,7 @@
         <v>52756</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
@@ -6322,7 +6313,7 @@
         <v>52691</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="s">
         <v>87</v>
       </c>
@@ -6337,7 +6328,7 @@
         <v>51198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="9" t="s">
         <v>88</v>
       </c>
@@ -6352,7 +6343,7 @@
         <v>52386</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="s">
         <v>89</v>
       </c>
@@ -6367,7 +6358,7 @@
         <v>52234</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="s">
         <v>90</v>
       </c>
@@ -6382,7 +6373,7 @@
         <v>50731</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="s">
         <v>91</v>
       </c>
@@ -6397,7 +6388,7 @@
         <v>50406</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
@@ -6412,7 +6403,7 @@
         <v>48630</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="s">
         <v>93</v>
       </c>
@@ -6427,7 +6418,7 @@
         <v>46802</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
@@ -6442,7 +6433,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="s">
         <v>95</v>
       </c>
@@ -6457,7 +6448,7 @@
         <v>44147</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
@@ -6472,7 +6463,7 @@
         <v>44057</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
@@ -6487,7 +6478,7 @@
         <v>41590</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
@@ -6502,7 +6493,7 @@
         <v>40044</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="s">
         <v>99</v>
       </c>
@@ -6517,7 +6508,7 @@
         <v>39348</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="9" t="s">
         <v>100</v>
       </c>
@@ -6532,7 +6523,7 @@
         <v>38109</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>101</v>
       </c>
@@ -6547,7 +6538,7 @@
         <v>37555</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
@@ -6562,7 +6553,7 @@
         <v>36069</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="s">
         <v>103</v>
       </c>
@@ -6577,7 +6568,7 @@
         <v>35049</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="s">
         <v>104</v>
       </c>
@@ -6592,7 +6583,7 @@
         <v>35464</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="s">
         <v>105</v>
       </c>
@@ -6607,7 +6598,7 @@
         <v>36919</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="s">
         <v>106</v>
       </c>
@@ -6622,7 +6613,7 @@
         <v>30984</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="s">
         <v>107</v>
       </c>
@@ -6637,7 +6628,7 @@
         <v>28543</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="s">
         <v>108</v>
       </c>
@@ -6652,7 +6643,7 @@
         <v>27858</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="s">
         <v>109</v>
       </c>
@@ -6667,7 +6658,7 @@
         <v>24567</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="9" t="s">
         <v>110</v>
       </c>
@@ -6682,7 +6673,7 @@
         <v>24510</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="s">
         <v>111</v>
       </c>
@@ -6697,7 +6688,7 @@
         <v>22998</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="s">
         <v>112</v>
       </c>
@@ -6712,7 +6703,7 @@
         <v>22512</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="s">
         <v>113</v>
       </c>
@@ -6727,7 +6718,7 @@
         <v>21184</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="s">
         <v>114</v>
       </c>
@@ -6742,7 +6733,7 @@
         <v>20306</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="s">
         <v>115</v>
       </c>
@@ -6757,7 +6748,7 @@
         <v>19188</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="s">
         <v>116</v>
       </c>
@@ -6772,7 +6763,7 @@
         <v>18359</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="9" t="s">
         <v>117</v>
       </c>
@@ -6787,7 +6778,7 @@
         <v>16636</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="s">
         <v>118</v>
       </c>
@@ -6802,7 +6793,7 @@
         <v>15857</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="s">
         <v>119</v>
       </c>
@@ -6817,7 +6808,7 @@
         <v>14574</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="s">
         <v>120</v>
       </c>
@@ -6832,7 +6823,7 @@
         <v>13566</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="s">
         <v>121</v>
       </c>
@@ -6847,7 +6838,7 @@
         <v>13090</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="s">
         <v>122</v>
       </c>
@@ -6862,7 +6853,7 @@
         <v>12415</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="s">
         <v>123</v>
       </c>
@@ -6877,7 +6868,7 @@
         <v>10624</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="s">
         <v>124</v>
       </c>
@@ -6892,7 +6883,7 @@
         <v>9445</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="9" t="s">
         <v>125</v>
       </c>
@@ -6907,7 +6898,7 @@
         <v>8388</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="s">
         <v>126</v>
       </c>
@@ -6922,7 +6913,7 @@
         <v>7233</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="s">
         <v>127</v>
       </c>
@@ -6937,7 +6928,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="s">
         <v>128</v>
       </c>
@@ -6952,7 +6943,7 @@
         <v>4814</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="s">
         <v>129</v>
       </c>
@@ -6967,7 +6958,7 @@
         <v>3853</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="s">
         <v>130</v>
       </c>
@@ -6982,7 +6973,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="s">
         <v>131</v>
       </c>
@@ -6997,7 +6988,7 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="s">
         <v>132</v>
       </c>
@@ -7012,7 +7003,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="s">
         <v>133</v>
       </c>
@@ -7027,7 +7018,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="s">
         <v>134</v>
       </c>
@@ -7042,7 +7033,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="9" t="s">
         <v>135</v>
       </c>
@@ -7057,7 +7048,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="s">
         <v>136</v>
       </c>
@@ -7072,7 +7063,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="s">
         <v>137</v>
       </c>
@@ -7087,7 +7078,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="s">
         <v>138</v>
       </c>
@@ -7102,7 +7093,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="s">
         <v>139</v>
       </c>
@@ -7117,7 +7108,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="9" t="s">
         <v>140</v>
       </c>
@@ -7132,7 +7123,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="s">
         <v>141</v>
       </c>
@@ -7147,7 +7138,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="s">
         <v>142</v>
       </c>
@@ -7162,7 +7153,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="s">
         <v>143</v>
       </c>
@@ -7177,7 +7168,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="s">
         <v>144</v>
       </c>
@@ -7192,7 +7183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="s">
         <v>145</v>
       </c>
@@ -7207,7 +7198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="s">
         <v>146</v>
       </c>
@@ -7222,7 +7213,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="9" t="s">
         <v>147</v>
       </c>
@@ -7237,7 +7228,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="s">
         <v>148</v>
       </c>
@@ -7252,7 +7243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="s">
         <v>149</v>
       </c>
@@ -7267,7 +7258,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="s">
         <v>150</v>
       </c>
@@ -7282,7 +7273,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="9" t="s">
         <v>151</v>
       </c>
@@ -7311,13 +7302,13 @@
       <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="18" t="s">
         <v>154</v>
       </c>
@@ -7328,7 +7319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>156</v>
       </c>
@@ -7339,7 +7330,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>158</v>
       </c>
@@ -7348,7 +7339,7 @@
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>159</v>
       </c>
@@ -7357,7 +7348,7 @@
       </c>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>160</v>
       </c>
@@ -7366,7 +7357,7 @@
       </c>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>161</v>
       </c>
@@ -7375,7 +7366,7 @@
       </c>
       <c r="C6" s="13"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>162</v>
       </c>
@@ -7396,24 +7387,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98290782-EDB5-8E49-BAFB-76C1B5158EA7}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="3" width="9.8984375" customWidth="1"/>
-    <col min="4" max="4" width="7.09765625" customWidth="1"/>
-    <col min="5" max="5" width="9.8984375" customWidth="1"/>
-    <col min="6" max="7" width="7.19921875" customWidth="1"/>
-    <col min="8" max="8" width="7.796875" customWidth="1"/>
-    <col min="9" max="11" width="7.59765625" customWidth="1"/>
+    <col min="3" max="3" width="9.9140625" customWidth="1"/>
+    <col min="4" max="4" width="7.08203125" customWidth="1"/>
+    <col min="5" max="5" width="9.9140625" customWidth="1"/>
+    <col min="6" max="7" width="7.1640625" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" customWidth="1"/>
+    <col min="9" max="11" width="7.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="28" t="s">
         <v>166</v>
       </c>
@@ -7448,7 +7439,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
         <v>172</v>
       </c>
@@ -7481,7 +7472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
         <v>174</v>
       </c>
@@ -7514,7 +7505,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
         <v>176</v>
       </c>
@@ -7547,7 +7538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
         <v>181</v>
       </c>
@@ -7581,7 +7572,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
         <v>177</v>
       </c>
@@ -7616,7 +7607,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
         <v>179</v>
       </c>
@@ -7651,7 +7642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
         <v>218</v>
       </c>
@@ -7687,7 +7678,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="29" t="s">
         <v>211</v>
       </c>
@@ -7723,7 +7714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="29" t="s">
         <v>221</v>
       </c>
@@ -7759,7 +7750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
         <v>212</v>
       </c>
@@ -7795,7 +7786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="29" t="s">
         <v>210</v>
       </c>
@@ -7830,7 +7821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
         <v>213</v>
       </c>
@@ -7866,7 +7857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="29" t="s">
         <v>215</v>
       </c>
@@ -7901,7 +7892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
@@ -7921,50 +7912,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84637A79-E027-48E7-B7DE-002E7C836FC2}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.09765625" style="31" customWidth="1"/>
-    <col min="2" max="2" width="50.69921875" style="30" customWidth="1"/>
-    <col min="3" max="3" width="4.09765625" style="54" customWidth="1"/>
-    <col min="4" max="4" width="4.09765625" style="59" customWidth="1"/>
-    <col min="5" max="7" width="4.09765625" style="31" customWidth="1"/>
-    <col min="8" max="16" width="7.3984375" style="31" customWidth="1"/>
-    <col min="17" max="17" width="7.796875" style="59" customWidth="1"/>
-    <col min="18" max="18" width="11.69921875" style="67" customWidth="1"/>
-    <col min="19" max="19" width="10.3984375" style="46" customWidth="1"/>
-    <col min="20" max="20" width="18.3984375" style="54" customWidth="1"/>
-    <col min="21" max="21" width="18.3984375" style="30" customWidth="1"/>
-    <col min="22" max="22" width="56.09765625" style="30" customWidth="1"/>
-    <col min="23" max="24" width="8.796875" style="31"/>
+    <col min="1" max="1" width="12.08203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="4.08203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="4.08203125" style="59" customWidth="1"/>
+    <col min="5" max="7" width="4.08203125" style="31" customWidth="1"/>
+    <col min="8" max="16" width="7.4140625" style="31" customWidth="1"/>
+    <col min="17" max="17" width="7.83203125" style="59" customWidth="1"/>
+    <col min="18" max="18" width="11.6640625" style="67" customWidth="1"/>
+    <col min="19" max="19" width="10.4140625" style="46" customWidth="1"/>
+    <col min="20" max="20" width="18.4140625" style="54" customWidth="1"/>
+    <col min="21" max="21" width="18.4140625" style="30" customWidth="1"/>
+    <col min="22" max="22" width="56.08203125" style="30" customWidth="1"/>
+    <col min="23" max="24" width="8.83203125" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D1" s="69" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="D1" s="70" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="72"/>
       <c r="Q1" s="64"/>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="S1" s="71"/>
-    </row>
-    <row r="2" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="S1" s="72"/>
+    </row>
+    <row r="2" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
         <v>208</v>
       </c>
@@ -8038,12 +8029,14 @@
       <c r="T2" s="60" t="s">
         <v>267</v>
       </c>
-      <c r="U2" s="51"/>
+      <c r="U2" s="51" t="s">
+        <v>269</v>
+      </c>
       <c r="V2" s="50"/>
       <c r="W2" s="49"/>
       <c r="X2" s="49"/>
     </row>
-    <row r="3" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
         <v>263</v>
       </c>
@@ -8097,15 +8090,15 @@
       </c>
       <c r="R3" s="63"/>
       <c r="S3" s="47"/>
-      <c r="T3" s="72">
+      <c r="T3" s="69">
         <v>43905</v>
       </c>
-      <c r="U3" s="43"/>
+      <c r="U3" s="73"/>
       <c r="V3" s="43"/>
       <c r="W3" s="42"/>
       <c r="X3" s="42"/>
     </row>
-    <row r="4" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
         <v>235</v>
       </c>
@@ -8159,7 +8152,7 @@
       </c>
       <c r="R4" s="63"/>
       <c r="S4" s="47"/>
-      <c r="T4" s="72">
+      <c r="T4" s="69">
         <v>43919</v>
       </c>
       <c r="U4" s="43"/>
@@ -8167,7 +8160,7 @@
       <c r="W4" s="42"/>
       <c r="X4" s="42"/>
     </row>
-    <row r="5" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="42" t="s">
         <v>223</v>
       </c>
@@ -8222,13 +8215,13 @@
       </c>
       <c r="R5" s="63"/>
       <c r="S5" s="47"/>
-      <c r="T5" s="68"/>
-      <c r="U5" s="43"/>
+      <c r="T5" s="74"/>
+      <c r="U5" s="73"/>
       <c r="V5" s="43"/>
       <c r="W5" s="42"/>
       <c r="X5" s="42"/>
     </row>
-    <row r="6" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
         <v>224</v>
       </c>
@@ -8283,13 +8276,13 @@
       </c>
       <c r="R6" s="63"/>
       <c r="S6" s="47"/>
-      <c r="T6" s="68"/>
-      <c r="U6" s="43"/>
+      <c r="T6" s="74"/>
+      <c r="U6" s="73"/>
       <c r="V6" s="43"/>
       <c r="W6" s="42"/>
       <c r="X6" s="42"/>
     </row>
-    <row r="7" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="42" t="s">
         <v>234</v>
       </c>
@@ -8343,7 +8336,7 @@
       </c>
       <c r="R7" s="63"/>
       <c r="S7" s="47"/>
-      <c r="T7" s="72">
+      <c r="T7" s="69">
         <v>43919</v>
       </c>
       <c r="U7" s="43"/>
@@ -8351,7 +8344,7 @@
       <c r="W7" s="42"/>
       <c r="X7" s="42"/>
     </row>
-    <row r="8" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="42" t="s">
         <v>237</v>
       </c>
@@ -8405,7 +8398,7 @@
       </c>
       <c r="R8" s="63"/>
       <c r="S8" s="47"/>
-      <c r="T8" s="72">
+      <c r="T8" s="69">
         <v>43912</v>
       </c>
       <c r="U8" s="43"/>
@@ -8413,7 +8406,7 @@
       <c r="W8" s="42"/>
       <c r="X8" s="42"/>
     </row>
-    <row r="9" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="42" t="s">
         <v>225</v>
       </c>
@@ -8467,15 +8460,18 @@
       </c>
       <c r="R9" s="63"/>
       <c r="S9" s="47"/>
-      <c r="T9" s="72">
+      <c r="T9" s="69">
         <v>43909</v>
       </c>
-      <c r="U9" s="43"/>
+      <c r="U9" s="73">
+        <f>T8</f>
+        <v>43912</v>
+      </c>
       <c r="V9" s="43"/>
       <c r="W9" s="42"/>
       <c r="X9" s="42"/>
     </row>
-    <row r="10" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
         <v>238</v>
       </c>
@@ -8529,7 +8525,7 @@
       </c>
       <c r="R10" s="63"/>
       <c r="S10" s="47"/>
-      <c r="T10" s="72">
+      <c r="T10" s="69">
         <v>43912</v>
       </c>
       <c r="U10" s="43"/>
@@ -8537,7 +8533,7 @@
       <c r="W10" s="42"/>
       <c r="X10" s="42"/>
     </row>
-    <row r="11" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="42" t="s">
         <v>226</v>
       </c>
@@ -8591,15 +8587,18 @@
       </c>
       <c r="R11" s="63"/>
       <c r="S11" s="47"/>
-      <c r="T11" s="72">
+      <c r="T11" s="69">
         <v>43909</v>
       </c>
-      <c r="U11" s="43"/>
+      <c r="U11" s="73">
+        <f>T10</f>
+        <v>43912</v>
+      </c>
       <c r="V11" s="43"/>
       <c r="W11" s="42"/>
       <c r="X11" s="42"/>
     </row>
-    <row r="12" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="42" t="s">
         <v>260</v>
       </c>
@@ -8653,7 +8652,7 @@
       </c>
       <c r="R12" s="63"/>
       <c r="S12" s="47"/>
-      <c r="T12" s="72">
+      <c r="T12" s="69">
         <v>43919</v>
       </c>
       <c r="U12" s="43"/>
@@ -8661,7 +8660,7 @@
       <c r="W12" s="42"/>
       <c r="X12" s="42"/>
     </row>
-    <row r="13" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
         <v>227</v>
       </c>
@@ -8715,13 +8714,13 @@
       </c>
       <c r="R13" s="63"/>
       <c r="S13" s="47"/>
-      <c r="T13" s="72"/>
-      <c r="U13" s="43"/>
+      <c r="T13" s="69"/>
+      <c r="U13" s="73"/>
       <c r="V13" s="43"/>
       <c r="W13" s="42"/>
       <c r="X13" s="42"/>
     </row>
-    <row r="14" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="42" t="s">
         <v>231</v>
       </c>
@@ -8775,15 +8774,18 @@
       </c>
       <c r="R14" s="63"/>
       <c r="S14" s="47"/>
-      <c r="T14" s="72">
+      <c r="T14" s="69">
         <v>43909</v>
       </c>
-      <c r="U14" s="43"/>
+      <c r="U14" s="73">
+        <f>T12</f>
+        <v>43919</v>
+      </c>
       <c r="V14" s="43"/>
       <c r="W14" s="42"/>
       <c r="X14" s="42"/>
     </row>
-    <row r="15" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="42" t="s">
         <v>228</v>
       </c>
@@ -8837,7 +8839,7 @@
       </c>
       <c r="R15" s="63"/>
       <c r="S15" s="47"/>
-      <c r="T15" s="72">
+      <c r="T15" s="69">
         <v>43912</v>
       </c>
       <c r="U15" s="43"/>
@@ -8845,7 +8847,7 @@
       <c r="W15" s="42"/>
       <c r="X15" s="42"/>
     </row>
-    <row r="16" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
         <v>229</v>
       </c>
@@ -8899,7 +8901,7 @@
       </c>
       <c r="R16" s="63"/>
       <c r="S16" s="47"/>
-      <c r="T16" s="72">
+      <c r="T16" s="69">
         <v>43912</v>
       </c>
       <c r="U16" s="43"/>
@@ -8907,7 +8909,7 @@
       <c r="W16" s="42"/>
       <c r="X16" s="42"/>
     </row>
-    <row r="17" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" s="44" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
         <v>230</v>
       </c>
@@ -8965,7 +8967,7 @@
       <c r="S17" s="47">
         <v>0.1</v>
       </c>
-      <c r="T17" s="72">
+      <c r="T17" s="69">
         <v>43915</v>
       </c>
       <c r="U17" s="43"/>
@@ -8973,7 +8975,7 @@
       <c r="W17" s="42"/>
       <c r="X17" s="42"/>
     </row>
-    <row r="18" spans="1:24" s="27" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="27" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="45" t="s">
         <v>232</v>
       </c>
@@ -9031,7 +9033,7 @@
       <c r="S18" s="33">
         <v>0.95</v>
       </c>
-      <c r="T18" s="72">
+      <c r="T18" s="69">
         <v>43919</v>
       </c>
       <c r="U18" s="37"/>
@@ -9039,7 +9041,7 @@
       <c r="W18" s="45"/>
       <c r="X18" s="45"/>
     </row>
-    <row r="19" spans="1:24" s="27" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" s="27" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="45" t="s">
         <v>221</v>
       </c>
@@ -9093,7 +9095,7 @@
       </c>
       <c r="R19" s="63"/>
       <c r="S19" s="33"/>
-      <c r="T19" s="72">
+      <c r="T19" s="69">
         <v>43912</v>
       </c>
       <c r="U19" s="37"/>
@@ -9101,7 +9103,7 @@
       <c r="W19" s="45"/>
       <c r="X19" s="45"/>
     </row>
-    <row r="20" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="36" t="s">
         <v>258</v>
       </c>
@@ -9159,7 +9161,7 @@
       <c r="S20" s="33">
         <v>0.5</v>
       </c>
-      <c r="T20" s="72">
+      <c r="T20" s="69">
         <v>43919</v>
       </c>
       <c r="U20" s="37"/>
@@ -9167,7 +9169,7 @@
       <c r="W20" s="36"/>
       <c r="X20" s="36"/>
     </row>
-    <row r="21" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="36" t="s">
         <v>246</v>
       </c>
@@ -9225,7 +9227,7 @@
       <c r="S21" s="33">
         <v>0.95</v>
       </c>
-      <c r="T21" s="72">
+      <c r="T21" s="69">
         <v>43919</v>
       </c>
       <c r="U21" s="37"/>
@@ -9233,7 +9235,7 @@
       <c r="W21" s="36"/>
       <c r="X21" s="36"/>
     </row>
-    <row r="22" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="36" t="s">
         <v>259</v>
       </c>
@@ -9287,7 +9289,7 @@
       </c>
       <c r="R22" s="63"/>
       <c r="S22" s="33"/>
-      <c r="T22" s="72">
+      <c r="T22" s="69">
         <v>43919</v>
       </c>
       <c r="U22" s="37"/>
@@ -9295,7 +9297,7 @@
       <c r="W22" s="36"/>
       <c r="X22" s="36"/>
     </row>
-    <row r="23" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="36"/>
       <c r="B23" s="32"/>
       <c r="C23" s="59"/>
@@ -9321,7 +9323,7 @@
       <c r="W23" s="36"/>
       <c r="X23" s="36"/>
     </row>
-    <row r="24" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="36"/>
       <c r="C24" s="59"/>
       <c r="D24" s="59"/>
@@ -9346,7 +9348,7 @@
       <c r="W24" s="36"/>
       <c r="X24" s="36"/>
     </row>
-    <row r="25" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="36"/>
       <c r="B25" s="32"/>
       <c r="C25" s="59"/>
@@ -9372,7 +9374,7 @@
       <c r="W25" s="36"/>
       <c r="X25" s="36"/>
     </row>
-    <row r="26" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="36"/>
       <c r="B26" s="32"/>
       <c r="C26" s="58"/>
@@ -9398,7 +9400,7 @@
       <c r="W26" s="36"/>
       <c r="X26" s="36"/>
     </row>
-    <row r="27" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="36"/>
       <c r="B27" s="36"/>
       <c r="C27" s="58"/>
@@ -9424,7 +9426,7 @@
       <c r="W27" s="36"/>
       <c r="X27" s="36"/>
     </row>
-    <row r="28" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="36"/>
       <c r="B28" s="32"/>
       <c r="C28" s="58"/>
@@ -9450,7 +9452,7 @@
       <c r="W28" s="36"/>
       <c r="X28" s="36"/>
     </row>
-    <row r="29" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="36"/>
       <c r="B29" s="36"/>
       <c r="C29" s="59"/>
@@ -9476,7 +9478,7 @@
       <c r="W29" s="36"/>
       <c r="X29" s="36"/>
     </row>
-    <row r="30" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="36"/>
       <c r="B30" s="32"/>
       <c r="C30" s="58"/>
@@ -9502,7 +9504,7 @@
       <c r="W30" s="36"/>
       <c r="X30" s="36"/>
     </row>
-    <row r="31" spans="1:24" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" s="26" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="36"/>
       <c r="C31" s="58"/>
       <c r="D31" s="61"/>
@@ -9533,17 +9535,17 @@
     <mergeCell ref="R1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:P20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:P22">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:P22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9561,13 +9563,13 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.69921875" customWidth="1"/>
-    <col min="3" max="3" width="51.796875" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>166</v>
       </c>
@@ -9578,7 +9580,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
         <v>195</v>
       </c>
@@ -9589,7 +9591,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="23" t="s">
         <v>196</v>
       </c>
@@ -9600,7 +9602,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="23" t="s">
         <v>199</v>
       </c>
@@ -9608,7 +9610,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -9619,7 +9621,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -9630,7 +9632,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>187</v>
       </c>
@@ -9638,7 +9640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>188</v>
       </c>
@@ -9649,7 +9651,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>194</v>
       </c>
@@ -9657,7 +9659,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>189</v>
       </c>
@@ -9668,7 +9670,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>200</v>
       </c>
@@ -9676,7 +9678,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Clustering for classrooms and workplaces
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164FE0F0-0E60-4679-9C0F-EEACF52334D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1135763E-A9F9-44B3-9328-EB0EBBD6F30F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="762" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data" sheetId="1" r:id="rId1"/>
@@ -351,6 +351,31 @@
           </rPr>
           <t xml:space="preserve">
 From Prem et al. age-weighted average community contacts is 5 for Victoria. Therefore when specific community locations are modelled, the "remaining" should be reduced</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{B5FF3F83-13AE-4712-9F02-E910F0981BAB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+11% of the population visit church weekly:
+http://www.2016ncls.org.au/resources/downloads/Local%20Churches%20in%20Australia-Research%20Findings%20from%20NCLS%20Research(2017).pdf</t>
         </r>
       </text>
     </comment>
@@ -825,7 +850,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="270">
   <si>
     <t>date</t>
   </si>
@@ -1632,6 +1657,9 @@
   </si>
   <si>
     <t>Change in baseline transmission risk for each network, relative to baseline</t>
+  </si>
+  <si>
+    <t>clusters</t>
   </si>
 </sst>
 </file>
@@ -2492,6 +2520,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2500,9 +2531,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -2553,28 +2581,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <b val="0"/>
@@ -7396,9 +7403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98290782-EDB5-8E49-BAFB-76C1B5158EA7}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7589,10 +7596,10 @@
         <v>178</v>
       </c>
       <c r="C6" s="29">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="D6" s="29">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E6" s="29">
         <v>0.5</v>
@@ -7604,7 +7611,7 @@
         <v>110</v>
       </c>
       <c r="H6" s="29" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="I6" s="29">
         <v>0</v>
@@ -7675,7 +7682,7 @@
         <v>65</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>183</v>
+        <v>269</v>
       </c>
       <c r="I8" s="29">
         <v>0</v>
@@ -7921,8 +7928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84637A79-E027-48E7-B7DE-002E7C836FC2}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7943,26 +7950,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="70" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="72"/>
       <c r="Q1" s="64"/>
-      <c r="R1" s="69" t="s">
+      <c r="R1" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="S1" s="71"/>
+      <c r="S1" s="72"/>
     </row>
     <row r="2" spans="1:24" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="49" t="s">
@@ -8097,7 +8104,7 @@
       </c>
       <c r="R3" s="63"/>
       <c r="S3" s="47"/>
-      <c r="T3" s="72">
+      <c r="T3" s="69">
         <v>43905</v>
       </c>
       <c r="U3" s="43"/>
@@ -8159,7 +8166,7 @@
       </c>
       <c r="R4" s="63"/>
       <c r="S4" s="47"/>
-      <c r="T4" s="72">
+      <c r="T4" s="69">
         <v>43919</v>
       </c>
       <c r="U4" s="43"/>
@@ -8343,7 +8350,7 @@
       </c>
       <c r="R7" s="63"/>
       <c r="S7" s="47"/>
-      <c r="T7" s="72">
+      <c r="T7" s="69">
         <v>43919</v>
       </c>
       <c r="U7" s="43"/>
@@ -8405,7 +8412,7 @@
       </c>
       <c r="R8" s="63"/>
       <c r="S8" s="47"/>
-      <c r="T8" s="72">
+      <c r="T8" s="69">
         <v>43912</v>
       </c>
       <c r="U8" s="43"/>
@@ -8467,7 +8474,7 @@
       </c>
       <c r="R9" s="63"/>
       <c r="S9" s="47"/>
-      <c r="T9" s="72">
+      <c r="T9" s="69">
         <v>43909</v>
       </c>
       <c r="U9" s="43"/>
@@ -8529,7 +8536,7 @@
       </c>
       <c r="R10" s="63"/>
       <c r="S10" s="47"/>
-      <c r="T10" s="72">
+      <c r="T10" s="69">
         <v>43912</v>
       </c>
       <c r="U10" s="43"/>
@@ -8591,7 +8598,7 @@
       </c>
       <c r="R11" s="63"/>
       <c r="S11" s="47"/>
-      <c r="T11" s="72">
+      <c r="T11" s="69">
         <v>43909</v>
       </c>
       <c r="U11" s="43"/>
@@ -8653,7 +8660,7 @@
       </c>
       <c r="R12" s="63"/>
       <c r="S12" s="47"/>
-      <c r="T12" s="72">
+      <c r="T12" s="69">
         <v>43919</v>
       </c>
       <c r="U12" s="43"/>
@@ -8715,7 +8722,7 @@
       </c>
       <c r="R13" s="63"/>
       <c r="S13" s="47"/>
-      <c r="T13" s="72"/>
+      <c r="T13" s="69"/>
       <c r="U13" s="43"/>
       <c r="V13" s="43"/>
       <c r="W13" s="42"/>
@@ -8775,7 +8782,7 @@
       </c>
       <c r="R14" s="63"/>
       <c r="S14" s="47"/>
-      <c r="T14" s="72">
+      <c r="T14" s="69">
         <v>43909</v>
       </c>
       <c r="U14" s="43"/>
@@ -8837,7 +8844,7 @@
       </c>
       <c r="R15" s="63"/>
       <c r="S15" s="47"/>
-      <c r="T15" s="72">
+      <c r="T15" s="69">
         <v>43912</v>
       </c>
       <c r="U15" s="43"/>
@@ -8899,7 +8906,7 @@
       </c>
       <c r="R16" s="63"/>
       <c r="S16" s="47"/>
-      <c r="T16" s="72">
+      <c r="T16" s="69">
         <v>43912</v>
       </c>
       <c r="U16" s="43"/>
@@ -8965,7 +8972,7 @@
       <c r="S17" s="47">
         <v>0.1</v>
       </c>
-      <c r="T17" s="72">
+      <c r="T17" s="69">
         <v>43915</v>
       </c>
       <c r="U17" s="43"/>
@@ -9031,7 +9038,7 @@
       <c r="S18" s="33">
         <v>0.95</v>
       </c>
-      <c r="T18" s="72">
+      <c r="T18" s="69">
         <v>43919</v>
       </c>
       <c r="U18" s="37"/>
@@ -9093,7 +9100,7 @@
       </c>
       <c r="R19" s="63"/>
       <c r="S19" s="33"/>
-      <c r="T19" s="72">
+      <c r="T19" s="69">
         <v>43912</v>
       </c>
       <c r="U19" s="37"/>
@@ -9142,7 +9149,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="38">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O20" s="38">
         <v>1</v>
@@ -9159,7 +9166,7 @@
       <c r="S20" s="33">
         <v>0.5</v>
       </c>
-      <c r="T20" s="72">
+      <c r="T20" s="69">
         <v>43919</v>
       </c>
       <c r="U20" s="37"/>
@@ -9225,7 +9232,7 @@
       <c r="S21" s="33">
         <v>0.95</v>
       </c>
-      <c r="T21" s="72">
+      <c r="T21" s="69">
         <v>43919</v>
       </c>
       <c r="U21" s="37"/>
@@ -9287,7 +9294,7 @@
       </c>
       <c r="R22" s="63"/>
       <c r="S22" s="33"/>
-      <c r="T22" s="72">
+      <c r="T22" s="69">
         <v>43919</v>
       </c>
       <c r="U22" s="37"/>
@@ -9533,17 +9540,17 @@
     <mergeCell ref="R1:S1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:P20">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:P22">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:P22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9557,8 +9564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Some cleaning but order seems to matter
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5E6D7F-E921-4571-81A4-91A01C0581D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BABC44-AC1F-415D-A5D6-970A8AEF0F68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="762" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data" sheetId="1" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="286">
   <si>
     <t>date</t>
   </si>
@@ -2134,6 +2134,12 @@
   </si>
   <si>
     <t>Schools closed</t>
+  </si>
+  <si>
+    <t>comm_relax</t>
+  </si>
+  <si>
+    <t>Physical distancing relaxed a bit</t>
   </si>
 </sst>
 </file>
@@ -2145,7 +2151,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="34">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2854,7 +2860,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3034,6 +3040,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3083,7 +3092,49 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3688,7 +3739,7 @@
       <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="10.796875" style="22"/>
     <col min="2" max="2" width="14.5" style="7" customWidth="1"/>
@@ -3705,7 +3756,7 @@
     <col min="13" max="16384" width="10.796875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="6" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3743,7 +3794,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" s="21">
         <v>43891</v>
       </c>
@@ -3763,7 +3814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" s="21">
         <v>43892</v>
       </c>
@@ -3783,7 +3834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" s="21">
         <v>43893</v>
       </c>
@@ -3803,7 +3854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" s="21">
         <v>43894</v>
       </c>
@@ -3823,7 +3874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" s="21">
         <v>43895</v>
       </c>
@@ -3843,7 +3894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12">
       <c r="A7" s="21">
         <v>43896</v>
       </c>
@@ -3863,7 +3914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" s="21">
         <v>43897</v>
       </c>
@@ -3883,7 +3934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" s="21">
         <v>43898</v>
       </c>
@@ -3903,7 +3954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" s="21">
         <v>43899</v>
       </c>
@@ -3923,7 +3974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" s="21">
         <v>43900</v>
       </c>
@@ -3943,7 +3994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" s="21">
         <v>43901</v>
       </c>
@@ -3963,7 +4014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" s="21">
         <v>43902</v>
       </c>
@@ -3983,7 +4034,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" s="21">
         <v>43903</v>
       </c>
@@ -4006,7 +4057,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" s="21">
         <v>43904</v>
       </c>
@@ -4029,7 +4080,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" s="21">
         <v>43905</v>
       </c>
@@ -4052,7 +4103,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" s="21">
         <v>43906</v>
       </c>
@@ -4081,7 +4132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12">
       <c r="A18" s="21">
         <v>43907</v>
       </c>
@@ -4110,7 +4161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" s="21">
         <v>43908</v>
       </c>
@@ -4139,7 +4190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" s="21">
         <v>43909</v>
       </c>
@@ -4168,7 +4219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" s="21">
         <v>43910</v>
       </c>
@@ -4197,7 +4248,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12">
       <c r="A22" s="21">
         <v>43911</v>
       </c>
@@ -4226,7 +4277,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" s="21">
         <v>43912</v>
       </c>
@@ -4255,7 +4306,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" s="21">
         <v>43913</v>
       </c>
@@ -4290,7 +4341,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" s="21">
         <v>43914</v>
       </c>
@@ -4322,7 +4373,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" s="21">
         <v>43915</v>
       </c>
@@ -4354,7 +4405,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" s="21">
         <v>43916</v>
       </c>
@@ -4386,7 +4437,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" s="21">
         <v>43917</v>
       </c>
@@ -4418,7 +4469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" s="21">
         <v>43918</v>
       </c>
@@ -4450,7 +4501,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" s="21">
         <v>43919</v>
       </c>
@@ -4488,7 +4539,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12">
       <c r="A31" s="21">
         <v>43920</v>
       </c>
@@ -4523,7 +4574,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" s="21">
         <v>43921</v>
       </c>
@@ -4561,7 +4612,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="A33" s="21">
         <v>43922</v>
       </c>
@@ -4599,7 +4650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="A34" s="21">
         <v>43923</v>
       </c>
@@ -4637,7 +4688,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="A35" s="21">
         <v>43924</v>
       </c>
@@ -4675,7 +4726,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="A36" s="21">
         <v>43925</v>
       </c>
@@ -4713,7 +4764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="A37" s="21">
         <v>43926</v>
       </c>
@@ -4751,7 +4802,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="A38" s="21">
         <v>43927</v>
       </c>
@@ -4789,7 +4840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="A39" s="21">
         <v>43928</v>
       </c>
@@ -4827,7 +4878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="A40" s="21">
         <v>43929</v>
       </c>
@@ -4865,7 +4916,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="A41" s="21">
         <v>43930</v>
       </c>
@@ -4903,7 +4954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="A42" s="21">
         <v>43931</v>
       </c>
@@ -4941,7 +4992,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="A43" s="21">
         <v>43932</v>
       </c>
@@ -4979,7 +5030,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="A44" s="21">
         <v>43933</v>
       </c>
@@ -5017,7 +5068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="A45" s="21">
         <v>43934</v>
       </c>
@@ -5055,7 +5106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="A46" s="21">
         <v>43935</v>
       </c>
@@ -5093,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" s="21">
         <v>43936</v>
       </c>
@@ -5131,7 +5182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="A48" s="21">
         <v>43937</v>
       </c>
@@ -5169,7 +5220,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="A49" s="21">
         <v>43938</v>
       </c>
@@ -5207,7 +5258,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="A50" s="21">
         <v>43939</v>
       </c>
@@ -5245,7 +5296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="A51" s="21">
         <v>43940</v>
       </c>
@@ -5283,7 +5334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="A52" s="21">
         <v>43941</v>
       </c>
@@ -5321,7 +5372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="A53" s="21">
         <v>43942</v>
       </c>
@@ -5372,9 +5423,9 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -5430,7 +5481,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -5486,7 +5537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -5539,7 +5590,7 @@
         <v>4.3559999999999996E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -5592,7 +5643,7 @@
         <v>4.1580000000000002E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -5645,7 +5696,7 @@
         <v>3.0739999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -5698,7 +5749,7 @@
         <v>3.6970000000000002E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -5751,7 +5802,7 @@
         <v>6.8170000000000001E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -5804,7 +5855,7 @@
         <v>3.594E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -5857,7 +5908,7 @@
         <v>2.7920000000000002E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -5910,7 +5961,7 @@
         <v>6.6759999999999996E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -5963,7 +6014,7 @@
         <v>1.2394000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -6016,7 +6067,7 @@
         <v>2.0105999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -6069,7 +6120,7 @@
         <v>2.0524000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -6122,7 +6173,7 @@
         <v>5.2319999999999997E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -6175,7 +6226,7 @@
         <v>1.4578000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18">
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
@@ -6228,7 +6279,7 @@
         <v>9.6379000000000006E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -6316,12 +6367,12 @@
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="16384" width="10.796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="17" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="17" customFormat="1">
       <c r="A1" s="14" t="s">
         <v>153</v>
       </c>
@@ -6338,7 +6389,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
@@ -6356,7 +6407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -6374,7 +6425,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5">
       <c r="A4" s="9" t="s">
         <v>38</v>
       </c>
@@ -6389,7 +6440,7 @@
         <v>53807</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5">
       <c r="A5" s="9" t="s">
         <v>39</v>
       </c>
@@ -6404,7 +6455,7 @@
         <v>54603</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5">
       <c r="A6" s="9" t="s">
         <v>40</v>
       </c>
@@ -6419,7 +6470,7 @@
         <v>53380</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5">
       <c r="A7" s="9" t="s">
         <v>41</v>
       </c>
@@ -6434,7 +6485,7 @@
         <v>52236</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5">
       <c r="A8" s="9" t="s">
         <v>42</v>
       </c>
@@ -6449,7 +6500,7 @@
         <v>52696</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5">
       <c r="A9" s="9" t="s">
         <v>43</v>
       </c>
@@ -6464,7 +6515,7 @@
         <v>51199</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5">
       <c r="A10" s="9" t="s">
         <v>44</v>
       </c>
@@ -6479,7 +6530,7 @@
         <v>51198</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5">
       <c r="A11" s="9" t="s">
         <v>45</v>
       </c>
@@ -6494,7 +6545,7 @@
         <v>50836</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5">
       <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
@@ -6509,7 +6560,7 @@
         <v>49144</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5">
       <c r="A13" s="9" t="s">
         <v>47</v>
       </c>
@@ -6524,7 +6575,7 @@
         <v>47266</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5">
       <c r="A14" s="9" t="s">
         <v>48</v>
       </c>
@@ -6539,7 +6590,7 @@
         <v>46880</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5">
       <c r="A15" s="9" t="s">
         <v>49</v>
       </c>
@@ -6554,7 +6605,7 @@
         <v>46060</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5">
       <c r="A16" s="9" t="s">
         <v>50</v>
       </c>
@@ -6569,7 +6620,7 @@
         <v>45087</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4">
       <c r="A17" s="9" t="s">
         <v>51</v>
       </c>
@@ -6584,7 +6635,7 @@
         <v>45958</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -6599,7 +6650,7 @@
         <v>47505</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4">
       <c r="A19" s="9" t="s">
         <v>53</v>
       </c>
@@ -6614,7 +6665,7 @@
         <v>47748</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4">
       <c r="A20" s="9" t="s">
         <v>54</v>
       </c>
@@ -6629,7 +6680,7 @@
         <v>51641</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4">
       <c r="A21" s="9" t="s">
         <v>55</v>
       </c>
@@ -6644,7 +6695,7 @@
         <v>57079</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4">
       <c r="A22" s="9" t="s">
         <v>56</v>
       </c>
@@ -6659,7 +6710,7 @@
         <v>60111</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4">
       <c r="A23" s="9" t="s">
         <v>57</v>
       </c>
@@ -6674,7 +6725,7 @@
         <v>62268</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4">
       <c r="A24" s="9" t="s">
         <v>58</v>
       </c>
@@ -6689,7 +6740,7 @@
         <v>62979</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4">
       <c r="A25" s="9" t="s">
         <v>59</v>
       </c>
@@ -6704,7 +6755,7 @@
         <v>65013</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4">
       <c r="A26" s="9" t="s">
         <v>60</v>
       </c>
@@ -6719,7 +6770,7 @@
         <v>65746</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4">
       <c r="A27" s="9" t="s">
         <v>61</v>
       </c>
@@ -6734,7 +6785,7 @@
         <v>67618</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4">
       <c r="A28" s="9" t="s">
         <v>62</v>
       </c>
@@ -6749,7 +6800,7 @@
         <v>69532</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4">
       <c r="A29" s="9" t="s">
         <v>63</v>
       </c>
@@ -6764,7 +6815,7 @@
         <v>68855</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4">
       <c r="A30" s="9" t="s">
         <v>64</v>
       </c>
@@ -6779,7 +6830,7 @@
         <v>70345</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4">
       <c r="A31" s="9" t="s">
         <v>65</v>
       </c>
@@ -6794,7 +6845,7 @@
         <v>69062</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4">
       <c r="A32" s="9" t="s">
         <v>66</v>
       </c>
@@ -6809,7 +6860,7 @@
         <v>70909</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="9" t="s">
         <v>67</v>
       </c>
@@ -6824,7 +6875,7 @@
         <v>70590</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="9" t="s">
         <v>68</v>
       </c>
@@ -6839,7 +6890,7 @@
         <v>70286</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" s="9" t="s">
         <v>69</v>
       </c>
@@ -6854,7 +6905,7 @@
         <v>70326</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4">
       <c r="A36" s="9" t="s">
         <v>70</v>
       </c>
@@ -6869,7 +6920,7 @@
         <v>68170</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4">
       <c r="A37" s="9" t="s">
         <v>71</v>
       </c>
@@ -6884,7 +6935,7 @@
         <v>66194</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4">
       <c r="A38" s="9" t="s">
         <v>72</v>
       </c>
@@ -6899,7 +6950,7 @@
         <v>63654</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4">
       <c r="A39" s="9" t="s">
         <v>73</v>
       </c>
@@ -6914,7 +6965,7 @@
         <v>61073</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4">
       <c r="A40" s="9" t="s">
         <v>74</v>
       </c>
@@ -6929,7 +6980,7 @@
         <v>58823</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4">
       <c r="A41" s="9" t="s">
         <v>75</v>
       </c>
@@ -6944,7 +6995,7 @@
         <v>57759</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4">
       <c r="A42" s="9" t="s">
         <v>76</v>
       </c>
@@ -6959,7 +7010,7 @@
         <v>57893</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4">
       <c r="A43" s="9" t="s">
         <v>77</v>
       </c>
@@ -6974,7 +7025,7 @@
         <v>57469</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4">
       <c r="A44" s="9" t="s">
         <v>78</v>
       </c>
@@ -6989,7 +7040,7 @@
         <v>58949</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
         <v>79</v>
       </c>
@@ -7004,7 +7055,7 @@
         <v>58767</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4">
       <c r="A46" s="9" t="s">
         <v>80</v>
       </c>
@@ -7019,7 +7070,7 @@
         <v>60562</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4">
       <c r="A47" s="9" t="s">
         <v>81</v>
       </c>
@@ -7034,7 +7085,7 @@
         <v>62190</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4">
       <c r="A48" s="9" t="s">
         <v>82</v>
       </c>
@@ -7049,7 +7100,7 @@
         <v>58515</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4">
       <c r="A49" s="9" t="s">
         <v>83</v>
       </c>
@@ -7064,7 +7115,7 @@
         <v>57148</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4">
       <c r="A50" s="9" t="s">
         <v>84</v>
       </c>
@@ -7079,7 +7130,7 @@
         <v>55722</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4">
       <c r="A51" s="9" t="s">
         <v>85</v>
       </c>
@@ -7094,7 +7145,7 @@
         <v>52756</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4">
       <c r="A52" s="9" t="s">
         <v>86</v>
       </c>
@@ -7109,7 +7160,7 @@
         <v>52691</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4">
       <c r="A53" s="9" t="s">
         <v>87</v>
       </c>
@@ -7124,7 +7175,7 @@
         <v>51198</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4">
       <c r="A54" s="9" t="s">
         <v>88</v>
       </c>
@@ -7139,7 +7190,7 @@
         <v>52386</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4">
       <c r="A55" s="9" t="s">
         <v>89</v>
       </c>
@@ -7154,7 +7205,7 @@
         <v>52234</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4">
       <c r="A56" s="9" t="s">
         <v>90</v>
       </c>
@@ -7169,7 +7220,7 @@
         <v>50731</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4">
       <c r="A57" s="9" t="s">
         <v>91</v>
       </c>
@@ -7184,7 +7235,7 @@
         <v>50406</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4">
       <c r="A58" s="9" t="s">
         <v>92</v>
       </c>
@@ -7199,7 +7250,7 @@
         <v>48630</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4">
       <c r="A59" s="9" t="s">
         <v>93</v>
       </c>
@@ -7214,7 +7265,7 @@
         <v>46802</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4">
       <c r="A60" s="9" t="s">
         <v>94</v>
       </c>
@@ -7229,7 +7280,7 @@
         <v>46045</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4">
       <c r="A61" s="9" t="s">
         <v>95</v>
       </c>
@@ -7244,7 +7295,7 @@
         <v>44147</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4">
       <c r="A62" s="9" t="s">
         <v>96</v>
       </c>
@@ -7259,7 +7310,7 @@
         <v>44057</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4">
       <c r="A63" s="9" t="s">
         <v>97</v>
       </c>
@@ -7274,7 +7325,7 @@
         <v>41590</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4">
       <c r="A64" s="9" t="s">
         <v>98</v>
       </c>
@@ -7289,7 +7340,7 @@
         <v>40044</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4">
       <c r="A65" s="9" t="s">
         <v>99</v>
       </c>
@@ -7304,7 +7355,7 @@
         <v>39348</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4">
       <c r="A66" s="9" t="s">
         <v>100</v>
       </c>
@@ -7319,7 +7370,7 @@
         <v>38109</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4">
       <c r="A67" s="9" t="s">
         <v>101</v>
       </c>
@@ -7334,7 +7385,7 @@
         <v>37555</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
@@ -7349,7 +7400,7 @@
         <v>36069</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4">
       <c r="A69" s="9" t="s">
         <v>103</v>
       </c>
@@ -7364,7 +7415,7 @@
         <v>35049</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4">
       <c r="A70" s="9" t="s">
         <v>104</v>
       </c>
@@ -7379,7 +7430,7 @@
         <v>35464</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4">
       <c r="A71" s="9" t="s">
         <v>105</v>
       </c>
@@ -7394,7 +7445,7 @@
         <v>36919</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4">
       <c r="A72" s="9" t="s">
         <v>106</v>
       </c>
@@ -7409,7 +7460,7 @@
         <v>30984</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4">
       <c r="A73" s="9" t="s">
         <v>107</v>
       </c>
@@ -7424,7 +7475,7 @@
         <v>28543</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4">
       <c r="A74" s="9" t="s">
         <v>108</v>
       </c>
@@ -7439,7 +7490,7 @@
         <v>27858</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4">
       <c r="A75" s="9" t="s">
         <v>109</v>
       </c>
@@ -7454,7 +7505,7 @@
         <v>24567</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4">
       <c r="A76" s="9" t="s">
         <v>110</v>
       </c>
@@ -7469,7 +7520,7 @@
         <v>24510</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4">
       <c r="A77" s="9" t="s">
         <v>111</v>
       </c>
@@ -7484,7 +7535,7 @@
         <v>22998</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4">
       <c r="A78" s="9" t="s">
         <v>112</v>
       </c>
@@ -7499,7 +7550,7 @@
         <v>22512</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4">
       <c r="A79" s="9" t="s">
         <v>113</v>
       </c>
@@ -7514,7 +7565,7 @@
         <v>21184</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4">
       <c r="A80" s="9" t="s">
         <v>114</v>
       </c>
@@ -7529,7 +7580,7 @@
         <v>20306</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4">
       <c r="A81" s="9" t="s">
         <v>115</v>
       </c>
@@ -7544,7 +7595,7 @@
         <v>19188</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4">
       <c r="A82" s="9" t="s">
         <v>116</v>
       </c>
@@ -7559,7 +7610,7 @@
         <v>18359</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4">
       <c r="A83" s="9" t="s">
         <v>117</v>
       </c>
@@ -7574,7 +7625,7 @@
         <v>16636</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4">
       <c r="A84" s="9" t="s">
         <v>118</v>
       </c>
@@ -7589,7 +7640,7 @@
         <v>15857</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4">
       <c r="A85" s="9" t="s">
         <v>119</v>
       </c>
@@ -7604,7 +7655,7 @@
         <v>14574</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4">
       <c r="A86" s="9" t="s">
         <v>120</v>
       </c>
@@ -7619,7 +7670,7 @@
         <v>13566</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4">
       <c r="A87" s="9" t="s">
         <v>121</v>
       </c>
@@ -7634,7 +7685,7 @@
         <v>13090</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4">
       <c r="A88" s="9" t="s">
         <v>122</v>
       </c>
@@ -7649,7 +7700,7 @@
         <v>12415</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4">
       <c r="A89" s="9" t="s">
         <v>123</v>
       </c>
@@ -7664,7 +7715,7 @@
         <v>10624</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4">
       <c r="A90" s="9" t="s">
         <v>124</v>
       </c>
@@ -7679,7 +7730,7 @@
         <v>9445</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4">
       <c r="A91" s="9" t="s">
         <v>125</v>
       </c>
@@ -7694,7 +7745,7 @@
         <v>8388</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4">
       <c r="A92" s="9" t="s">
         <v>126</v>
       </c>
@@ -7709,7 +7760,7 @@
         <v>7233</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4">
       <c r="A93" s="9" t="s">
         <v>127</v>
       </c>
@@ -7724,7 +7775,7 @@
         <v>5795</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4">
       <c r="A94" s="9" t="s">
         <v>128</v>
       </c>
@@ -7739,7 +7790,7 @@
         <v>4814</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4">
       <c r="A95" s="9" t="s">
         <v>129</v>
       </c>
@@ -7754,7 +7805,7 @@
         <v>3853</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4">
       <c r="A96" s="9" t="s">
         <v>130</v>
       </c>
@@ -7769,7 +7820,7 @@
         <v>2893</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4">
       <c r="A97" s="9" t="s">
         <v>131</v>
       </c>
@@ -7784,7 +7835,7 @@
         <v>2327</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4">
       <c r="A98" s="9" t="s">
         <v>132</v>
       </c>
@@ -7799,7 +7850,7 @@
         <v>1586</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4">
       <c r="A99" s="9" t="s">
         <v>133</v>
       </c>
@@ -7814,7 +7865,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4">
       <c r="A100" s="9" t="s">
         <v>134</v>
       </c>
@@ -7829,7 +7880,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4">
       <c r="A101" s="9" t="s">
         <v>135</v>
       </c>
@@ -7844,7 +7895,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4">
       <c r="A102" s="9" t="s">
         <v>136</v>
       </c>
@@ -7859,7 +7910,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4">
       <c r="A103" s="9" t="s">
         <v>137</v>
       </c>
@@ -7874,7 +7925,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4">
       <c r="A104" s="9" t="s">
         <v>138</v>
       </c>
@@ -7889,7 +7940,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4">
       <c r="A105" s="9" t="s">
         <v>139</v>
       </c>
@@ -7904,7 +7955,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4">
       <c r="A106" s="9" t="s">
         <v>140</v>
       </c>
@@ -7919,7 +7970,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4">
       <c r="A107" s="9" t="s">
         <v>141</v>
       </c>
@@ -7934,7 +7985,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4">
       <c r="A108" s="9" t="s">
         <v>142</v>
       </c>
@@ -7949,7 +8000,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4">
       <c r="A109" s="9" t="s">
         <v>143</v>
       </c>
@@ -7964,7 +8015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4">
       <c r="A110" s="9" t="s">
         <v>144</v>
       </c>
@@ -7979,7 +8030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4">
       <c r="A111" s="9" t="s">
         <v>145</v>
       </c>
@@ -7994,7 +8045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4">
       <c r="A112" s="9" t="s">
         <v>146</v>
       </c>
@@ -8009,7 +8060,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4">
       <c r="A113" s="9" t="s">
         <v>147</v>
       </c>
@@ -8024,7 +8075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4">
       <c r="A114" s="9" t="s">
         <v>148</v>
       </c>
@@ -8039,7 +8090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4">
       <c r="A115" s="9" t="s">
         <v>149</v>
       </c>
@@ -8054,7 +8105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4">
       <c r="A116" s="9" t="s">
         <v>150</v>
       </c>
@@ -8069,7 +8120,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4">
       <c r="A117" s="9" t="s">
         <v>151</v>
       </c>
@@ -8098,13 +8149,13 @@
       <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="20" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>154</v>
       </c>
@@ -8115,7 +8166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="11" t="s">
         <v>156</v>
       </c>
@@ -8126,7 +8177,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="11" t="s">
         <v>158</v>
       </c>
@@ -8135,7 +8186,7 @@
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="11" t="s">
         <v>159</v>
       </c>
@@ -8144,7 +8195,7 @@
       </c>
       <c r="C4" s="13"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" s="11" t="s">
         <v>160</v>
       </c>
@@ -8153,7 +8204,7 @@
       </c>
       <c r="C5" s="13"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="11" t="s">
         <v>161</v>
       </c>
@@ -8162,7 +8213,7 @@
       </c>
       <c r="C6" s="13"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="11" t="s">
         <v>162</v>
       </c>
@@ -8185,10 +8236,10 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:K18"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
@@ -8200,7 +8251,7 @@
     <col min="9" max="11" width="7.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="19" customFormat="1">
       <c r="A1" s="28" t="s">
         <v>166</v>
       </c>
@@ -8235,7 +8286,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="29" t="s">
         <v>172</v>
       </c>
@@ -8268,7 +8319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="29" t="s">
         <v>174</v>
       </c>
@@ -8303,7 +8354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="29" t="s">
         <v>176</v>
       </c>
@@ -8338,7 +8389,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="29" t="s">
         <v>181</v>
       </c>
@@ -8374,7 +8425,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="29" t="s">
         <v>177</v>
       </c>
@@ -8409,7 +8460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="29" t="s">
         <v>179</v>
       </c>
@@ -8444,7 +8495,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="29" t="s">
         <v>215</v>
       </c>
@@ -8480,7 +8531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="29" t="s">
         <v>209</v>
       </c>
@@ -8516,7 +8567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" s="29" t="s">
         <v>218</v>
       </c>
@@ -8552,7 +8603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="29" t="s">
         <v>272</v>
       </c>
@@ -8588,7 +8639,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="29" t="s">
         <v>273</v>
       </c>
@@ -8624,7 +8675,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" s="29" t="s">
         <v>208</v>
       </c>
@@ -8659,7 +8710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="29" t="s">
         <v>210</v>
       </c>
@@ -8695,7 +8746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" s="29" t="s">
         <v>212</v>
       </c>
@@ -8730,7 +8781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="29" t="s">
         <v>263</v>
       </c>
@@ -8766,7 +8817,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="29" t="s">
         <v>264</v>
       </c>
@@ -8802,7 +8853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18" s="29" t="s">
         <v>267</v>
       </c>
@@ -8849,11 +8900,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84637A79-E027-48E7-B7DE-002E7C836FC2}">
   <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:Y27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="12.09765625" style="31" customWidth="1"/>
     <col min="2" max="2" width="50.69921875" style="30" customWidth="1"/>
@@ -8870,7 +8921,7 @@
     <col min="27" max="28" width="8.796875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28">
       <c r="D1" s="78" t="s">
         <v>259</v>
       </c>
@@ -8896,7 +8947,7 @@
       </c>
       <c r="W1" s="79"/>
     </row>
-    <row r="2" spans="1:28" s="53" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" s="53" customFormat="1">
       <c r="A2" s="49" t="s">
         <v>206</v>
       </c>
@@ -8993,7 +9044,7 @@
       <c r="AA2" s="49"/>
       <c r="AB2" s="49"/>
     </row>
-    <row r="3" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="44" customFormat="1">
       <c r="A3" s="42" t="s">
         <v>255</v>
       </c>
@@ -9067,7 +9118,7 @@
       <c r="AA3" s="42"/>
       <c r="AB3" s="42"/>
     </row>
-    <row r="4" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" s="44" customFormat="1">
       <c r="A4" s="42" t="s">
         <v>231</v>
       </c>
@@ -9141,7 +9192,7 @@
       <c r="AA4" s="42"/>
       <c r="AB4" s="42"/>
     </row>
-    <row r="5" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" s="44" customFormat="1">
       <c r="A5" s="42" t="s">
         <v>220</v>
       </c>
@@ -9214,7 +9265,7 @@
       <c r="AA5" s="42"/>
       <c r="AB5" s="42"/>
     </row>
-    <row r="6" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" s="44" customFormat="1">
       <c r="A6" s="42" t="s">
         <v>221</v>
       </c>
@@ -9287,7 +9338,7 @@
       <c r="AA6" s="42"/>
       <c r="AB6" s="42"/>
     </row>
-    <row r="7" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" s="44" customFormat="1">
       <c r="A7" s="42" t="s">
         <v>230</v>
       </c>
@@ -9361,7 +9412,7 @@
       <c r="AA7" s="42"/>
       <c r="AB7" s="42"/>
     </row>
-    <row r="8" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" s="44" customFormat="1">
       <c r="A8" s="42" t="s">
         <v>233</v>
       </c>
@@ -9435,7 +9486,7 @@
       <c r="AA8" s="42"/>
       <c r="AB8" s="42"/>
     </row>
-    <row r="9" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" s="44" customFormat="1">
       <c r="A9" s="42" t="s">
         <v>222</v>
       </c>
@@ -9512,7 +9563,7 @@
       <c r="AA9" s="42"/>
       <c r="AB9" s="42"/>
     </row>
-    <row r="10" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" s="44" customFormat="1">
       <c r="A10" s="42" t="s">
         <v>275</v>
       </c>
@@ -9586,7 +9637,7 @@
       <c r="AA10" s="42"/>
       <c r="AB10" s="42"/>
     </row>
-    <row r="11" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" s="44" customFormat="1">
       <c r="A11" s="42" t="s">
         <v>276</v>
       </c>
@@ -9663,7 +9714,7 @@
       <c r="AA11" s="42"/>
       <c r="AB11" s="42"/>
     </row>
-    <row r="12" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" s="44" customFormat="1">
       <c r="A12" s="42" t="s">
         <v>277</v>
       </c>
@@ -9737,7 +9788,7 @@
       <c r="AA12" s="42"/>
       <c r="AB12" s="42"/>
     </row>
-    <row r="13" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" s="44" customFormat="1">
       <c r="A13" s="42" t="s">
         <v>279</v>
       </c>
@@ -9814,7 +9865,7 @@
       <c r="AA13" s="42"/>
       <c r="AB13" s="42"/>
     </row>
-    <row r="14" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" s="44" customFormat="1">
       <c r="A14" s="42" t="s">
         <v>252</v>
       </c>
@@ -9888,7 +9939,7 @@
       <c r="AA14" s="42"/>
       <c r="AB14" s="42"/>
     </row>
-    <row r="15" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" s="44" customFormat="1">
       <c r="A15" s="42" t="s">
         <v>223</v>
       </c>
@@ -9960,7 +10011,7 @@
       <c r="AA15" s="42"/>
       <c r="AB15" s="42"/>
     </row>
-    <row r="16" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" s="44" customFormat="1">
       <c r="A16" s="42" t="s">
         <v>227</v>
       </c>
@@ -10037,7 +10088,7 @@
       <c r="AA16" s="42"/>
       <c r="AB16" s="42"/>
     </row>
-    <row r="17" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" s="44" customFormat="1">
       <c r="A17" s="42" t="s">
         <v>224</v>
       </c>
@@ -10111,7 +10162,7 @@
       <c r="AA17" s="42"/>
       <c r="AB17" s="42"/>
     </row>
-    <row r="18" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" s="44" customFormat="1">
       <c r="A18" s="42" t="s">
         <v>225</v>
       </c>
@@ -10185,7 +10236,7 @@
       <c r="AA18" s="42"/>
       <c r="AB18" s="42"/>
     </row>
-    <row r="19" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" s="44" customFormat="1">
       <c r="A19" s="42" t="s">
         <v>264</v>
       </c>
@@ -10257,7 +10308,7 @@
       <c r="AA19" s="42"/>
       <c r="AB19" s="42"/>
     </row>
-    <row r="20" spans="1:28" s="44" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" s="44" customFormat="1">
       <c r="A20" s="42" t="s">
         <v>226</v>
       </c>
@@ -10335,7 +10386,7 @@
       <c r="AA20" s="42"/>
       <c r="AB20" s="42"/>
     </row>
-    <row r="21" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1">
       <c r="A21" s="45" t="s">
         <v>228</v>
       </c>
@@ -10413,7 +10464,7 @@
       <c r="AA21" s="45"/>
       <c r="AB21" s="45"/>
     </row>
-    <row r="22" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1">
       <c r="A22" s="45" t="s">
         <v>218</v>
       </c>
@@ -10487,7 +10538,7 @@
       <c r="AA22" s="45"/>
       <c r="AB22" s="45"/>
     </row>
-    <row r="23" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" s="27" customFormat="1" ht="19.2" customHeight="1">
       <c r="A23" s="45" t="s">
         <v>263</v>
       </c>
@@ -10561,7 +10612,7 @@
       <c r="AA23" s="45"/>
       <c r="AB23" s="45"/>
     </row>
-    <row r="24" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A24" s="36" t="s">
         <v>250</v>
       </c>
@@ -10639,7 +10690,7 @@
       <c r="AA24" s="36"/>
       <c r="AB24" s="36"/>
     </row>
-    <row r="25" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A25" s="36" t="s">
         <v>239</v>
       </c>
@@ -10717,7 +10768,7 @@
       <c r="AA25" s="36"/>
       <c r="AB25" s="36"/>
     </row>
-    <row r="26" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A26" s="36" t="s">
         <v>251</v>
       </c>
@@ -10791,7 +10842,7 @@
       <c r="AA26" s="36"/>
       <c r="AB26" s="36"/>
     </row>
-    <row r="27" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A27" s="36" t="s">
         <v>267</v>
       </c>
@@ -10865,27 +10916,70 @@
       <c r="AA27" s="36"/>
       <c r="AB27" s="36"/>
     </row>
-    <row r="28" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="34"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="34"/>
-      <c r="N28" s="34"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="34"/>
-      <c r="Q28" s="34"/>
-      <c r="R28" s="34"/>
-      <c r="S28" s="34"/>
-      <c r="T28" s="34"/>
-      <c r="U28" s="61"/>
+    <row r="28" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
+      <c r="A28" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="B28" s="81" t="s">
+        <v>285</v>
+      </c>
+      <c r="C28" s="59">
+        <v>1</v>
+      </c>
+      <c r="D28" s="57">
+        <v>1</v>
+      </c>
+      <c r="E28" s="38">
+        <v>1</v>
+      </c>
+      <c r="F28" s="38">
+        <v>1</v>
+      </c>
+      <c r="G28" s="38">
+        <v>1</v>
+      </c>
+      <c r="H28" s="38">
+        <v>1</v>
+      </c>
+      <c r="I28" s="38">
+        <v>1</v>
+      </c>
+      <c r="J28" s="38">
+        <v>1</v>
+      </c>
+      <c r="K28" s="38">
+        <v>1</v>
+      </c>
+      <c r="L28" s="38">
+        <v>1</v>
+      </c>
+      <c r="M28" s="38">
+        <v>1</v>
+      </c>
+      <c r="N28" s="38">
+        <v>1</v>
+      </c>
+      <c r="O28" s="38">
+        <v>1</v>
+      </c>
+      <c r="P28" s="38">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="38">
+        <v>1</v>
+      </c>
+      <c r="R28" s="38">
+        <v>1</v>
+      </c>
+      <c r="S28" s="38">
+        <v>1</v>
+      </c>
+      <c r="T28" s="38">
+        <v>1</v>
+      </c>
+      <c r="U28" s="65">
+        <v>0</v>
+      </c>
       <c r="V28" s="62"/>
       <c r="W28" s="35"/>
       <c r="X28" s="58"/>
@@ -10894,7 +10988,7 @@
       <c r="AA28" s="36"/>
       <c r="AB28" s="36"/>
     </row>
-    <row r="29" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A29" s="36"/>
       <c r="B29" s="32"/>
       <c r="C29" s="59"/>
@@ -10924,7 +11018,7 @@
       <c r="AA29" s="36"/>
       <c r="AB29" s="36"/>
     </row>
-    <row r="30" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A30" s="36"/>
       <c r="B30" s="32"/>
       <c r="C30" s="58"/>
@@ -10954,7 +11048,7 @@
       <c r="AA30" s="36"/>
       <c r="AB30" s="36"/>
     </row>
-    <row r="31" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A31" s="36"/>
       <c r="B31" s="36"/>
       <c r="C31" s="58"/>
@@ -10984,7 +11078,7 @@
       <c r="AA31" s="36"/>
       <c r="AB31" s="36"/>
     </row>
-    <row r="32" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A32" s="36"/>
       <c r="B32" s="32"/>
       <c r="C32" s="58"/>
@@ -11014,7 +11108,7 @@
       <c r="AA32" s="36"/>
       <c r="AB32" s="36"/>
     </row>
-    <row r="33" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A33" s="36"/>
       <c r="B33" s="36"/>
       <c r="C33" s="59"/>
@@ -11044,7 +11138,7 @@
       <c r="AA33" s="36"/>
       <c r="AB33" s="36"/>
     </row>
-    <row r="34" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A34" s="36"/>
       <c r="B34" s="32"/>
       <c r="C34" s="58"/>
@@ -11074,7 +11168,7 @@
       <c r="AA34" s="36"/>
       <c r="AB34" s="36"/>
     </row>
-    <row r="35" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:28" s="26" customFormat="1" ht="19.2" customHeight="1">
       <c r="A35" s="36"/>
       <c r="C35" s="58"/>
       <c r="D35" s="61"/>
@@ -11109,207 +11203,237 @@
     <mergeCell ref="D1:T1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:P11 C24:P24 C20:P22 C12:C13 C14:P18">
+    <cfRule type="cellIs" dxfId="46" priority="58" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:P11 C24:P26 C20:P22 C12:C13 C14:P18">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:P26">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:K23 M23:P23">
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:K23 M23:P23">
+    <cfRule type="cellIs" dxfId="42" priority="53" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23">
+    <cfRule type="cellIs" dxfId="41" priority="44" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:S6 Q24 Q7:Q11 Q20:Q22 Q14:Q18">
     <cfRule type="cellIs" dxfId="40" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:P11 C24:P26 C20:P22 C12:C13 C14:P18">
+  <conditionalFormatting sqref="Q3:S6 Q25:S26 Q24 Q7:Q11 Q20:Q22 Q14:Q18">
     <cfRule type="cellIs" dxfId="39" priority="51" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25:P26">
-    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
+  <conditionalFormatting sqref="Q25:S26">
+    <cfRule type="cellIs" dxfId="38" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:K23 M23:P23">
-    <cfRule type="cellIs" dxfId="37" priority="48" operator="equal">
+  <conditionalFormatting sqref="Q23">
+    <cfRule type="cellIs" dxfId="37" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23:K23 M23:P23">
-    <cfRule type="cellIs" dxfId="36" priority="47" operator="notEqual">
+  <conditionalFormatting sqref="Q23">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:S11 R20:S24 R14:S18">
+    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R7:S11 R20:S24 R14:S18">
+    <cfRule type="cellIs" dxfId="34" priority="46" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="35" priority="38" operator="notEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:S6 Q24 Q7:Q11 Q20:Q22 Q14:Q18">
-    <cfRule type="cellIs" dxfId="34" priority="46" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:S6 Q25:S26 Q24 Q7:Q11 Q20:Q22 Q14:Q18">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="notEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q25:S26">
-    <cfRule type="cellIs" dxfId="32" priority="44" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q23">
-    <cfRule type="cellIs" dxfId="31" priority="43" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q23">
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="notEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7:S11 R20:S24 R14:S18">
-    <cfRule type="cellIs" dxfId="29" priority="41" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R7:S11 R20:S24 R14:S18">
-    <cfRule type="cellIs" dxfId="28" priority="40" operator="notEqual">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:P19">
-    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19:P19">
-    <cfRule type="cellIs" dxfId="25" priority="36" operator="notEqual">
+    <cfRule type="cellIs" dxfId="31" priority="42" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q19">
-    <cfRule type="cellIs" dxfId="24" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q19">
-    <cfRule type="cellIs" dxfId="23" priority="34" operator="notEqual">
+    <cfRule type="cellIs" dxfId="29" priority="40" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R19:S19">
+    <cfRule type="cellIs" dxfId="28" priority="39" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R19:S19">
+    <cfRule type="cellIs" dxfId="27" priority="38" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:P27">
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27:P27">
+    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q27:S27">
+    <cfRule type="cellIs" dxfId="24" priority="35" operator="notEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q27:S27">
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="T3:T6">
     <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R19:S19">
+  <conditionalFormatting sqref="T3:T6 T25:T26">
     <cfRule type="cellIs" dxfId="21" priority="32" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:P27">
-    <cfRule type="cellIs" dxfId="20" priority="31" operator="notEqual">
+  <conditionalFormatting sqref="T25:T26">
+    <cfRule type="cellIs" dxfId="20" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27:P27">
+  <conditionalFormatting sqref="T7:T11 T20:T24 T14:T18">
     <cfRule type="cellIs" dxfId="19" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27:S27">
+  <conditionalFormatting sqref="T7:T11 T20:T24 T14:T18">
     <cfRule type="cellIs" dxfId="18" priority="29" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q27:S27">
+  <conditionalFormatting sqref="T19">
     <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T6">
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
+  <conditionalFormatting sqref="T19">
+    <cfRule type="cellIs" dxfId="16" priority="27" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T3:T6 T25:T26">
+  <conditionalFormatting sqref="T27">
     <cfRule type="cellIs" dxfId="15" priority="26" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T25:T26">
+  <conditionalFormatting sqref="T27">
     <cfRule type="cellIs" dxfId="14" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T7:T11 T20:T24 T14:T18">
+  <conditionalFormatting sqref="D12:P13">
     <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T7:T11 T20:T24 T14:T18">
+  <conditionalFormatting sqref="D12:P13">
     <cfRule type="cellIs" dxfId="12" priority="23" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T19">
+  <conditionalFormatting sqref="Q12:Q13">
     <cfRule type="cellIs" dxfId="11" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T19">
+  <conditionalFormatting sqref="Q12:Q13">
     <cfRule type="cellIs" dxfId="10" priority="21" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27">
-    <cfRule type="cellIs" dxfId="9" priority="20" operator="notEqual">
+  <conditionalFormatting sqref="R12:S13">
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T27">
-    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
+  <conditionalFormatting sqref="R12:S13">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:P13">
+  <conditionalFormatting sqref="T12:T13">
     <cfRule type="cellIs" dxfId="7" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D12:P13">
+  <conditionalFormatting sqref="T12:T13">
     <cfRule type="cellIs" dxfId="6" priority="17" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q12:Q13">
-    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+  <conditionalFormatting sqref="D28:P28">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q12:Q13">
-    <cfRule type="cellIs" dxfId="4" priority="15" operator="notEqual">
+  <conditionalFormatting sqref="D28:P28">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R12:S13">
-    <cfRule type="cellIs" dxfId="3" priority="14" operator="equal">
+  <conditionalFormatting sqref="Q28:S28">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R12:S13">
-    <cfRule type="cellIs" dxfId="2" priority="13" operator="notEqual">
+  <conditionalFormatting sqref="Q28:S28">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T12:T13">
-    <cfRule type="cellIs" dxfId="1" priority="12" operator="equal">
+  <conditionalFormatting sqref="T28">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T12:T13">
-    <cfRule type="cellIs" dxfId="0" priority="11" operator="notEqual">
+  <conditionalFormatting sqref="T28">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11323,17 +11447,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="21.69921875" customWidth="1"/>
     <col min="3" max="3" width="51.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="19" customFormat="1">
       <c r="A1" s="19" t="s">
         <v>166</v>
       </c>
@@ -11344,7 +11468,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" s="23" customFormat="1">
       <c r="A2" s="23" t="s">
         <v>195</v>
       </c>
@@ -11355,7 +11479,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" s="23" customFormat="1">
       <c r="A3" s="23" t="s">
         <v>196</v>
       </c>
@@ -11366,7 +11490,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="23" customFormat="1">
       <c r="A4" s="23" t="s">
         <v>199</v>
       </c>
@@ -11374,7 +11498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>185</v>
       </c>
@@ -11385,7 +11509,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -11396,7 +11520,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>187</v>
       </c>
@@ -11404,26 +11528,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>188</v>
       </c>
       <c r="B8">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="C8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>194</v>
       </c>
       <c r="B9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>189</v>
       </c>
@@ -11434,7 +11558,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>200</v>
       </c>
@@ -11442,7 +11566,7 @@
         <v>1.5E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
new scenarios and data
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick.scott\Desktop\Github\covasim-australia\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262F5C1A-D6BD-4B9F-A087-597A13D3C249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5E994A-410B-4633-BC10-93B7A3771654}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="762" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10470" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="762" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="epi_data" sheetId="1" r:id="rId1"/>
@@ -2092,10 +2092,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -2826,7 +2825,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2982,7 +2981,6 @@
     <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="29" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3062,7 +3060,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="171">
+  <dxfs count="80">
     <dxf>
       <fill>
         <patternFill>
@@ -3623,643 +3621,6 @@
         <color theme="0" tint="-0.34998626667073579"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4924,7 +4285,7 @@
       <c r="J14" s="6">
         <v>0</v>
       </c>
-      <c r="K14" s="73">
+      <c r="K14" s="72">
         <v>500</v>
       </c>
       <c r="L14" s="6">
@@ -4947,7 +4308,7 @@
       <c r="J15" s="6">
         <v>0</v>
       </c>
-      <c r="K15" s="73">
+      <c r="K15" s="72">
         <v>500</v>
       </c>
       <c r="L15" s="6">
@@ -4970,7 +4331,7 @@
       <c r="J16" s="6">
         <v>0</v>
       </c>
-      <c r="K16" s="73">
+      <c r="K16" s="72">
         <v>500</v>
       </c>
       <c r="L16" s="6">
@@ -4999,7 +4360,7 @@
       <c r="J17" s="6">
         <v>0</v>
       </c>
-      <c r="K17" s="73">
+      <c r="K17" s="72">
         <v>500</v>
       </c>
       <c r="L17" s="6">
@@ -5028,7 +4389,7 @@
       <c r="J18" s="6">
         <v>0</v>
       </c>
-      <c r="K18" s="73">
+      <c r="K18" s="72">
         <v>1000</v>
       </c>
       <c r="L18" s="6">
@@ -6363,52 +5724,52 @@
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="82">
+      <c r="B2" s="81">
         <v>0.65986800000000001</v>
       </c>
-      <c r="C2" s="82">
+      <c r="C2" s="81">
         <v>0.503965</v>
       </c>
-      <c r="D2" s="82">
+      <c r="D2" s="81">
         <v>0.21477299999999999</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="81">
         <v>9.4509999999999997E-2</v>
       </c>
-      <c r="F2" s="82">
+      <c r="F2" s="81">
         <v>0.15807499999999999</v>
       </c>
-      <c r="G2" s="82">
+      <c r="G2" s="81">
         <v>0.33119399999999999</v>
       </c>
-      <c r="H2" s="82">
+      <c r="H2" s="81">
         <v>0.61729000000000001</v>
       </c>
-      <c r="I2" s="82">
+      <c r="I2" s="81">
         <v>0.62299000000000004</v>
       </c>
-      <c r="J2" s="82">
+      <c r="J2" s="81">
         <v>0.22986699999999999</v>
       </c>
-      <c r="K2" s="82">
+      <c r="K2" s="81">
         <v>7.7709E-2</v>
       </c>
-      <c r="L2" s="82">
+      <c r="L2" s="81">
         <v>7.2123999999999994E-2</v>
       </c>
-      <c r="M2" s="82">
+      <c r="M2" s="81">
         <v>3.5873000000000002E-2</v>
       </c>
-      <c r="N2" s="82">
+      <c r="N2" s="81">
         <v>2.9784999999999999E-2</v>
       </c>
-      <c r="O2" s="82">
+      <c r="O2" s="81">
         <v>9.92E-3</v>
       </c>
-      <c r="P2" s="82">
+      <c r="P2" s="81">
         <v>4.2420000000000001E-3</v>
       </c>
-      <c r="Q2" s="82">
+      <c r="Q2" s="81">
         <v>6.1619999999999999E-3</v>
       </c>
       <c r="R2" s="3" t="s">
@@ -6419,52 +5780,52 @@
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="82">
+      <c r="B3" s="81">
         <v>0.31477699999999997</v>
       </c>
-      <c r="C3" s="82">
+      <c r="C3" s="81">
         <v>0.89546000000000003</v>
       </c>
-      <c r="D3" s="82">
+      <c r="D3" s="81">
         <v>0.412466</v>
       </c>
-      <c r="E3" s="82">
+      <c r="E3" s="81">
         <v>0.12892600000000001</v>
       </c>
-      <c r="F3" s="82">
+      <c r="F3" s="81">
         <v>3.9333E-2</v>
       </c>
-      <c r="G3" s="82">
+      <c r="G3" s="81">
         <v>0.149588</v>
       </c>
-      <c r="H3" s="82">
+      <c r="H3" s="81">
         <v>0.431338</v>
       </c>
-      <c r="I3" s="82">
+      <c r="I3" s="81">
         <v>0.62494499999999997</v>
       </c>
-      <c r="J3" s="82">
+      <c r="J3" s="81">
         <v>0.47687299999999999</v>
       </c>
-      <c r="K3" s="82">
+      <c r="K3" s="81">
         <v>0.162493</v>
       </c>
-      <c r="L3" s="82">
+      <c r="L3" s="81">
         <v>4.9998000000000001E-2</v>
       </c>
-      <c r="M3" s="82">
+      <c r="M3" s="81">
         <v>2.9618999999999999E-2</v>
       </c>
-      <c r="N3" s="82">
+      <c r="N3" s="81">
         <v>1.6726000000000001E-2</v>
       </c>
-      <c r="O3" s="82">
+      <c r="O3" s="81">
         <v>9.5239999999999995E-3</v>
       </c>
-      <c r="P3" s="82">
+      <c r="P3" s="81">
         <v>4.1780000000000003E-3</v>
       </c>
-      <c r="Q3" s="82">
+      <c r="Q3" s="81">
         <v>4.3559999999999996E-3</v>
       </c>
     </row>
@@ -6472,52 +5833,52 @@
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="82">
+      <c r="B4" s="81">
         <v>0.13282099999999999</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="81">
         <v>0.40507300000000002</v>
       </c>
-      <c r="D4" s="82">
+      <c r="D4" s="81">
         <v>1.433889</v>
       </c>
-      <c r="E4" s="82">
+      <c r="E4" s="81">
         <v>0.39880599999999999</v>
       </c>
-      <c r="F4" s="82">
+      <c r="F4" s="81">
         <v>5.5355000000000001E-2</v>
       </c>
-      <c r="G4" s="82">
+      <c r="G4" s="81">
         <v>3.4249000000000002E-2</v>
       </c>
-      <c r="H4" s="82">
+      <c r="H4" s="81">
         <v>0.119908</v>
       </c>
-      <c r="I4" s="82">
+      <c r="I4" s="81">
         <v>0.375305</v>
       </c>
-      <c r="J4" s="82">
+      <c r="J4" s="81">
         <v>0.56235800000000002</v>
       </c>
-      <c r="K4" s="82">
+      <c r="K4" s="81">
         <v>0.27133200000000002</v>
       </c>
-      <c r="L4" s="82">
+      <c r="L4" s="81">
         <v>7.5578999999999993E-2</v>
       </c>
-      <c r="M4" s="82">
+      <c r="M4" s="81">
         <v>1.8716E-2</v>
       </c>
-      <c r="N4" s="82">
+      <c r="N4" s="81">
         <v>1.4074E-2</v>
       </c>
-      <c r="O4" s="82">
+      <c r="O4" s="81">
         <v>1.0442E-2</v>
       </c>
-      <c r="P4" s="82">
+      <c r="P4" s="81">
         <v>7.698E-3</v>
       </c>
-      <c r="Q4" s="82">
+      <c r="Q4" s="81">
         <v>4.1580000000000002E-3</v>
       </c>
     </row>
@@ -6525,52 +5886,52 @@
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="82">
+      <c r="B5" s="81">
         <v>6.1564000000000001E-2</v>
       </c>
-      <c r="C5" s="82">
+      <c r="C5" s="81">
         <v>0.116366</v>
       </c>
-      <c r="D5" s="82">
+      <c r="D5" s="81">
         <v>0.45097300000000001</v>
       </c>
-      <c r="E5" s="82">
+      <c r="E5" s="81">
         <v>1.1951130000000001</v>
       </c>
-      <c r="F5" s="82">
+      <c r="F5" s="81">
         <v>0.18948100000000001</v>
       </c>
-      <c r="G5" s="82">
+      <c r="G5" s="81">
         <v>4.1827000000000003E-2</v>
       </c>
-      <c r="H5" s="82">
+      <c r="H5" s="81">
         <v>2.5562999999999999E-2</v>
       </c>
-      <c r="I5" s="82">
+      <c r="I5" s="81">
         <v>0.15873200000000001</v>
       </c>
-      <c r="J5" s="82">
+      <c r="J5" s="81">
         <v>0.359678</v>
       </c>
-      <c r="K5" s="82">
+      <c r="K5" s="81">
         <v>0.46463599999999999</v>
       </c>
-      <c r="L5" s="82">
+      <c r="L5" s="81">
         <v>0.211951</v>
       </c>
-      <c r="M5" s="82">
+      <c r="M5" s="81">
         <v>4.7126000000000001E-2</v>
       </c>
-      <c r="N5" s="82">
+      <c r="N5" s="81">
         <v>1.9890000000000001E-2</v>
       </c>
-      <c r="O5" s="82">
+      <c r="O5" s="81">
         <v>1.1908E-2</v>
       </c>
-      <c r="P5" s="82">
+      <c r="P5" s="81">
         <v>4.9189999999999998E-3</v>
       </c>
-      <c r="Q5" s="82">
+      <c r="Q5" s="81">
         <v>3.0739999999999999E-3</v>
       </c>
     </row>
@@ -6578,52 +5939,52 @@
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="82">
+      <c r="B6" s="81">
         <v>0.14102200000000001</v>
       </c>
-      <c r="C6" s="82">
+      <c r="C6" s="81">
         <v>6.4642000000000005E-2</v>
       </c>
-      <c r="D6" s="82">
+      <c r="D6" s="81">
         <v>8.3546999999999996E-2</v>
       </c>
-      <c r="E6" s="82">
+      <c r="E6" s="81">
         <v>0.40224300000000002</v>
       </c>
-      <c r="F6" s="82">
+      <c r="F6" s="81">
         <v>1.1921930000000001</v>
       </c>
-      <c r="G6" s="82">
+      <c r="G6" s="81">
         <v>0.248001</v>
       </c>
-      <c r="H6" s="82">
+      <c r="H6" s="81">
         <v>4.6676000000000002E-2</v>
       </c>
-      <c r="I6" s="82">
+      <c r="I6" s="81">
         <v>2.2216E-2</v>
       </c>
-      <c r="J6" s="82">
+      <c r="J6" s="81">
         <v>0.139739</v>
       </c>
-      <c r="K6" s="82">
+      <c r="K6" s="81">
         <v>0.43590299999999998</v>
       </c>
-      <c r="L6" s="82">
+      <c r="L6" s="81">
         <v>0.28106300000000001</v>
       </c>
-      <c r="M6" s="82">
+      <c r="M6" s="81">
         <v>0.103923</v>
       </c>
-      <c r="N6" s="82">
+      <c r="N6" s="81">
         <v>2.0109999999999999E-2</v>
       </c>
-      <c r="O6" s="82">
+      <c r="O6" s="81">
         <v>4.0249999999999999E-3</v>
       </c>
-      <c r="P6" s="82">
+      <c r="P6" s="81">
         <v>5.359E-3</v>
       </c>
-      <c r="Q6" s="82">
+      <c r="Q6" s="81">
         <v>3.6970000000000002E-3</v>
       </c>
     </row>
@@ -6631,52 +5992,52 @@
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="82">
+      <c r="B7" s="81">
         <v>0.42515599999999998</v>
       </c>
-      <c r="C7" s="82">
+      <c r="C7" s="81">
         <v>0.13725799999999999</v>
       </c>
-      <c r="D7" s="82">
+      <c r="D7" s="81">
         <v>4.3091999999999998E-2</v>
       </c>
-      <c r="E7" s="82">
+      <c r="E7" s="81">
         <v>8.3335999999999993E-2</v>
       </c>
-      <c r="F7" s="82">
+      <c r="F7" s="81">
         <v>0.27788800000000002</v>
       </c>
-      <c r="G7" s="82">
+      <c r="G7" s="81">
         <v>1.089831</v>
       </c>
-      <c r="H7" s="82">
+      <c r="H7" s="81">
         <v>0.22731799999999999</v>
       </c>
-      <c r="I7" s="82">
+      <c r="I7" s="81">
         <v>4.1119000000000003E-2</v>
       </c>
-      <c r="J7" s="82">
+      <c r="J7" s="81">
         <v>2.086E-2</v>
       </c>
-      <c r="K7" s="82">
+      <c r="K7" s="81">
         <v>7.6337000000000002E-2</v>
       </c>
-      <c r="L7" s="82">
+      <c r="L7" s="81">
         <v>0.20813300000000001</v>
       </c>
-      <c r="M7" s="82">
+      <c r="M7" s="81">
         <v>0.106445</v>
       </c>
-      <c r="N7" s="82">
+      <c r="N7" s="81">
         <v>4.3403999999999998E-2</v>
       </c>
-      <c r="O7" s="82">
+      <c r="O7" s="81">
         <v>1.0788000000000001E-2</v>
       </c>
-      <c r="P7" s="82">
+      <c r="P7" s="81">
         <v>1.526E-3</v>
       </c>
-      <c r="Q7" s="82">
+      <c r="Q7" s="81">
         <v>6.8170000000000001E-3</v>
       </c>
     </row>
@@ -6684,52 +6045,52 @@
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="82">
+      <c r="B8" s="81">
         <v>0.63256400000000002</v>
       </c>
-      <c r="C8" s="82">
+      <c r="C8" s="81">
         <v>0.52978800000000004</v>
       </c>
-      <c r="D8" s="82">
+      <c r="D8" s="81">
         <v>0.221806</v>
       </c>
-      <c r="E8" s="82">
+      <c r="E8" s="81">
         <v>4.1730000000000003E-2</v>
       </c>
-      <c r="F8" s="82">
+      <c r="F8" s="81">
         <v>6.4195000000000002E-2</v>
       </c>
-      <c r="G8" s="82">
+      <c r="G8" s="81">
         <v>0.22583800000000001</v>
       </c>
-      <c r="H8" s="82">
+      <c r="H8" s="81">
         <v>0.93633699999999997</v>
       </c>
-      <c r="I8" s="82">
+      <c r="I8" s="81">
         <v>0.236536</v>
       </c>
-      <c r="J8" s="82">
+      <c r="J8" s="81">
         <v>7.1504999999999999E-2</v>
       </c>
-      <c r="K8" s="82">
+      <c r="K8" s="81">
         <v>2.2377000000000001E-2</v>
       </c>
-      <c r="L8" s="82">
+      <c r="L8" s="81">
         <v>4.0784000000000001E-2</v>
       </c>
-      <c r="M8" s="82">
+      <c r="M8" s="81">
         <v>6.2238000000000002E-2</v>
       </c>
-      <c r="N8" s="82">
+      <c r="N8" s="81">
         <v>5.9047000000000002E-2</v>
       </c>
-      <c r="O8" s="82">
+      <c r="O8" s="81">
         <v>1.0583E-2</v>
       </c>
-      <c r="P8" s="82">
+      <c r="P8" s="81">
         <v>5.4229999999999999E-3</v>
       </c>
-      <c r="Q8" s="82">
+      <c r="Q8" s="81">
         <v>3.594E-3</v>
       </c>
     </row>
@@ -6737,52 +6098,52 @@
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="82">
+      <c r="B9" s="81">
         <v>0.53381800000000001</v>
       </c>
-      <c r="C9" s="82">
+      <c r="C9" s="81">
         <v>0.76395199999999996</v>
       </c>
-      <c r="D9" s="82">
+      <c r="D9" s="81">
         <v>0.56459199999999998</v>
       </c>
-      <c r="E9" s="82">
+      <c r="E9" s="81">
         <v>0.20846700000000001</v>
       </c>
-      <c r="F9" s="82">
+      <c r="F9" s="81">
         <v>3.1192000000000001E-2</v>
       </c>
-      <c r="G9" s="82">
+      <c r="G9" s="81">
         <v>4.0858999999999999E-2</v>
       </c>
-      <c r="H9" s="82">
+      <c r="H9" s="81">
         <v>0.16445899999999999</v>
       </c>
-      <c r="I9" s="82">
+      <c r="I9" s="81">
         <v>0.94722799999999996</v>
       </c>
-      <c r="J9" s="82">
+      <c r="J9" s="81">
         <v>0.174175</v>
       </c>
-      <c r="K9" s="82">
+      <c r="K9" s="81">
         <v>4.2037999999999999E-2</v>
       </c>
-      <c r="L9" s="82">
+      <c r="L9" s="81">
         <v>2.5260000000000001E-2</v>
       </c>
-      <c r="M9" s="82">
+      <c r="M9" s="81">
         <v>1.8571000000000001E-2</v>
       </c>
-      <c r="N9" s="82">
+      <c r="N9" s="81">
         <v>3.2816999999999999E-2</v>
       </c>
-      <c r="O9" s="82">
+      <c r="O9" s="81">
         <v>1.9281E-2</v>
       </c>
-      <c r="P9" s="82">
+      <c r="P9" s="81">
         <v>9.4479999999999998E-3</v>
       </c>
-      <c r="Q9" s="82">
+      <c r="Q9" s="81">
         <v>2.7920000000000002E-3</v>
       </c>
     </row>
@@ -6790,52 +6151,52 @@
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="82">
+      <c r="B10" s="81">
         <v>0.24148500000000001</v>
       </c>
-      <c r="C10" s="82">
+      <c r="C10" s="81">
         <v>0.53524700000000003</v>
       </c>
-      <c r="D10" s="82">
+      <c r="D10" s="81">
         <v>0.726603</v>
       </c>
-      <c r="E10" s="82">
+      <c r="E10" s="81">
         <v>0.44772899999999999</v>
       </c>
-      <c r="F10" s="82">
+      <c r="F10" s="81">
         <v>0.109945</v>
       </c>
-      <c r="G10" s="82">
+      <c r="G10" s="81">
         <v>3.4540000000000001E-2</v>
       </c>
-      <c r="H10" s="82">
+      <c r="H10" s="81">
         <v>7.7090000000000006E-2</v>
       </c>
-      <c r="I10" s="82">
+      <c r="I10" s="81">
         <v>0.18113699999999999</v>
       </c>
-      <c r="J10" s="82">
+      <c r="J10" s="81">
         <v>0.77208200000000005</v>
       </c>
-      <c r="K10" s="82">
+      <c r="K10" s="81">
         <v>0.16217000000000001</v>
       </c>
-      <c r="L10" s="82">
+      <c r="L10" s="81">
         <v>3.7186999999999998E-2</v>
       </c>
-      <c r="M10" s="82">
+      <c r="M10" s="81">
         <v>7.443E-3</v>
       </c>
-      <c r="N10" s="82">
+      <c r="N10" s="81">
         <v>2.1396999999999999E-2</v>
       </c>
-      <c r="O10" s="82">
+      <c r="O10" s="81">
         <v>2.512E-2</v>
       </c>
-      <c r="P10" s="82">
+      <c r="P10" s="81">
         <v>9.8720000000000006E-3</v>
       </c>
-      <c r="Q10" s="82">
+      <c r="Q10" s="81">
         <v>6.6759999999999996E-3</v>
       </c>
     </row>
@@ -6843,52 +6204,52 @@
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="82">
+      <c r="B11" s="81">
         <v>0.122279</v>
       </c>
-      <c r="C11" s="82">
+      <c r="C11" s="81">
         <v>0.276169</v>
       </c>
-      <c r="D11" s="82">
+      <c r="D11" s="81">
         <v>0.46051500000000001</v>
       </c>
-      <c r="E11" s="82">
+      <c r="E11" s="81">
         <v>0.61675800000000003</v>
       </c>
-      <c r="F11" s="82">
+      <c r="F11" s="81">
         <v>0.32389400000000002</v>
       </c>
-      <c r="G11" s="82">
+      <c r="G11" s="81">
         <v>7.7887999999999999E-2</v>
       </c>
-      <c r="H11" s="82">
+      <c r="H11" s="81">
         <v>3.0709E-2</v>
       </c>
-      <c r="I11" s="82">
+      <c r="I11" s="81">
         <v>8.0238000000000004E-2</v>
       </c>
-      <c r="J11" s="82">
+      <c r="J11" s="81">
         <v>0.164073</v>
       </c>
-      <c r="K11" s="82">
+      <c r="K11" s="81">
         <v>0.67377399999999998</v>
       </c>
-      <c r="L11" s="82">
+      <c r="L11" s="81">
         <v>0.140821</v>
       </c>
-      <c r="M11" s="82">
+      <c r="M11" s="81">
         <v>2.7285E-2</v>
       </c>
-      <c r="N11" s="82">
+      <c r="N11" s="81">
         <v>1.1768000000000001E-2</v>
       </c>
-      <c r="O11" s="82">
+      <c r="O11" s="81">
         <v>9.0639999999999991E-3</v>
       </c>
-      <c r="P11" s="82">
+      <c r="P11" s="81">
         <v>8.3899999999999999E-3</v>
       </c>
-      <c r="Q11" s="82">
+      <c r="Q11" s="81">
         <v>1.2394000000000001E-2</v>
       </c>
     </row>
@@ -6896,52 +6257,52 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="82">
+      <c r="B12" s="81">
         <v>0.202735</v>
       </c>
-      <c r="C12" s="82">
+      <c r="C12" s="81">
         <v>0.16897499999999999</v>
       </c>
-      <c r="D12" s="82">
+      <c r="D12" s="81">
         <v>0.30529200000000001</v>
       </c>
-      <c r="E12" s="82">
+      <c r="E12" s="81">
         <v>0.41128100000000001</v>
       </c>
-      <c r="F12" s="82">
+      <c r="F12" s="81">
         <v>0.39054499999999998</v>
       </c>
-      <c r="G12" s="82">
+      <c r="G12" s="81">
         <v>0.23483599999999999</v>
       </c>
-      <c r="H12" s="82">
+      <c r="H12" s="81">
         <v>9.1048000000000004E-2</v>
       </c>
-      <c r="I12" s="82">
+      <c r="I12" s="81">
         <v>4.861E-2</v>
       </c>
-      <c r="J12" s="82">
+      <c r="J12" s="81">
         <v>7.9533999999999994E-2</v>
       </c>
-      <c r="K12" s="82">
+      <c r="K12" s="81">
         <v>0.187475</v>
       </c>
-      <c r="L12" s="82">
+      <c r="L12" s="81">
         <v>0.66868700000000003</v>
       </c>
-      <c r="M12" s="82">
+      <c r="M12" s="81">
         <v>0.13591600000000001</v>
       </c>
-      <c r="N12" s="82">
+      <c r="N12" s="81">
         <v>2.6984999999999999E-2</v>
       </c>
-      <c r="O12" s="82">
+      <c r="O12" s="81">
         <v>8.7309999999999992E-3</v>
       </c>
-      <c r="P12" s="82">
+      <c r="P12" s="81">
         <v>9.3959999999999998E-3</v>
       </c>
-      <c r="Q12" s="82">
+      <c r="Q12" s="81">
         <v>2.0105999999999999E-2</v>
       </c>
     </row>
@@ -6949,52 +6310,52 @@
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="82">
+      <c r="B13" s="81">
         <v>0.32726300000000003</v>
       </c>
-      <c r="C13" s="82">
+      <c r="C13" s="81">
         <v>0.32473099999999999</v>
       </c>
-      <c r="D13" s="82">
+      <c r="D13" s="81">
         <v>0.21896099999999999</v>
       </c>
-      <c r="E13" s="82">
+      <c r="E13" s="81">
         <v>0.30264000000000002</v>
       </c>
-      <c r="F13" s="82">
+      <c r="F13" s="81">
         <v>0.28360600000000002</v>
       </c>
-      <c r="G13" s="82">
+      <c r="G13" s="81">
         <v>0.32831300000000002</v>
       </c>
-      <c r="H13" s="82">
+      <c r="H13" s="81">
         <v>0.25703799999999999</v>
       </c>
-      <c r="I13" s="82">
+      <c r="I13" s="81">
         <v>8.4280999999999995E-2</v>
       </c>
-      <c r="J13" s="82">
+      <c r="J13" s="81">
         <v>4.2615E-2</v>
       </c>
-      <c r="K13" s="82">
+      <c r="K13" s="81">
         <v>0.12336</v>
       </c>
-      <c r="L13" s="82">
+      <c r="L13" s="81">
         <v>0.21965000000000001</v>
       </c>
-      <c r="M13" s="82">
+      <c r="M13" s="81">
         <v>0.70332499999999998</v>
       </c>
-      <c r="N13" s="82">
+      <c r="N13" s="81">
         <v>0.14740900000000001</v>
       </c>
-      <c r="O13" s="82">
+      <c r="O13" s="81">
         <v>4.3435000000000001E-2</v>
       </c>
-      <c r="P13" s="82">
+      <c r="P13" s="81">
         <v>7.1599999999999997E-3</v>
       </c>
-      <c r="Q13" s="82">
+      <c r="Q13" s="81">
         <v>2.0524000000000001E-2</v>
       </c>
     </row>
@@ -7002,52 +6363,52 @@
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="82">
+      <c r="B14" s="81">
         <v>0.39001200000000003</v>
       </c>
-      <c r="C14" s="82">
+      <c r="C14" s="81">
         <v>0.34861300000000001</v>
       </c>
-      <c r="D14" s="82">
+      <c r="D14" s="81">
         <v>0.24646000000000001</v>
       </c>
-      <c r="E14" s="82">
+      <c r="E14" s="81">
         <v>0.221558</v>
       </c>
-      <c r="F14" s="82">
+      <c r="F14" s="81">
         <v>0.154866</v>
       </c>
-      <c r="G14" s="82">
+      <c r="G14" s="81">
         <v>0.21662200000000001</v>
       </c>
-      <c r="H14" s="82">
+      <c r="H14" s="81">
         <v>0.292574</v>
       </c>
-      <c r="I14" s="82">
+      <c r="I14" s="81">
         <v>0.21071000000000001</v>
       </c>
-      <c r="J14" s="82">
+      <c r="J14" s="81">
         <v>9.5468999999999998E-2</v>
       </c>
-      <c r="K14" s="82">
+      <c r="K14" s="81">
         <v>5.0065999999999999E-2</v>
       </c>
-      <c r="L14" s="82">
+      <c r="L14" s="81">
         <v>9.9140000000000006E-2</v>
       </c>
-      <c r="M14" s="82">
+      <c r="M14" s="81">
         <v>0.20558000000000001</v>
       </c>
-      <c r="N14" s="82">
+      <c r="N14" s="81">
         <v>0.67306100000000002</v>
       </c>
-      <c r="O14" s="82">
+      <c r="O14" s="81">
         <v>0.117825</v>
       </c>
-      <c r="P14" s="82">
+      <c r="P14" s="81">
         <v>2.2641000000000001E-2</v>
       </c>
-      <c r="Q14" s="82">
+      <c r="Q14" s="81">
         <v>5.2319999999999997E-3</v>
       </c>
     </row>
@@ -7055,52 +6416,52 @@
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="82">
+      <c r="B15" s="81">
         <v>0.27691300000000002</v>
       </c>
-      <c r="C15" s="82">
+      <c r="C15" s="81">
         <v>0.40850700000000001</v>
       </c>
-      <c r="D15" s="82">
+      <c r="D15" s="81">
         <v>0.36937399999999998</v>
       </c>
-      <c r="E15" s="82">
+      <c r="E15" s="81">
         <v>0.194775</v>
       </c>
-      <c r="F15" s="82">
+      <c r="F15" s="81">
         <v>0.13383900000000001</v>
       </c>
-      <c r="G15" s="82">
+      <c r="G15" s="81">
         <v>0.15487699999999999</v>
       </c>
-      <c r="H15" s="82">
+      <c r="H15" s="81">
         <v>0.26593499999999998</v>
       </c>
-      <c r="I15" s="82">
+      <c r="I15" s="81">
         <v>0.315639</v>
       </c>
-      <c r="J15" s="82">
+      <c r="J15" s="81">
         <v>0.26062400000000002</v>
       </c>
-      <c r="K15" s="82">
+      <c r="K15" s="81">
         <v>8.1602999999999995E-2</v>
       </c>
-      <c r="L15" s="82">
+      <c r="L15" s="81">
         <v>7.9352000000000006E-2</v>
       </c>
-      <c r="M15" s="82">
+      <c r="M15" s="81">
         <v>0.11375300000000001</v>
       </c>
-      <c r="N15" s="82">
+      <c r="N15" s="81">
         <v>0.165434</v>
       </c>
-      <c r="O15" s="82">
+      <c r="O15" s="81">
         <v>0.67988899999999997</v>
       </c>
-      <c r="P15" s="82">
+      <c r="P15" s="81">
         <v>0.102949</v>
       </c>
-      <c r="Q15" s="82">
+      <c r="Q15" s="81">
         <v>1.4578000000000001E-2</v>
       </c>
     </row>
@@ -7108,52 +6469,52 @@
       <c r="A16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="82">
+      <c r="B16" s="81">
         <v>0.124528</v>
       </c>
-      <c r="C16" s="82">
+      <c r="C16" s="81">
         <v>0.37307600000000002</v>
       </c>
-      <c r="D16" s="82">
+      <c r="D16" s="81">
         <v>0.33174900000000002</v>
       </c>
-      <c r="E16" s="82">
+      <c r="E16" s="81">
         <v>0.26471499999999998</v>
       </c>
-      <c r="F16" s="82">
+      <c r="F16" s="81">
         <v>5.3835000000000001E-2</v>
       </c>
-      <c r="G16" s="82">
+      <c r="G16" s="81">
         <v>0.113358</v>
       </c>
-      <c r="H16" s="82">
+      <c r="H16" s="81">
         <v>0.102258</v>
       </c>
-      <c r="I16" s="82">
+      <c r="I16" s="81">
         <v>0.24501899999999999</v>
       </c>
-      <c r="J16" s="82">
+      <c r="J16" s="81">
         <v>0.23438200000000001</v>
       </c>
-      <c r="K16" s="82">
+      <c r="K16" s="81">
         <v>0.18404599999999999</v>
       </c>
-      <c r="L16" s="82">
+      <c r="L16" s="81">
         <v>0.10995099999999999</v>
       </c>
-      <c r="M16" s="82">
+      <c r="M16" s="81">
         <v>5.3179999999999998E-2</v>
       </c>
-      <c r="N16" s="82">
+      <c r="N16" s="81">
         <v>0.104953</v>
       </c>
-      <c r="O16" s="82">
+      <c r="O16" s="81">
         <v>0.15714600000000001</v>
       </c>
-      <c r="P16" s="82">
+      <c r="P16" s="81">
         <v>0.434751</v>
       </c>
-      <c r="Q16" s="82">
+      <c r="Q16" s="81">
         <v>9.6379000000000006E-2</v>
       </c>
     </row>
@@ -7161,52 +6522,52 @@
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="82">
+      <c r="B17" s="81">
         <v>0.223936</v>
       </c>
-      <c r="C17" s="82">
+      <c r="C17" s="81">
         <v>0.29398800000000003</v>
       </c>
-      <c r="D17" s="82">
+      <c r="D17" s="81">
         <v>0.46812700000000002</v>
       </c>
-      <c r="E17" s="82">
+      <c r="E17" s="81">
         <v>0.36628500000000003</v>
       </c>
-      <c r="F17" s="82">
+      <c r="F17" s="81">
         <v>9.4772999999999996E-2</v>
       </c>
-      <c r="G17" s="82">
+      <c r="G17" s="81">
         <v>8.3843000000000001E-2</v>
       </c>
-      <c r="H17" s="82">
+      <c r="H17" s="81">
         <v>0.104393</v>
       </c>
-      <c r="I17" s="82">
+      <c r="I17" s="81">
         <v>0.23522100000000001</v>
       </c>
-      <c r="J17" s="82">
+      <c r="J17" s="81">
         <v>0.28778300000000001</v>
       </c>
-      <c r="K17" s="82">
+      <c r="K17" s="81">
         <v>0.26388600000000001</v>
       </c>
-      <c r="L17" s="82">
+      <c r="L17" s="81">
         <v>0.29662300000000003</v>
       </c>
-      <c r="M17" s="82">
+      <c r="M17" s="81">
         <v>0.126778</v>
       </c>
-      <c r="N17" s="82">
+      <c r="N17" s="81">
         <v>4.9124000000000001E-2</v>
       </c>
-      <c r="O17" s="82">
+      <c r="O17" s="81">
         <v>9.4159999999999994E-2</v>
       </c>
-      <c r="P17" s="82">
+      <c r="P17" s="81">
         <v>0.10020999999999999</v>
       </c>
-      <c r="Q17" s="82">
+      <c r="Q17" s="81">
         <v>0.304143</v>
       </c>
     </row>
@@ -9117,9 +8478,9 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C33" sqref="C33"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -9176,22 +8537,22 @@
       <c r="B2" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="C2" s="79">
-        <v>1</v>
-      </c>
-      <c r="D2" s="79">
+      <c r="C2" s="78">
+        <v>1</v>
+      </c>
+      <c r="D2" s="78">
         <v>4</v>
       </c>
-      <c r="E2" s="79">
-        <v>1</v>
-      </c>
-      <c r="F2" s="79">
-        <v>0</v>
-      </c>
-      <c r="G2" s="79">
+      <c r="E2" s="78">
+        <v>1</v>
+      </c>
+      <c r="F2" s="78">
+        <v>0</v>
+      </c>
+      <c r="G2" s="78">
         <v>110</v>
       </c>
-      <c r="H2" s="79" t="s">
+      <c r="H2" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I2" s="28">
@@ -9211,22 +8572,22 @@
       <c r="B3" s="28" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="79">
-        <v>1</v>
-      </c>
-      <c r="D3" s="79">
+      <c r="C3" s="78">
+        <v>1</v>
+      </c>
+      <c r="D3" s="78">
         <v>21</v>
       </c>
-      <c r="E3" s="28">
-        <v>0.23574999999999999</v>
-      </c>
-      <c r="F3" s="79">
+      <c r="E3" s="44">
+        <v>0.13389041095890411</v>
+      </c>
+      <c r="F3" s="78">
         <v>5</v>
       </c>
-      <c r="G3" s="79">
+      <c r="G3" s="78">
         <v>18</v>
       </c>
-      <c r="H3" s="79" t="s">
+      <c r="H3" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I3" s="28">
@@ -9246,22 +8607,22 @@
       <c r="B4" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="79">
-        <v>1</v>
-      </c>
-      <c r="D4" s="80">
+      <c r="C4" s="78">
+        <v>1</v>
+      </c>
+      <c r="D4" s="79">
         <v>5</v>
       </c>
-      <c r="E4" s="28">
-        <v>0.2137</v>
-      </c>
-      <c r="F4" s="79">
+      <c r="E4" s="44">
+        <v>0.15656</v>
+      </c>
+      <c r="F4" s="78">
         <v>18</v>
       </c>
-      <c r="G4" s="79">
+      <c r="G4" s="78">
         <v>65</v>
       </c>
-      <c r="H4" s="79" t="s">
+      <c r="H4" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I4" s="28">
@@ -9281,14 +8642,14 @@
       <c r="B5" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="C5" s="81">
-        <v>1</v>
-      </c>
-      <c r="D5" s="81">
-        <v>1</v>
-      </c>
-      <c r="E5" s="28">
-        <v>8.6550000000000002E-2</v>
+      <c r="C5" s="80">
+        <v>1</v>
+      </c>
+      <c r="D5" s="80">
+        <v>1</v>
+      </c>
+      <c r="E5" s="44">
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="F5" s="28">
         <v>0</v>
@@ -9296,7 +8657,7 @@
       <c r="G5" s="28">
         <v>110</v>
       </c>
-      <c r="H5" s="79" t="s">
+      <c r="H5" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I5" s="28">
@@ -9316,14 +8677,14 @@
       <c r="B6" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="C6" s="81">
+      <c r="C6" s="80">
         <v>0.11</v>
       </c>
-      <c r="D6" s="81">
-        <v>13</v>
-      </c>
-      <c r="E6" s="28">
-        <v>0.1778875</v>
+      <c r="D6" s="80">
+        <v>10</v>
+      </c>
+      <c r="E6" s="44">
+        <v>2.8493150684931509E-2</v>
       </c>
       <c r="F6" s="28">
         <v>0</v>
@@ -9331,7 +8692,7 @@
       <c r="G6" s="28">
         <v>110</v>
       </c>
-      <c r="H6" s="79" t="s">
+      <c r="H6" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I6" s="28">
@@ -9351,14 +8712,14 @@
       <c r="B7" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="C7" s="81">
-        <v>0.01</v>
-      </c>
-      <c r="D7" s="81">
-        <v>17</v>
-      </c>
-      <c r="E7" s="28">
-        <v>0.33090000000000003</v>
+      <c r="C7" s="80">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="D7" s="80">
+        <v>44</v>
+      </c>
+      <c r="E7" s="44">
+        <v>7.1232876712328766E-2</v>
       </c>
       <c r="F7" s="28">
         <v>18</v>
@@ -9366,7 +8727,7 @@
       <c r="G7" s="28">
         <v>40</v>
       </c>
-      <c r="H7" s="79" t="s">
+      <c r="H7" s="78" t="s">
         <v>182</v>
       </c>
       <c r="I7" s="28">
@@ -9386,14 +8747,14 @@
       <c r="B8" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="C8" s="81">
+      <c r="C8" s="80">
         <v>0.34</v>
       </c>
-      <c r="D8" s="81">
-        <v>23</v>
+      <c r="D8" s="80">
+        <v>20</v>
       </c>
       <c r="E8" s="44">
-        <v>0.2145</v>
+        <v>4.2739726027397257E-2</v>
       </c>
       <c r="F8" s="28">
         <v>4</v>
@@ -9401,7 +8762,7 @@
       <c r="G8" s="28">
         <v>30</v>
       </c>
-      <c r="H8" s="79" t="s">
+      <c r="H8" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I8" s="28">
@@ -9421,14 +8782,14 @@
       <c r="B9" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="81">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="D9" s="81">
+      <c r="C9" s="80">
+        <v>0.2</v>
+      </c>
+      <c r="D9" s="80">
         <v>7</v>
       </c>
       <c r="E9" s="44">
-        <v>4.07E-2</v>
+        <v>3.2876712328767121E-3</v>
       </c>
       <c r="F9" s="28">
         <v>18</v>
@@ -9436,7 +8797,7 @@
       <c r="G9" s="28">
         <v>110</v>
       </c>
-      <c r="H9" s="79" t="s">
+      <c r="H9" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I9" s="28">
@@ -9456,14 +8817,14 @@
       <c r="B10" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C10" s="81">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="D10" s="81">
+      <c r="C10" s="80">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="80">
         <v>17</v>
       </c>
       <c r="E10" s="44">
-        <v>0.17799999999999999</v>
+        <v>1.7534246575342468E-2</v>
       </c>
       <c r="F10" s="28">
         <v>18</v>
@@ -9471,7 +8832,7 @@
       <c r="G10" s="28">
         <v>110</v>
       </c>
-      <c r="H10" s="79" t="s">
+      <c r="H10" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I10" s="28">
@@ -9491,14 +8852,14 @@
       <c r="B11" s="28" t="s">
         <v>270</v>
       </c>
-      <c r="C11" s="81">
-        <v>0.5</v>
-      </c>
-      <c r="D11" s="81">
-        <v>13</v>
+      <c r="C11" s="80">
+        <v>0.6</v>
+      </c>
+      <c r="D11" s="80">
+        <v>12</v>
       </c>
       <c r="E11" s="44">
-        <v>0.17954999999999999</v>
+        <v>4.2739726027397264E-2</v>
       </c>
       <c r="F11" s="28">
         <v>18</v>
@@ -9506,7 +8867,7 @@
       <c r="G11" s="28">
         <v>110</v>
       </c>
-      <c r="H11" s="79" t="s">
+      <c r="H11" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I11" s="28">
@@ -9527,13 +8888,13 @@
         <v>273</v>
       </c>
       <c r="C12" s="28">
-        <v>0.375</v>
-      </c>
-      <c r="D12" s="81">
-        <v>19</v>
+        <v>0.4</v>
+      </c>
+      <c r="D12" s="80">
+        <v>15</v>
       </c>
       <c r="E12" s="44">
-        <v>0.2286</v>
+        <v>4.2739726027397257E-2</v>
       </c>
       <c r="F12" s="28">
         <v>18</v>
@@ -9541,7 +8902,7 @@
       <c r="G12" s="28">
         <v>110</v>
       </c>
-      <c r="H12" s="79" t="s">
+      <c r="H12" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I12" s="28">
@@ -9564,11 +8925,11 @@
       <c r="C13" s="28">
         <v>0.114</v>
       </c>
-      <c r="D13" s="81">
-        <v>62</v>
-      </c>
-      <c r="E13" s="28">
-        <v>0.21740000000000001</v>
+      <c r="D13" s="80">
+        <v>10</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0.17808219178082191</v>
       </c>
       <c r="F13" s="28">
         <v>15</v>
@@ -9576,7 +8937,7 @@
       <c r="G13" s="28">
         <v>110</v>
       </c>
-      <c r="H13" s="79" t="s">
+      <c r="H13" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I13" s="28">
@@ -9599,11 +8960,11 @@
       <c r="C14" s="28">
         <v>5.5E-2</v>
       </c>
-      <c r="D14" s="81">
-        <v>7</v>
+      <c r="D14" s="80">
+        <v>1</v>
       </c>
       <c r="E14" s="44">
-        <v>4.0599999999999997E-2</v>
+        <v>1.2328767123287671E-3</v>
       </c>
       <c r="F14" s="28">
         <v>0</v>
@@ -9611,7 +8972,7 @@
       <c r="G14" s="28">
         <v>110</v>
       </c>
-      <c r="H14" s="79" t="s">
+      <c r="H14" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I14" s="28">
@@ -9632,13 +8993,13 @@
         <v>235</v>
       </c>
       <c r="C15" s="28">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="D15" s="81">
-        <v>7</v>
-      </c>
-      <c r="E15" s="28">
-        <v>4.0599999999999997E-2</v>
+        <v>0.6</v>
+      </c>
+      <c r="D15" s="80">
+        <v>6</v>
+      </c>
+      <c r="E15" s="44">
+        <v>1.0684931506849316E-2</v>
       </c>
       <c r="F15" s="28">
         <v>0</v>
@@ -9646,7 +9007,7 @@
       <c r="G15" s="28">
         <v>110</v>
       </c>
-      <c r="H15" s="79" t="s">
+      <c r="H15" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I15" s="28">
@@ -9669,11 +9030,11 @@
       <c r="C16" s="28">
         <v>0.2</v>
       </c>
-      <c r="D16" s="81">
-        <v>29</v>
-      </c>
-      <c r="E16" s="71">
-        <v>0.18010000000000001</v>
+      <c r="D16" s="80">
+        <v>20</v>
+      </c>
+      <c r="E16" s="44">
+        <v>5.1369863013698627E-3</v>
       </c>
       <c r="F16" s="28">
         <v>0</v>
@@ -9681,7 +9042,7 @@
       <c r="G16" s="28">
         <v>110</v>
       </c>
-      <c r="H16" s="79" t="s">
+      <c r="H16" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I16" s="28">
@@ -9704,11 +9065,11 @@
       <c r="C17" s="28">
         <v>0.54500000000000004</v>
       </c>
-      <c r="D17" s="81">
-        <v>15</v>
-      </c>
-      <c r="E17" s="28">
-        <v>0.18779999999999999</v>
+      <c r="D17" s="80">
+        <v>18</v>
+      </c>
+      <c r="E17" s="44">
+        <v>0.17808219178082191</v>
       </c>
       <c r="F17" s="28">
         <v>1</v>
@@ -9716,7 +9077,7 @@
       <c r="G17" s="28">
         <v>6</v>
       </c>
-      <c r="H17" s="79" t="s">
+      <c r="H17" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I17" s="28">
@@ -9737,13 +9098,13 @@
         <v>268</v>
       </c>
       <c r="C18" s="28">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="D18" s="81">
+        <v>0.6</v>
+      </c>
+      <c r="D18" s="80">
         <v>5</v>
       </c>
       <c r="E18" s="44">
-        <v>0.2306</v>
+        <v>4.9863013698630131E-2</v>
       </c>
       <c r="F18" s="28">
         <v>15</v>
@@ -9751,7 +9112,7 @@
       <c r="G18" s="28">
         <v>110</v>
       </c>
-      <c r="H18" s="79" t="s">
+      <c r="H18" s="78" t="s">
         <v>183</v>
       </c>
       <c r="I18" s="28">
@@ -9774,11 +9135,11 @@
       <c r="C19" s="28">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D19" s="81">
-        <v>15</v>
+      <c r="D19" s="80">
+        <v>14</v>
       </c>
       <c r="E19" s="44">
-        <v>0.79762500000000003</v>
+        <v>0.97024999999999995</v>
       </c>
       <c r="F19" s="28">
         <v>80</v>
@@ -9786,7 +9147,7 @@
       <c r="G19" s="28">
         <v>110</v>
       </c>
-      <c r="H19" s="79" t="s">
+      <c r="H19" s="78" t="s">
         <v>260</v>
       </c>
       <c r="I19" s="28">
@@ -9813,8 +9174,8 @@
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -9835,31 +9196,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="83" t="s">
         <v>258</v>
       </c>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="I1" s="85"/>
+      <c r="J1" s="85"/>
+      <c r="K1" s="85"/>
+      <c r="L1" s="85"/>
+      <c r="M1" s="85"/>
+      <c r="N1" s="85"/>
+      <c r="O1" s="85"/>
+      <c r="P1" s="85"/>
+      <c r="Q1" s="85"/>
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="84"/>
       <c r="V1" s="60"/>
-      <c r="W1" s="84" t="s">
+      <c r="W1" s="83" t="s">
         <v>240</v>
       </c>
-      <c r="X1" s="85"/>
+      <c r="X1" s="84"/>
     </row>
     <row r="2" spans="1:29" s="49" customFormat="1">
       <c r="A2" s="45" t="s">
@@ -10147,7 +9508,7 @@
       <c r="J5" s="37">
         <v>1</v>
       </c>
-      <c r="K5" s="83">
+      <c r="K5" s="82">
         <v>0.1</v>
       </c>
       <c r="L5" s="37">
@@ -10222,8 +9583,8 @@
       <c r="J6" s="37">
         <v>1</v>
       </c>
-      <c r="K6" s="83">
-        <v>0.5</v>
+      <c r="K6" s="82">
+        <v>0.55000000000000004</v>
       </c>
       <c r="L6" s="37">
         <v>1</v>
@@ -10442,8 +9803,8 @@
       <c r="G9" s="37">
         <v>1</v>
       </c>
-      <c r="H9" s="83">
-        <v>0.8</v>
+      <c r="H9" s="82">
+        <v>0.55000000000000004</v>
       </c>
       <c r="I9" s="37">
         <v>1</v>
@@ -10614,8 +9975,8 @@
       <c r="L11" s="37">
         <v>1</v>
       </c>
-      <c r="M11" s="83">
-        <v>0.3</v>
+      <c r="M11" s="82">
+        <v>0.27500000000000002</v>
       </c>
       <c r="N11" s="37">
         <v>1</v>
@@ -10667,8 +10028,8 @@
       <c r="C12" s="53">
         <v>1</v>
       </c>
-      <c r="D12" s="83">
-        <v>1.1000000000000001</v>
+      <c r="D12" s="82">
+        <v>1.0607142857142859</v>
       </c>
       <c r="E12" s="37">
         <v>1</v>
@@ -10774,8 +10135,8 @@
       <c r="M13" s="37">
         <v>1</v>
       </c>
-      <c r="N13" s="83">
-        <v>0.5</v>
+      <c r="N13" s="82">
+        <v>0.4</v>
       </c>
       <c r="O13" s="37">
         <v>1</v>
@@ -10824,8 +10185,8 @@
       <c r="C14" s="53">
         <v>1</v>
       </c>
-      <c r="D14" s="83">
-        <v>1</v>
+      <c r="D14" s="82">
+        <v>1.2</v>
       </c>
       <c r="E14" s="37">
         <v>1</v>
@@ -10833,8 +10194,8 @@
       <c r="F14" s="37">
         <v>1</v>
       </c>
-      <c r="G14" s="83">
-        <v>0.7</v>
+      <c r="G14" s="82">
+        <v>0.1</v>
       </c>
       <c r="H14" s="37">
         <v>1</v>
@@ -10858,13 +10219,13 @@
         <v>1</v>
       </c>
       <c r="O14" s="37">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="P14" s="37">
         <v>0</v>
       </c>
-      <c r="Q14" s="83">
-        <v>0.5</v>
+      <c r="Q14" s="82">
+        <v>0.2</v>
       </c>
       <c r="R14" s="37">
         <v>0</v>
@@ -10872,8 +10233,8 @@
       <c r="S14" s="37">
         <v>1</v>
       </c>
-      <c r="T14" s="83">
-        <v>0.5</v>
+      <c r="T14" s="82">
+        <v>0.3</v>
       </c>
       <c r="U14" s="37">
         <v>1</v>
@@ -10901,8 +10262,8 @@
       <c r="C15" s="53">
         <v>1</v>
       </c>
-      <c r="D15" s="83">
-        <v>1</v>
+      <c r="D15" s="82">
+        <v>1.05</v>
       </c>
       <c r="E15" s="37">
         <v>1</v>
@@ -10910,8 +10271,8 @@
       <c r="F15" s="37">
         <v>1</v>
       </c>
-      <c r="G15" s="83">
-        <v>0.9</v>
+      <c r="G15" s="82">
+        <v>0.5</v>
       </c>
       <c r="H15" s="37">
         <v>1</v>
@@ -10926,7 +10287,7 @@
         <v>1</v>
       </c>
       <c r="L15" s="37">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M15" s="37">
         <v>1</v>
@@ -10934,14 +10295,14 @@
       <c r="N15" s="37">
         <v>1</v>
       </c>
-      <c r="O15" s="83">
-        <v>0.8</v>
+      <c r="O15" s="82">
+        <v>0.7</v>
       </c>
       <c r="P15" s="37">
         <v>1</v>
       </c>
-      <c r="Q15" s="83">
-        <v>0.7</v>
+      <c r="Q15" s="82">
+        <v>0.75</v>
       </c>
       <c r="R15" s="37">
         <v>0</v>
@@ -10976,8 +10337,8 @@
       <c r="C16" s="53">
         <v>1</v>
       </c>
-      <c r="D16" s="83">
-        <v>1</v>
+      <c r="D16" s="82">
+        <v>1.0249999999999999</v>
       </c>
       <c r="E16" s="37">
         <v>1</v>
@@ -10985,8 +10346,8 @@
       <c r="F16" s="37">
         <v>1</v>
       </c>
-      <c r="G16" s="83">
-        <v>1</v>
+      <c r="G16" s="82">
+        <v>0.98</v>
       </c>
       <c r="H16" s="37">
         <v>1</v>
@@ -11000,8 +10361,8 @@
       <c r="K16" s="37">
         <v>1</v>
       </c>
-      <c r="L16" s="83">
-        <v>0.95</v>
+      <c r="L16" s="82">
+        <v>0.5</v>
       </c>
       <c r="M16" s="37">
         <v>1</v>
@@ -11009,7 +10370,7 @@
       <c r="N16" s="37">
         <v>1</v>
       </c>
-      <c r="O16" s="83">
+      <c r="O16" s="82">
         <v>0.95</v>
       </c>
       <c r="P16" s="37">
@@ -11071,7 +10432,7 @@
       <c r="H17" s="37">
         <v>1</v>
       </c>
-      <c r="I17" s="83">
+      <c r="I17" s="82">
         <v>0</v>
       </c>
       <c r="J17" s="37">
@@ -11142,7 +10503,7 @@
       <c r="F18" s="37">
         <v>1</v>
       </c>
-      <c r="G18" s="83">
+      <c r="G18" s="82">
         <v>0.8</v>
       </c>
       <c r="H18" s="37">
@@ -11151,7 +10512,7 @@
       <c r="I18" s="37">
         <v>1</v>
       </c>
-      <c r="J18" s="83">
+      <c r="J18" s="82">
         <v>0</v>
       </c>
       <c r="K18" s="37">
@@ -11295,7 +10656,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="37">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="H20" s="37">
         <v>1</v>
@@ -11367,7 +10728,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="53">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E21" s="37">
         <v>1</v>
@@ -11375,8 +10736,8 @@
       <c r="F21" s="37">
         <v>1</v>
       </c>
-      <c r="G21" s="83">
-        <v>0.9</v>
+      <c r="G21" s="82">
+        <v>0.4</v>
       </c>
       <c r="H21" s="37">
         <v>1</v>
@@ -11448,7 +10809,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="53">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E22" s="37">
         <v>1</v>
@@ -11471,7 +10832,7 @@
       <c r="K22" s="37">
         <v>1</v>
       </c>
-      <c r="L22" s="83">
+      <c r="L22" s="82">
         <v>0</v>
       </c>
       <c r="M22" s="37">
@@ -11525,7 +10886,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="53">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E23" s="37">
         <v>1</v>
@@ -11602,7 +10963,7 @@
         <v>1</v>
       </c>
       <c r="D24" s="53">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E24" s="37">
         <v>1</v>
@@ -11899,7 +11260,7 @@
       </c>
       <c r="W27" s="58"/>
       <c r="X27" s="34"/>
-      <c r="Y27" s="72">
+      <c r="Y27" s="71">
         <v>43919</v>
       </c>
       <c r="Z27" s="31"/>
@@ -11911,7 +11272,7 @@
       <c r="A28" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="73" t="s">
         <v>301</v>
       </c>
       <c r="C28" s="52">
@@ -12051,7 +11412,7 @@
       </c>
       <c r="W29" s="58"/>
       <c r="X29" s="34"/>
-      <c r="Y29" s="72">
+      <c r="Y29" s="71">
         <v>43919</v>
       </c>
       <c r="Z29" s="36"/>
@@ -12660,7 +12021,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -12696,7 +12057,7 @@
         <v>196</v>
       </c>
       <c r="B3" s="23">
-        <v>44044</v>
+        <v>44075</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>198</v>
@@ -12875,7 +12236,7 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="74" t="s">
         <v>13</v>
       </c>
       <c r="B2">
@@ -12884,13 +12245,13 @@
       <c r="C2">
         <v>82289</v>
       </c>
-      <c r="D2" s="76">
+      <c r="D2" s="75">
         <f>B2/C2</f>
         <v>0.22103804882791139</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="74" t="s">
         <v>14</v>
       </c>
       <c r="B3">
@@ -12899,13 +12260,13 @@
       <c r="C3">
         <v>395365</v>
       </c>
-      <c r="D3" s="76">
+      <c r="D3" s="75">
         <f t="shared" ref="D3:D7" si="0">B3/C3</f>
         <v>0.56577086995561066</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="74" t="s">
         <v>15</v>
       </c>
       <c r="B4">
@@ -12914,13 +12275,13 @@
       <c r="C4">
         <v>363542</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="75">
         <f t="shared" si="0"/>
         <v>0.67502241831755339</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="74" t="s">
         <v>16</v>
       </c>
       <c r="B5">
@@ -12929,13 +12290,13 @@
       <c r="C5">
         <v>374094</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="75">
         <f t="shared" si="0"/>
         <v>0.32347484856747233</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="74" t="s">
         <v>17</v>
       </c>
       <c r="B6">
@@ -12944,13 +12305,13 @@
       <c r="C6">
         <v>466003</v>
       </c>
-      <c r="D6" s="76">
+      <c r="D6" s="75">
         <f t="shared" si="0"/>
         <v>0.15124580743042426</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="74" t="s">
         <v>18</v>
       </c>
       <c r="B7">
@@ -12959,16 +12320,16 @@
       <c r="C7">
         <v>500215</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="75">
         <f t="shared" si="0"/>
         <v>0.10410123646831862</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="C8" s="77" t="s">
+      <c r="C8" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="77">
         <f>SUM(B2:B7)/SUM(C2:C7)</f>
         <v>0.33501504463884618</v>
       </c>

</xml_diff>

<commit_message>
Read in policies from book
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwork/Documents/GitHub/covasim-australia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A66B23-4698-0747-9842-4A58F5E61398}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001AFDD4-C31F-FC49-BFF1-99096789486D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact matrices-home" sheetId="2" r:id="rId1"/>
@@ -18,8 +18,9 @@
     <sheet name="households" sheetId="4" r:id="rId3"/>
     <sheet name="layers" sheetId="5" r:id="rId4"/>
     <sheet name="policies" sheetId="7" r:id="rId5"/>
-    <sheet name="other_par" sheetId="6" r:id="rId6"/>
-    <sheet name="data" sheetId="8" r:id="rId7"/>
+    <sheet name="policies-lockdown" sheetId="10" r:id="rId6"/>
+    <sheet name="other_par" sheetId="6" r:id="rId7"/>
+    <sheet name="data" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -838,7 +839,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -847,12 +848,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-These are relative changes, so 0.8 means 20% reduction due to the policy change</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>These are relative changes, so 0.8 means 20% reduction due to the policy change</t>
         </r>
       </text>
     </comment>
@@ -862,7 +872,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -871,12 +881,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Any overall change in transmission risk per contact (e.g. reduction from generall better hand washing)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any overall change in transmission risk per contact (e.g. reduction from generall better hand washing)</t>
         </r>
       </text>
     </comment>
@@ -910,7 +929,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -919,12 +938,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assumed daily number of infections imported per day, from other states or internationally</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assumed daily number of infections imported per day, from other states or internationally</t>
         </r>
       </text>
     </comment>
@@ -934,7 +962,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -943,12 +971,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-remove this percentage of contacts from the network layer</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>remove this percentage of contacts from the network layer</t>
         </r>
       </text>
     </comment>
@@ -958,7 +995,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -967,12 +1004,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Proportion of people unaffected - the remainder are removed from the network layer</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Proportion of people unaffected - the remainder are removed from the network layer</t>
         </r>
       </text>
     </comment>
@@ -982,7 +1028,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -991,13 +1037,41 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-From flutracker, 0.2% fever and cough prevalence compared to ~1.4% the same time last yer --&gt; 86% reduction 
-https://info.flutracking.net/reports-2/australia-reports/</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">From flutracker, 0.2% fever and cough prevalence compared to ~1.4% the same time last yer --&gt; 86% reduction 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>https://info.flutracking.net/reports-2/australia-reports/</t>
         </r>
       </text>
     </comment>
@@ -1007,7 +1081,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1016,12 +1090,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-E.g. 0.1 here means that 90% of children are removed from the school netowrk layer</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>E.g. 0.1 here means that 90% of children are removed from the school netowrk layer</t>
         </r>
       </text>
     </comment>
@@ -1131,6 +1214,205 @@
     <author>Nick Scott</author>
   </authors>
   <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3C870F46-9F50-5C4A-9E46-40642E805023}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>These are relative changes, so 0.8 means 20% reduction due to the policy change</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{19273178-DC1F-9742-AC05-0E232D76FA02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any overall change in transmission risk per contact (e.g. reduction from generall better hand washing)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{6B4AC3B5-CA50-AC4B-90E6-F104AE39D6CA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Each row is the change in the risk of transmission on the associated network, relative to pre-COVID. 0 means that there is no risk, 1 means that the risk is the same as pre-any intervention.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{3CA18A6A-8ACE-D845-B9E6-D16E193EE499}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assumed daily number of infections imported per day, from other states or internationally</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{43CA845B-84F7-D141-A4C2-40CB783920BF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>remove this percentage of contacts from the network layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{0BFBE1CD-EA75-8C40-9504-584095318FA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Proportion of people unaffected - the remainder are removed from the network layer</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nick Scott</author>
+  </authors>
+  <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{31C3822A-7583-49A7-A327-50B1E0C442BF}">
       <text>
         <r>
@@ -1160,7 +1442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="299">
   <si>
     <t>age</t>
   </si>
@@ -2042,6 +2324,21 @@
   </si>
   <si>
     <t>iso_factor</t>
+  </si>
+  <si>
+    <t>lockdown</t>
+  </si>
+  <si>
+    <t>Broad term for firm state-wide shutdown</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2349,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2303,6 +2600,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -2521,7 +2831,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -2711,6 +3021,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2769,7 +3103,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2947,6 +3281,30 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="47">
@@ -3561,6 +3919,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFC63500"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3570,6 +3933,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3871,7 +4238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71292FC5-4B23-A74E-B513-C8525EFF9EE0}">
   <dimension ref="A1:R17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7445,12 +7812,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84637A79-E027-48E7-B7DE-002E7C836FC2}">
   <sheetPr>
-    <tabColor rgb="FF00B050"/>
+    <tabColor rgb="FFC63500"/>
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:XFD12"/>
+    <sheetView topLeftCell="D1" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9885,12 +10252,12 @@
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="D1:U1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C3:P11 C12:C13 C14:P18 C20:P22 D23 C24:P24">
+  <conditionalFormatting sqref="C14:P18 C20:P22 D23 C24:P24 C3:P11 C12:C13">
     <cfRule type="cellIs" dxfId="79" priority="80" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:P11 C12:C13 C14:P18 C20:P22 D23 C24:P26">
+  <conditionalFormatting sqref="C14:P18 C20:P22 D23 C24:P26 C3:P11 C12:C13">
     <cfRule type="cellIs" dxfId="78" priority="79" operator="notEqual">
       <formula>1</formula>
     </cfRule>
@@ -10292,6 +10659,238 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288C3D6A-28F1-7940-82D1-054C6895C15C}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="84"/>
+    <col min="21" max="21" width="10.83203125" style="80"/>
+    <col min="22" max="22" width="10.83203125" style="84"/>
+    <col min="24" max="24" width="10.83203125" style="80"/>
+    <col min="26" max="26" width="10.83203125" style="80"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="77" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="82"/>
+      <c r="W1" s="77" t="s">
+        <v>228</v>
+      </c>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="85"/>
+      <c r="Z1" s="87"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+    </row>
+    <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="42" t="str">
+        <f ca="1">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
+        <v>H</v>
+      </c>
+      <c r="E2" s="42" t="str">
+        <f t="shared" ref="E2:U2" ca="1" si="0">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
+        <v>S</v>
+      </c>
+      <c r="F2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>W</v>
+      </c>
+      <c r="G2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="H2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Church</v>
+      </c>
+      <c r="I2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>pSport</v>
+      </c>
+      <c r="J2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>cSport</v>
+      </c>
+      <c r="K2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>beach</v>
+      </c>
+      <c r="L2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>entertainment</v>
+      </c>
+      <c r="M2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>cafe_restaurant</v>
+      </c>
+      <c r="N2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>pub_bar</v>
+      </c>
+      <c r="O2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>transport</v>
+      </c>
+      <c r="P2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>national_parks</v>
+      </c>
+      <c r="Q2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>public_parks</v>
+      </c>
+      <c r="R2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>large_events</v>
+      </c>
+      <c r="S2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>child_care</v>
+      </c>
+      <c r="T2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>social</v>
+      </c>
+      <c r="U2" s="81" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>aged_care</v>
+      </c>
+      <c r="V2" s="83" t="s">
+        <v>229</v>
+      </c>
+      <c r="W2" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="X2" s="86" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y2" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z2" s="81" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="84">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="84">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="W1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -10486,7 +11085,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3870F7-A576-4BD3-9D23-1C9E10583711}">
   <dimension ref="A1:D8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added back sheet to check old code (marked in red)
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwork/Documents/GitHub/covasim-australia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001AFDD4-C31F-FC49-BFF1-99096789486D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83EF8E0-5766-3D41-A473-D172BDC28CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-6640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="762" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact matrices-home" sheetId="2" r:id="rId1"/>
     <sheet name="age_sex" sheetId="3" r:id="rId2"/>
     <sheet name="households" sheetId="4" r:id="rId3"/>
     <sheet name="layers" sheetId="5" r:id="rId4"/>
-    <sheet name="policies" sheetId="7" r:id="rId5"/>
-    <sheet name="policies-lockdown" sheetId="10" r:id="rId6"/>
-    <sheet name="other_par" sheetId="6" r:id="rId7"/>
-    <sheet name="data" sheetId="8" r:id="rId8"/>
+    <sheet name="policies-lockdown" sheetId="10" r:id="rId5"/>
+    <sheet name="other_par" sheetId="6" r:id="rId6"/>
+    <sheet name="epi_data" sheetId="11" r:id="rId7"/>
+    <sheet name="policies" sheetId="7" r:id="rId8"/>
+    <sheet name="data" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -97,7 +98,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -106,12 +107,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Relative risk of infection compared to a household contatct (note: this is not the absolute risk per contact)</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Relative risk of infection compared to a household contatct (note: this is not the absolute risk per contact)</t>
         </r>
       </text>
     </comment>
@@ -534,7 +544,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -543,12 +553,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assuming a sport contact is equal to a house contact, but only occurs once per week so divide by 7</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assuming a sport contact is equal to a house contact, but only occurs once per week so divide by 7</t>
         </r>
       </text>
     </comment>
@@ -828,6 +847,205 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Nick Scott</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3C870F46-9F50-5C4A-9E46-40642E805023}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>These are relative changes, so 0.8 means 20% reduction due to the policy change</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{19273178-DC1F-9742-AC05-0E232D76FA02}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any overall change in transmission risk per contact (e.g. reduction from generall better hand washing)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{6B4AC3B5-CA50-AC4B-90E6-F104AE39D6CA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Each row is the change in the risk of transmission on the associated network, relative to pre-COVID. 0 means that there is no risk, 1 means that the risk is the same as pre-any intervention.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{3CA18A6A-8ACE-D845-B9E6-D16E193EE499}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assumed daily number of infections imported per day, from other states or internationally</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{43CA845B-84F7-D141-A4C2-40CB783920BF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>remove this percentage of contacts from the network layer</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{0BFBE1CD-EA75-8C40-9504-584095318FA7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nick Scott:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Proportion of people unaffected - the remainder are removed from the network layer</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nick Scott</author>
@@ -1208,205 +1426,6 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Nick Scott</author>
-  </authors>
-  <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{3C870F46-9F50-5C4A-9E46-40642E805023}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>These are relative changes, so 0.8 means 20% reduction due to the policy change</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{19273178-DC1F-9742-AC05-0E232D76FA02}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Any overall change in transmission risk per contact (e.g. reduction from generall better hand washing)</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{6B4AC3B5-CA50-AC4B-90E6-F104AE39D6CA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Each row is the change in the risk of transmission on the associated network, relative to pre-COVID. 0 means that there is no risk, 1 means that the risk is the same as pre-any intervention.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{3CA18A6A-8ACE-D845-B9E6-D16E193EE499}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assumed daily number of infections imported per day, from other states or internationally</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{43CA845B-84F7-D141-A4C2-40CB783920BF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>remove this percentage of contacts from the network layer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{0BFBE1CD-EA75-8C40-9504-584095318FA7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nick Scott:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Proportion of people unaffected - the remainder are removed from the network layer</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
@@ -1442,7 +1461,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="311">
   <si>
     <t>age</t>
   </si>
@@ -2339,6 +2358,42 @@
   </si>
   <si>
     <t>end_date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>cum_infections</t>
+  </si>
+  <si>
+    <t>cum_deaths</t>
+  </si>
+  <si>
+    <t>cum_test</t>
+  </si>
+  <si>
+    <t>cum_neg</t>
+  </si>
+  <si>
+    <t>n_severe</t>
+  </si>
+  <si>
+    <t>n_critical</t>
+  </si>
+  <si>
+    <t>cum_recovered</t>
+  </si>
+  <si>
+    <t>new_diagnoses</t>
+  </si>
+  <si>
+    <t>new_deaths</t>
+  </si>
+  <si>
+    <t>new_tests</t>
+  </si>
+  <si>
+    <t>daily_imported_cases</t>
   </si>
 </sst>
 </file>
@@ -2349,7 +2404,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="39" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2613,8 +2668,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2828,6 +2898,18 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -3103,7 +3185,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3273,15 +3355,6 @@
     <xf numFmtId="2" fontId="31" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3306,6 +3379,19 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="38" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3935,10 +4021,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7810,14 +7892,2257 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288C3D6A-28F1-7940-82D1-054C6895C15C}">
+  <dimension ref="A1:AC3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="81"/>
+    <col min="21" max="21" width="10.83203125" style="77"/>
+    <col min="22" max="22" width="10.83203125" style="81"/>
+    <col min="24" max="24" width="10.83203125" style="77"/>
+    <col min="26" max="26" width="10.83203125" style="77"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" s="25"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="87" t="s">
+        <v>246</v>
+      </c>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="88"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="87" t="s">
+        <v>228</v>
+      </c>
+      <c r="X1" s="88"/>
+      <c r="Y1" s="82"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="24"/>
+      <c r="AB1" s="25"/>
+      <c r="AC1" s="25"/>
+    </row>
+    <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="42" t="str">
+        <f ca="1">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
+        <v>H</v>
+      </c>
+      <c r="E2" s="42" t="str">
+        <f t="shared" ref="E2:U2" ca="1" si="0">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
+        <v>S</v>
+      </c>
+      <c r="F2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>W</v>
+      </c>
+      <c r="G2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>C</v>
+      </c>
+      <c r="H2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Church</v>
+      </c>
+      <c r="I2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>pSport</v>
+      </c>
+      <c r="J2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>cSport</v>
+      </c>
+      <c r="K2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>beach</v>
+      </c>
+      <c r="L2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>entertainment</v>
+      </c>
+      <c r="M2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>cafe_restaurant</v>
+      </c>
+      <c r="N2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>pub_bar</v>
+      </c>
+      <c r="O2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>transport</v>
+      </c>
+      <c r="P2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>national_parks</v>
+      </c>
+      <c r="Q2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>public_parks</v>
+      </c>
+      <c r="R2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>large_events</v>
+      </c>
+      <c r="S2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>child_care</v>
+      </c>
+      <c r="T2" s="42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>social</v>
+      </c>
+      <c r="U2" s="78" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>aged_care</v>
+      </c>
+      <c r="V2" s="80" t="s">
+        <v>229</v>
+      </c>
+      <c r="W2" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="X2" s="83" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y2" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z2" s="78" t="s">
+        <v>298</v>
+      </c>
+      <c r="AA2" s="41"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C3" s="81">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3">
+        <v>1</v>
+      </c>
+      <c r="V3" s="81">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D1:U1"/>
+    <mergeCell ref="W1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="51.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="18">
+        <v>43891</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="18">
+        <v>44075</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B5">
+        <v>20000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6">
+        <f>6200000/B5</f>
+        <v>310</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8">
+        <v>0.2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>188</v>
+      </c>
+      <c r="B11">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12">
+        <v>0.6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>283</v>
+      </c>
+      <c r="B16">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>284</v>
+      </c>
+      <c r="B17">
+        <v>2000</v>
+      </c>
+      <c r="C17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3091FBE5-3E95-934F-B436-B236BC518E77}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:L53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="90" t="s">
+        <v>299</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>301</v>
+      </c>
+      <c r="D1" s="90" t="s">
+        <v>302</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>303</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>304</v>
+      </c>
+      <c r="G1" s="90" t="s">
+        <v>305</v>
+      </c>
+      <c r="H1" s="90" t="s">
+        <v>306</v>
+      </c>
+      <c r="I1" s="90" t="s">
+        <v>307</v>
+      </c>
+      <c r="J1" s="90" t="s">
+        <v>308</v>
+      </c>
+      <c r="K1" s="90" t="s">
+        <v>309</v>
+      </c>
+      <c r="L1" s="90" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="91">
+        <v>43891</v>
+      </c>
+      <c r="B2" s="92">
+        <v>9</v>
+      </c>
+      <c r="C2" s="92">
+        <v>0</v>
+      </c>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92">
+        <v>2</v>
+      </c>
+      <c r="J2" s="92">
+        <v>0</v>
+      </c>
+      <c r="K2" s="92">
+        <v>0</v>
+      </c>
+      <c r="L2" s="92">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="91">
+        <v>43892</v>
+      </c>
+      <c r="B3" s="92">
+        <v>9</v>
+      </c>
+      <c r="C3" s="92">
+        <v>0</v>
+      </c>
+      <c r="D3" s="92"/>
+      <c r="E3" s="92"/>
+      <c r="F3" s="92"/>
+      <c r="G3" s="92"/>
+      <c r="H3" s="92"/>
+      <c r="I3" s="92">
+        <v>0</v>
+      </c>
+      <c r="J3" s="92">
+        <v>0</v>
+      </c>
+      <c r="K3" s="92">
+        <v>0</v>
+      </c>
+      <c r="L3" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="91">
+        <v>43893</v>
+      </c>
+      <c r="B4" s="92">
+        <v>9</v>
+      </c>
+      <c r="C4" s="92">
+        <v>0</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92">
+        <v>0</v>
+      </c>
+      <c r="J4" s="92">
+        <v>0</v>
+      </c>
+      <c r="K4" s="92">
+        <v>0</v>
+      </c>
+      <c r="L4" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="91">
+        <v>43894</v>
+      </c>
+      <c r="B5" s="92">
+        <v>10</v>
+      </c>
+      <c r="C5" s="92">
+        <v>0</v>
+      </c>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92">
+        <v>1</v>
+      </c>
+      <c r="J5" s="92">
+        <v>0</v>
+      </c>
+      <c r="K5" s="92">
+        <v>0</v>
+      </c>
+      <c r="L5" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="91">
+        <v>43895</v>
+      </c>
+      <c r="B6" s="92">
+        <v>10</v>
+      </c>
+      <c r="C6" s="92">
+        <v>0</v>
+      </c>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92">
+        <v>0</v>
+      </c>
+      <c r="J6" s="92">
+        <v>0</v>
+      </c>
+      <c r="K6" s="92">
+        <v>0</v>
+      </c>
+      <c r="L6" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="91">
+        <v>43896</v>
+      </c>
+      <c r="B7" s="92">
+        <v>10</v>
+      </c>
+      <c r="C7" s="92">
+        <v>0</v>
+      </c>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="92">
+        <v>0</v>
+      </c>
+      <c r="J7" s="92">
+        <v>0</v>
+      </c>
+      <c r="K7" s="92">
+        <v>0</v>
+      </c>
+      <c r="L7" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="91">
+        <v>43897</v>
+      </c>
+      <c r="B8" s="92">
+        <v>11</v>
+      </c>
+      <c r="C8" s="92">
+        <v>0</v>
+      </c>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92">
+        <v>1</v>
+      </c>
+      <c r="J8" s="92">
+        <v>0</v>
+      </c>
+      <c r="K8" s="92">
+        <v>0</v>
+      </c>
+      <c r="L8" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="91">
+        <v>43898</v>
+      </c>
+      <c r="B9" s="92">
+        <v>12</v>
+      </c>
+      <c r="C9" s="92">
+        <v>0</v>
+      </c>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="92">
+        <v>1</v>
+      </c>
+      <c r="J9" s="92">
+        <v>0</v>
+      </c>
+      <c r="K9" s="92">
+        <v>0</v>
+      </c>
+      <c r="L9" s="92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="91">
+        <v>43899</v>
+      </c>
+      <c r="B10" s="92">
+        <v>15</v>
+      </c>
+      <c r="C10" s="92">
+        <v>0</v>
+      </c>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="92">
+        <v>3</v>
+      </c>
+      <c r="J10" s="92">
+        <v>0</v>
+      </c>
+      <c r="K10" s="92">
+        <v>0</v>
+      </c>
+      <c r="L10" s="92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="91">
+        <v>43900</v>
+      </c>
+      <c r="B11" s="92">
+        <v>18</v>
+      </c>
+      <c r="C11" s="92">
+        <v>0</v>
+      </c>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92">
+        <v>3</v>
+      </c>
+      <c r="J11" s="92">
+        <v>0</v>
+      </c>
+      <c r="K11" s="92">
+        <v>0</v>
+      </c>
+      <c r="L11" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="91">
+        <v>43901</v>
+      </c>
+      <c r="B12" s="92">
+        <v>21</v>
+      </c>
+      <c r="C12" s="92">
+        <v>0</v>
+      </c>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92">
+        <v>3</v>
+      </c>
+      <c r="J12" s="92">
+        <v>0</v>
+      </c>
+      <c r="K12" s="92">
+        <v>0</v>
+      </c>
+      <c r="L12" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="91">
+        <v>43902</v>
+      </c>
+      <c r="B13" s="92">
+        <v>27</v>
+      </c>
+      <c r="C13" s="92">
+        <v>0</v>
+      </c>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92">
+        <v>6</v>
+      </c>
+      <c r="J13" s="92">
+        <v>0</v>
+      </c>
+      <c r="K13" s="92">
+        <v>0</v>
+      </c>
+      <c r="L13" s="92">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="91">
+        <v>43903</v>
+      </c>
+      <c r="B14" s="92">
+        <v>36</v>
+      </c>
+      <c r="C14" s="92">
+        <v>0</v>
+      </c>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92">
+        <v>9</v>
+      </c>
+      <c r="J14" s="92">
+        <v>0</v>
+      </c>
+      <c r="K14" s="93">
+        <v>500</v>
+      </c>
+      <c r="L14" s="92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="91">
+        <v>43904</v>
+      </c>
+      <c r="B15" s="92">
+        <v>49</v>
+      </c>
+      <c r="C15" s="92">
+        <v>0</v>
+      </c>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="92"/>
+      <c r="I15" s="92">
+        <v>13</v>
+      </c>
+      <c r="J15" s="92">
+        <v>0</v>
+      </c>
+      <c r="K15" s="93">
+        <v>500</v>
+      </c>
+      <c r="L15" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="91">
+        <v>43905</v>
+      </c>
+      <c r="B16" s="92">
+        <v>57</v>
+      </c>
+      <c r="C16" s="92">
+        <v>0</v>
+      </c>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="92"/>
+      <c r="I16" s="92">
+        <v>8</v>
+      </c>
+      <c r="J16" s="92">
+        <v>0</v>
+      </c>
+      <c r="K16" s="93">
+        <v>500</v>
+      </c>
+      <c r="L16" s="92">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" s="91">
+        <v>43906</v>
+      </c>
+      <c r="B17" s="92">
+        <v>71</v>
+      </c>
+      <c r="C17" s="92">
+        <v>0</v>
+      </c>
+      <c r="D17" s="92">
+        <v>11700</v>
+      </c>
+      <c r="E17" s="92">
+        <v>11629</v>
+      </c>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92">
+        <v>14</v>
+      </c>
+      <c r="J17" s="92">
+        <v>0</v>
+      </c>
+      <c r="K17" s="93">
+        <v>500</v>
+      </c>
+      <c r="L17" s="92">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" s="91">
+        <v>43907</v>
+      </c>
+      <c r="B18" s="92">
+        <v>94</v>
+      </c>
+      <c r="C18" s="92">
+        <v>0</v>
+      </c>
+      <c r="D18" s="92">
+        <v>14200</v>
+      </c>
+      <c r="E18" s="92">
+        <v>14106</v>
+      </c>
+      <c r="F18" s="92"/>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92">
+        <v>23</v>
+      </c>
+      <c r="J18" s="92">
+        <v>0</v>
+      </c>
+      <c r="K18" s="93">
+        <v>1000</v>
+      </c>
+      <c r="L18" s="92">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" s="91">
+        <v>43908</v>
+      </c>
+      <c r="B19" s="92">
+        <v>121</v>
+      </c>
+      <c r="C19" s="92">
+        <v>0</v>
+      </c>
+      <c r="D19" s="92">
+        <v>15200</v>
+      </c>
+      <c r="E19" s="92">
+        <v>15079</v>
+      </c>
+      <c r="F19" s="92"/>
+      <c r="G19" s="92"/>
+      <c r="H19" s="92"/>
+      <c r="I19" s="92">
+        <v>27</v>
+      </c>
+      <c r="J19" s="92">
+        <v>0</v>
+      </c>
+      <c r="K19" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L19" s="92">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="91">
+        <v>43909</v>
+      </c>
+      <c r="B20" s="92">
+        <v>150</v>
+      </c>
+      <c r="C20" s="92">
+        <v>0</v>
+      </c>
+      <c r="D20" s="92">
+        <v>17180</v>
+      </c>
+      <c r="E20" s="92">
+        <v>17030</v>
+      </c>
+      <c r="F20" s="92"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="92"/>
+      <c r="I20" s="92">
+        <v>29</v>
+      </c>
+      <c r="J20" s="92">
+        <v>0</v>
+      </c>
+      <c r="K20" s="92">
+        <v>1980</v>
+      </c>
+      <c r="L20" s="92">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="91">
+        <v>43910</v>
+      </c>
+      <c r="B21" s="92">
+        <v>178</v>
+      </c>
+      <c r="C21" s="92">
+        <v>0</v>
+      </c>
+      <c r="D21" s="92">
+        <v>19337</v>
+      </c>
+      <c r="E21" s="92">
+        <v>19159</v>
+      </c>
+      <c r="F21" s="92"/>
+      <c r="G21" s="92"/>
+      <c r="H21" s="92"/>
+      <c r="I21" s="92">
+        <v>28</v>
+      </c>
+      <c r="J21" s="92">
+        <v>0</v>
+      </c>
+      <c r="K21" s="92">
+        <v>2157</v>
+      </c>
+      <c r="L21" s="92">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="91">
+        <v>43911</v>
+      </c>
+      <c r="B22" s="92">
+        <v>229</v>
+      </c>
+      <c r="C22" s="92">
+        <v>0</v>
+      </c>
+      <c r="D22" s="92">
+        <v>20500</v>
+      </c>
+      <c r="E22" s="92">
+        <v>20271</v>
+      </c>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92">
+        <v>51</v>
+      </c>
+      <c r="J22" s="92">
+        <v>0</v>
+      </c>
+      <c r="K22" s="92">
+        <v>1163</v>
+      </c>
+      <c r="L22" s="92">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="91">
+        <v>43912</v>
+      </c>
+      <c r="B23" s="92">
+        <v>296</v>
+      </c>
+      <c r="C23" s="92">
+        <v>0</v>
+      </c>
+      <c r="D23" s="92">
+        <v>22900</v>
+      </c>
+      <c r="E23" s="92">
+        <v>22604</v>
+      </c>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92">
+        <v>67</v>
+      </c>
+      <c r="J23" s="92">
+        <v>0</v>
+      </c>
+      <c r="K23" s="92">
+        <v>2400</v>
+      </c>
+      <c r="L23" s="92">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" s="91">
+        <v>43913</v>
+      </c>
+      <c r="B24" s="92">
+        <v>355</v>
+      </c>
+      <c r="C24" s="92">
+        <v>0</v>
+      </c>
+      <c r="D24" s="92">
+        <v>23700</v>
+      </c>
+      <c r="E24" s="92">
+        <v>23345</v>
+      </c>
+      <c r="F24" s="92">
+        <v>6</v>
+      </c>
+      <c r="G24" s="92"/>
+      <c r="H24" s="92">
+        <v>96</v>
+      </c>
+      <c r="I24" s="92">
+        <v>59</v>
+      </c>
+      <c r="J24" s="92">
+        <v>0</v>
+      </c>
+      <c r="K24" s="92">
+        <v>800</v>
+      </c>
+      <c r="L24" s="92">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="91">
+        <v>43914</v>
+      </c>
+      <c r="B25" s="92">
+        <v>411</v>
+      </c>
+      <c r="C25" s="92">
+        <v>0</v>
+      </c>
+      <c r="D25" s="92">
+        <v>25000</v>
+      </c>
+      <c r="E25" s="92">
+        <v>24589</v>
+      </c>
+      <c r="F25" s="92"/>
+      <c r="G25" s="92"/>
+      <c r="H25" s="92">
+        <v>113</v>
+      </c>
+      <c r="I25" s="92">
+        <v>56</v>
+      </c>
+      <c r="J25" s="92">
+        <v>0</v>
+      </c>
+      <c r="K25" s="92">
+        <v>1300</v>
+      </c>
+      <c r="L25" s="92">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="91">
+        <v>43915</v>
+      </c>
+      <c r="B26" s="92">
+        <v>466</v>
+      </c>
+      <c r="C26" s="92">
+        <v>0</v>
+      </c>
+      <c r="D26" s="92">
+        <v>25500</v>
+      </c>
+      <c r="E26" s="92">
+        <v>25034</v>
+      </c>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92">
+        <v>128</v>
+      </c>
+      <c r="I26" s="92">
+        <v>55</v>
+      </c>
+      <c r="J26" s="92">
+        <v>0</v>
+      </c>
+      <c r="K26" s="92">
+        <v>500</v>
+      </c>
+      <c r="L26" s="92">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="91">
+        <v>43916</v>
+      </c>
+      <c r="B27" s="92">
+        <v>520</v>
+      </c>
+      <c r="C27" s="92">
+        <v>2</v>
+      </c>
+      <c r="D27" s="92">
+        <v>26900</v>
+      </c>
+      <c r="E27" s="92">
+        <v>26380</v>
+      </c>
+      <c r="F27" s="92"/>
+      <c r="G27" s="92"/>
+      <c r="H27" s="92">
+        <v>149</v>
+      </c>
+      <c r="I27" s="92">
+        <v>54</v>
+      </c>
+      <c r="J27" s="92">
+        <v>2</v>
+      </c>
+      <c r="K27" s="92">
+        <v>1400</v>
+      </c>
+      <c r="L27" s="92">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28" s="91">
+        <v>43917</v>
+      </c>
+      <c r="B28" s="92">
+        <v>574</v>
+      </c>
+      <c r="C28" s="92">
+        <v>3</v>
+      </c>
+      <c r="D28" s="92">
+        <v>27800</v>
+      </c>
+      <c r="E28" s="92">
+        <v>27226</v>
+      </c>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92">
+        <v>172</v>
+      </c>
+      <c r="I28" s="92">
+        <v>54</v>
+      </c>
+      <c r="J28" s="92">
+        <v>1</v>
+      </c>
+      <c r="K28" s="92">
+        <v>900</v>
+      </c>
+      <c r="L28" s="92">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29" s="91">
+        <v>43918</v>
+      </c>
+      <c r="B29" s="92">
+        <v>685</v>
+      </c>
+      <c r="C29" s="92">
+        <v>4</v>
+      </c>
+      <c r="D29" s="92">
+        <v>35000</v>
+      </c>
+      <c r="E29" s="92">
+        <v>34315</v>
+      </c>
+      <c r="F29" s="92"/>
+      <c r="G29" s="92"/>
+      <c r="H29" s="92">
+        <v>191</v>
+      </c>
+      <c r="I29" s="92">
+        <v>111</v>
+      </c>
+      <c r="J29" s="92">
+        <v>1</v>
+      </c>
+      <c r="K29" s="92">
+        <v>7200</v>
+      </c>
+      <c r="L29" s="92">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30" s="91">
+        <v>43919</v>
+      </c>
+      <c r="B30" s="92">
+        <v>769</v>
+      </c>
+      <c r="C30" s="92">
+        <v>4</v>
+      </c>
+      <c r="D30" s="92">
+        <v>39000</v>
+      </c>
+      <c r="E30" s="92">
+        <v>38231</v>
+      </c>
+      <c r="F30" s="92">
+        <v>26</v>
+      </c>
+      <c r="G30" s="92">
+        <v>4</v>
+      </c>
+      <c r="H30" s="92">
+        <v>193</v>
+      </c>
+      <c r="I30" s="92">
+        <v>84</v>
+      </c>
+      <c r="J30" s="92">
+        <v>0</v>
+      </c>
+      <c r="K30" s="92">
+        <v>4000</v>
+      </c>
+      <c r="L30" s="92">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31" s="91">
+        <v>43920</v>
+      </c>
+      <c r="B31" s="92">
+        <v>821</v>
+      </c>
+      <c r="C31" s="92">
+        <v>4</v>
+      </c>
+      <c r="D31" s="92">
+        <v>42000</v>
+      </c>
+      <c r="E31" s="92">
+        <v>41179</v>
+      </c>
+      <c r="F31" s="92"/>
+      <c r="G31" s="92">
+        <v>4</v>
+      </c>
+      <c r="H31" s="92">
+        <v>248</v>
+      </c>
+      <c r="I31" s="92">
+        <v>52</v>
+      </c>
+      <c r="J31" s="92">
+        <v>0</v>
+      </c>
+      <c r="K31" s="92">
+        <v>3000</v>
+      </c>
+      <c r="L31" s="92">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32" s="91">
+        <v>43921</v>
+      </c>
+      <c r="B32" s="92">
+        <v>917</v>
+      </c>
+      <c r="C32" s="92">
+        <v>4</v>
+      </c>
+      <c r="D32" s="92">
+        <v>45000</v>
+      </c>
+      <c r="E32" s="92">
+        <v>44083</v>
+      </c>
+      <c r="F32" s="92">
+        <v>29</v>
+      </c>
+      <c r="G32" s="92">
+        <v>4</v>
+      </c>
+      <c r="H32" s="92">
+        <v>291</v>
+      </c>
+      <c r="I32" s="92">
+        <v>96</v>
+      </c>
+      <c r="J32" s="92">
+        <v>0</v>
+      </c>
+      <c r="K32" s="92">
+        <v>3000</v>
+      </c>
+      <c r="L32" s="92">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A33" s="91">
+        <v>43922</v>
+      </c>
+      <c r="B33" s="92">
+        <v>968</v>
+      </c>
+      <c r="C33" s="92">
+        <v>5</v>
+      </c>
+      <c r="D33" s="92">
+        <v>47000</v>
+      </c>
+      <c r="E33" s="92">
+        <v>46032</v>
+      </c>
+      <c r="F33" s="92">
+        <v>32</v>
+      </c>
+      <c r="G33" s="92">
+        <v>6</v>
+      </c>
+      <c r="H33" s="92">
+        <v>343</v>
+      </c>
+      <c r="I33" s="92">
+        <v>51</v>
+      </c>
+      <c r="J33" s="92">
+        <v>1</v>
+      </c>
+      <c r="K33" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L33" s="92">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A34" s="91">
+        <v>43923</v>
+      </c>
+      <c r="B34" s="92">
+        <v>1036</v>
+      </c>
+      <c r="C34" s="92">
+        <v>6</v>
+      </c>
+      <c r="D34" s="92">
+        <v>49000</v>
+      </c>
+      <c r="E34" s="92">
+        <v>47964</v>
+      </c>
+      <c r="F34" s="92">
+        <v>34</v>
+      </c>
+      <c r="G34" s="92">
+        <v>6</v>
+      </c>
+      <c r="H34" s="92">
+        <v>422</v>
+      </c>
+      <c r="I34" s="92">
+        <v>68</v>
+      </c>
+      <c r="J34" s="92">
+        <v>1</v>
+      </c>
+      <c r="K34" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L34" s="92">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" s="91">
+        <v>43924</v>
+      </c>
+      <c r="B35" s="92">
+        <v>1085</v>
+      </c>
+      <c r="C35" s="92">
+        <v>7</v>
+      </c>
+      <c r="D35" s="92">
+        <v>51000</v>
+      </c>
+      <c r="E35" s="92">
+        <v>49915</v>
+      </c>
+      <c r="F35" s="92">
+        <v>37</v>
+      </c>
+      <c r="G35" s="92">
+        <v>7</v>
+      </c>
+      <c r="H35" s="92">
+        <v>476</v>
+      </c>
+      <c r="I35" s="92">
+        <v>49</v>
+      </c>
+      <c r="J35" s="92">
+        <v>1</v>
+      </c>
+      <c r="K35" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L35" s="92">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" s="91">
+        <v>43925</v>
+      </c>
+      <c r="B36" s="92">
+        <v>1115</v>
+      </c>
+      <c r="C36" s="92">
+        <v>8</v>
+      </c>
+      <c r="D36" s="92">
+        <v>54000</v>
+      </c>
+      <c r="E36" s="92">
+        <v>52885</v>
+      </c>
+      <c r="F36" s="92">
+        <v>42</v>
+      </c>
+      <c r="G36" s="92">
+        <v>10</v>
+      </c>
+      <c r="H36" s="92">
+        <v>527</v>
+      </c>
+      <c r="I36" s="92">
+        <v>30</v>
+      </c>
+      <c r="J36" s="92">
+        <v>1</v>
+      </c>
+      <c r="K36" s="92">
+        <v>3000</v>
+      </c>
+      <c r="L36" s="92">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37" s="91">
+        <v>43926</v>
+      </c>
+      <c r="B37" s="92">
+        <v>1135</v>
+      </c>
+      <c r="C37" s="92">
+        <v>8</v>
+      </c>
+      <c r="D37" s="92">
+        <v>56000</v>
+      </c>
+      <c r="E37" s="92">
+        <v>54865</v>
+      </c>
+      <c r="F37" s="92">
+        <v>47</v>
+      </c>
+      <c r="G37" s="92">
+        <v>11</v>
+      </c>
+      <c r="H37" s="92">
+        <v>573</v>
+      </c>
+      <c r="I37" s="92">
+        <v>20</v>
+      </c>
+      <c r="J37" s="92">
+        <v>0</v>
+      </c>
+      <c r="K37" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L37" s="92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" s="91">
+        <v>43927</v>
+      </c>
+      <c r="B38" s="92">
+        <v>1158</v>
+      </c>
+      <c r="C38" s="92">
+        <v>10</v>
+      </c>
+      <c r="D38" s="92">
+        <v>57000</v>
+      </c>
+      <c r="E38" s="92">
+        <v>55842</v>
+      </c>
+      <c r="F38" s="92">
+        <v>45</v>
+      </c>
+      <c r="G38" s="92">
+        <v>11</v>
+      </c>
+      <c r="H38" s="92">
+        <v>620</v>
+      </c>
+      <c r="I38" s="92">
+        <v>23</v>
+      </c>
+      <c r="J38" s="92">
+        <v>2</v>
+      </c>
+      <c r="K38" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L38" s="92">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" s="91">
+        <v>43928</v>
+      </c>
+      <c r="B39" s="92">
+        <v>1191</v>
+      </c>
+      <c r="C39" s="92">
+        <v>11</v>
+      </c>
+      <c r="D39" s="92">
+        <v>58000</v>
+      </c>
+      <c r="E39" s="92">
+        <v>56809</v>
+      </c>
+      <c r="F39" s="92">
+        <v>47</v>
+      </c>
+      <c r="G39" s="92">
+        <v>13</v>
+      </c>
+      <c r="H39" s="92">
+        <v>686</v>
+      </c>
+      <c r="I39" s="92">
+        <v>33</v>
+      </c>
+      <c r="J39" s="92">
+        <v>1</v>
+      </c>
+      <c r="K39" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L39" s="92">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" s="91">
+        <v>43929</v>
+      </c>
+      <c r="B40" s="92">
+        <v>1212</v>
+      </c>
+      <c r="C40" s="92">
+        <v>12</v>
+      </c>
+      <c r="D40" s="92">
+        <v>60000</v>
+      </c>
+      <c r="E40" s="92">
+        <v>58788</v>
+      </c>
+      <c r="F40" s="92">
+        <v>45</v>
+      </c>
+      <c r="G40" s="92">
+        <v>12</v>
+      </c>
+      <c r="H40" s="92">
+        <v>736</v>
+      </c>
+      <c r="I40" s="92">
+        <v>21</v>
+      </c>
+      <c r="J40" s="92">
+        <v>1</v>
+      </c>
+      <c r="K40" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L40" s="92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41" s="91">
+        <v>43930</v>
+      </c>
+      <c r="B41" s="92">
+        <v>1228</v>
+      </c>
+      <c r="C41" s="92">
+        <v>12</v>
+      </c>
+      <c r="D41" s="92">
+        <v>62000</v>
+      </c>
+      <c r="E41" s="92">
+        <v>60772</v>
+      </c>
+      <c r="F41" s="92">
+        <v>50</v>
+      </c>
+      <c r="G41" s="92">
+        <v>13</v>
+      </c>
+      <c r="H41" s="92">
+        <v>806</v>
+      </c>
+      <c r="I41" s="92">
+        <v>16</v>
+      </c>
+      <c r="J41" s="92">
+        <v>0</v>
+      </c>
+      <c r="K41" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L41" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="91">
+        <v>43931</v>
+      </c>
+      <c r="B42" s="92">
+        <v>1241</v>
+      </c>
+      <c r="C42" s="92">
+        <v>13</v>
+      </c>
+      <c r="D42" s="92">
+        <v>65000</v>
+      </c>
+      <c r="E42" s="92">
+        <v>63759</v>
+      </c>
+      <c r="F42" s="92">
+        <v>43</v>
+      </c>
+      <c r="G42" s="92">
+        <v>13</v>
+      </c>
+      <c r="H42" s="92">
+        <v>926</v>
+      </c>
+      <c r="I42" s="92">
+        <v>13</v>
+      </c>
+      <c r="J42" s="92">
+        <v>1</v>
+      </c>
+      <c r="K42" s="92">
+        <v>3000</v>
+      </c>
+      <c r="L42" s="92">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A43" s="91">
+        <v>43932</v>
+      </c>
+      <c r="B43" s="92">
+        <v>1265</v>
+      </c>
+      <c r="C43" s="92">
+        <v>14</v>
+      </c>
+      <c r="D43" s="92">
+        <v>67000</v>
+      </c>
+      <c r="E43" s="92">
+        <v>65735</v>
+      </c>
+      <c r="F43" s="92">
+        <v>44</v>
+      </c>
+      <c r="G43" s="92">
+        <v>15</v>
+      </c>
+      <c r="H43" s="92">
+        <v>986</v>
+      </c>
+      <c r="I43" s="92">
+        <v>24</v>
+      </c>
+      <c r="J43" s="92">
+        <v>1</v>
+      </c>
+      <c r="K43" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L43" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" s="91">
+        <v>43933</v>
+      </c>
+      <c r="B44" s="92">
+        <v>1268</v>
+      </c>
+      <c r="C44" s="92">
+        <v>14</v>
+      </c>
+      <c r="D44" s="92">
+        <v>69000</v>
+      </c>
+      <c r="E44" s="92">
+        <v>67732</v>
+      </c>
+      <c r="F44" s="92">
+        <v>44</v>
+      </c>
+      <c r="G44" s="92">
+        <v>16</v>
+      </c>
+      <c r="H44" s="92">
+        <v>1015</v>
+      </c>
+      <c r="I44" s="92">
+        <v>3</v>
+      </c>
+      <c r="J44" s="92">
+        <v>0</v>
+      </c>
+      <c r="K44" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L44" s="92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A45" s="91">
+        <v>43934</v>
+      </c>
+      <c r="B45" s="92">
+        <v>1281</v>
+      </c>
+      <c r="C45" s="92">
+        <v>14</v>
+      </c>
+      <c r="D45" s="92">
+        <v>70000</v>
+      </c>
+      <c r="E45" s="92">
+        <v>68719</v>
+      </c>
+      <c r="F45" s="92">
+        <v>40</v>
+      </c>
+      <c r="G45" s="92">
+        <v>14</v>
+      </c>
+      <c r="H45" s="92">
+        <v>1075</v>
+      </c>
+      <c r="I45" s="92">
+        <v>13</v>
+      </c>
+      <c r="J45" s="92">
+        <v>0</v>
+      </c>
+      <c r="K45" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L45" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A46" s="91">
+        <v>43935</v>
+      </c>
+      <c r="B46" s="92">
+        <v>1291</v>
+      </c>
+      <c r="C46" s="92">
+        <v>14</v>
+      </c>
+      <c r="D46" s="92">
+        <v>71000</v>
+      </c>
+      <c r="E46" s="92">
+        <v>69709</v>
+      </c>
+      <c r="F46" s="92">
+        <v>40</v>
+      </c>
+      <c r="G46" s="92">
+        <v>15</v>
+      </c>
+      <c r="H46" s="92">
+        <v>1118</v>
+      </c>
+      <c r="I46" s="92">
+        <v>10</v>
+      </c>
+      <c r="J46" s="92">
+        <v>0</v>
+      </c>
+      <c r="K46" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L46" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="91">
+        <v>43936</v>
+      </c>
+      <c r="B47" s="92">
+        <v>1299</v>
+      </c>
+      <c r="C47" s="92">
+        <v>14</v>
+      </c>
+      <c r="D47" s="92">
+        <v>72000</v>
+      </c>
+      <c r="E47" s="92">
+        <v>70701</v>
+      </c>
+      <c r="F47" s="92">
+        <v>39</v>
+      </c>
+      <c r="G47" s="92">
+        <v>18</v>
+      </c>
+      <c r="H47" s="92">
+        <v>1137</v>
+      </c>
+      <c r="I47" s="92">
+        <v>8</v>
+      </c>
+      <c r="J47" s="92">
+        <v>0</v>
+      </c>
+      <c r="K47" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L47" s="92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="91">
+        <v>43937</v>
+      </c>
+      <c r="B48" s="92">
+        <v>1301</v>
+      </c>
+      <c r="C48" s="92">
+        <v>14</v>
+      </c>
+      <c r="D48" s="92">
+        <v>73000</v>
+      </c>
+      <c r="E48" s="92">
+        <v>71699</v>
+      </c>
+      <c r="F48" s="92">
+        <v>39</v>
+      </c>
+      <c r="G48" s="92">
+        <v>18</v>
+      </c>
+      <c r="H48" s="92">
+        <v>1153</v>
+      </c>
+      <c r="I48" s="92">
+        <v>2</v>
+      </c>
+      <c r="J48" s="92">
+        <v>0</v>
+      </c>
+      <c r="K48" s="92">
+        <v>1000</v>
+      </c>
+      <c r="L48" s="92">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A49" s="91">
+        <v>43938</v>
+      </c>
+      <c r="B49" s="92">
+        <v>1302</v>
+      </c>
+      <c r="C49" s="92">
+        <v>14</v>
+      </c>
+      <c r="D49" s="92">
+        <v>75000</v>
+      </c>
+      <c r="E49" s="92">
+        <v>73698</v>
+      </c>
+      <c r="F49" s="92">
+        <v>32</v>
+      </c>
+      <c r="G49" s="92">
+        <v>13</v>
+      </c>
+      <c r="H49" s="92">
+        <v>1159</v>
+      </c>
+      <c r="I49" s="92">
+        <v>1</v>
+      </c>
+      <c r="J49" s="92">
+        <v>0</v>
+      </c>
+      <c r="K49" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L49" s="92">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" s="91">
+        <v>43939</v>
+      </c>
+      <c r="B50" s="92">
+        <v>1319</v>
+      </c>
+      <c r="C50" s="92">
+        <v>14</v>
+      </c>
+      <c r="D50" s="92">
+        <v>79000</v>
+      </c>
+      <c r="E50" s="92">
+        <v>77681</v>
+      </c>
+      <c r="F50" s="92">
+        <v>30</v>
+      </c>
+      <c r="G50" s="92">
+        <v>12</v>
+      </c>
+      <c r="H50" s="92">
+        <v>1172</v>
+      </c>
+      <c r="I50" s="92">
+        <v>17</v>
+      </c>
+      <c r="J50" s="92">
+        <v>0</v>
+      </c>
+      <c r="K50" s="92">
+        <v>4000</v>
+      </c>
+      <c r="L50" s="92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" s="91">
+        <v>43940</v>
+      </c>
+      <c r="B51" s="92">
+        <v>1328</v>
+      </c>
+      <c r="C51" s="92">
+        <v>15</v>
+      </c>
+      <c r="D51" s="92">
+        <v>82000</v>
+      </c>
+      <c r="E51" s="92">
+        <v>80672</v>
+      </c>
+      <c r="F51" s="92">
+        <v>29</v>
+      </c>
+      <c r="G51" s="92">
+        <v>10</v>
+      </c>
+      <c r="H51" s="92">
+        <v>1188</v>
+      </c>
+      <c r="I51" s="92">
+        <v>9</v>
+      </c>
+      <c r="J51" s="92">
+        <v>1</v>
+      </c>
+      <c r="K51" s="92">
+        <v>3000</v>
+      </c>
+      <c r="L51" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52" s="91">
+        <v>43941</v>
+      </c>
+      <c r="B52" s="92">
+        <v>1329</v>
+      </c>
+      <c r="C52" s="92">
+        <v>15</v>
+      </c>
+      <c r="D52" s="92">
+        <v>86000</v>
+      </c>
+      <c r="E52" s="92">
+        <v>84671</v>
+      </c>
+      <c r="F52" s="92">
+        <v>28</v>
+      </c>
+      <c r="G52" s="92">
+        <v>11</v>
+      </c>
+      <c r="H52" s="92">
+        <v>1196</v>
+      </c>
+      <c r="I52" s="92">
+        <v>1</v>
+      </c>
+      <c r="J52" s="92">
+        <v>0</v>
+      </c>
+      <c r="K52" s="92">
+        <v>4000</v>
+      </c>
+      <c r="L52" s="92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A53" s="91">
+        <v>43942</v>
+      </c>
+      <c r="B53" s="92">
+        <v>1336</v>
+      </c>
+      <c r="C53" s="92">
+        <v>15</v>
+      </c>
+      <c r="D53" s="92">
+        <v>88000</v>
+      </c>
+      <c r="E53" s="92">
+        <v>86664</v>
+      </c>
+      <c r="F53" s="92">
+        <v>28</v>
+      </c>
+      <c r="G53" s="92">
+        <v>12</v>
+      </c>
+      <c r="H53" s="92">
+        <v>1202</v>
+      </c>
+      <c r="I53" s="92">
+        <v>7</v>
+      </c>
+      <c r="J53" s="92">
+        <v>0</v>
+      </c>
+      <c r="K53" s="92">
+        <v>2000</v>
+      </c>
+      <c r="L53" s="92">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84637A79-E027-48E7-B7DE-002E7C836FC2}">
   <sheetPr>
     <tabColor rgb="FFC63500"/>
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y2" sqref="Y2"/>
+    <sheetView zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7838,31 +10163,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="87" t="s">
         <v>246</v>
       </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="78"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="88"/>
       <c r="V1" s="55"/>
-      <c r="W1" s="77" t="s">
+      <c r="W1" s="87" t="s">
         <v>228</v>
       </c>
-      <c r="X1" s="78"/>
+      <c r="X1" s="88"/>
     </row>
     <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
@@ -10658,434 +12983,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{288C3D6A-28F1-7940-82D1-054C6895C15C}">
-  <dimension ref="A1:AC3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="84"/>
-    <col min="21" max="21" width="10.83203125" style="80"/>
-    <col min="22" max="22" width="10.83203125" style="84"/>
-    <col min="24" max="24" width="10.83203125" style="80"/>
-    <col min="26" max="26" width="10.83203125" style="80"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="25"/>
-      <c r="B1" s="24"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="77" t="s">
-        <v>246</v>
-      </c>
-      <c r="E1" s="79"/>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79"/>
-      <c r="I1" s="79"/>
-      <c r="J1" s="79"/>
-      <c r="K1" s="79"/>
-      <c r="L1" s="79"/>
-      <c r="M1" s="79"/>
-      <c r="N1" s="79"/>
-      <c r="O1" s="79"/>
-      <c r="P1" s="79"/>
-      <c r="Q1" s="79"/>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="77" t="s">
-        <v>228</v>
-      </c>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="24"/>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25"/>
-    </row>
-    <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
-        <v>296</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>151</v>
-      </c>
-      <c r="C2" s="89" t="s">
-        <v>188</v>
-      </c>
-      <c r="D2" s="42" t="str">
-        <f ca="1">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
-        <v>H</v>
-      </c>
-      <c r="E2" s="42" t="str">
-        <f t="shared" ref="E2:U2" ca="1" si="0">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
-        <v>S</v>
-      </c>
-      <c r="F2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>W</v>
-      </c>
-      <c r="G2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>C</v>
-      </c>
-      <c r="H2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>Church</v>
-      </c>
-      <c r="I2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>pSport</v>
-      </c>
-      <c r="J2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>cSport</v>
-      </c>
-      <c r="K2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>beach</v>
-      </c>
-      <c r="L2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>entertainment</v>
-      </c>
-      <c r="M2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>cafe_restaurant</v>
-      </c>
-      <c r="N2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>pub_bar</v>
-      </c>
-      <c r="O2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>transport</v>
-      </c>
-      <c r="P2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>national_parks</v>
-      </c>
-      <c r="Q2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>public_parks</v>
-      </c>
-      <c r="R2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>large_events</v>
-      </c>
-      <c r="S2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>child_care</v>
-      </c>
-      <c r="T2" s="42" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>social</v>
-      </c>
-      <c r="U2" s="81" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>aged_care</v>
-      </c>
-      <c r="V2" s="83" t="s">
-        <v>229</v>
-      </c>
-      <c r="W2" s="43" t="s">
-        <v>225</v>
-      </c>
-      <c r="X2" s="86" t="s">
-        <v>224</v>
-      </c>
-      <c r="Y2" s="42" t="s">
-        <v>297</v>
-      </c>
-      <c r="Z2" s="81" t="s">
-        <v>298</v>
-      </c>
-      <c r="AA2" s="41"/>
-      <c r="AB2" s="40"/>
-      <c r="AC2" s="40"/>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>294</v>
-      </c>
-      <c r="B3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C3" s="84">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3">
-        <v>1</v>
-      </c>
-      <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-      <c r="U3">
-        <v>1</v>
-      </c>
-      <c r="V3" s="84">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="D1:U1"/>
-    <mergeCell ref="W1:X1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
-  <dimension ref="A1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="51.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>172</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="B2" s="18">
-        <v>43891</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="B3" s="18">
-        <v>44075</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="19">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B5">
-        <v>20000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>174</v>
-      </c>
-      <c r="B6">
-        <f>6200000/B5</f>
-        <v>310</v>
-      </c>
-      <c r="C6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>175</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>176</v>
-      </c>
-      <c r="B8">
-        <v>0.2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>182</v>
-      </c>
-      <c r="B9">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12">
-        <v>0.6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>290</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>282</v>
-      </c>
-      <c r="B15">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>283</v>
-      </c>
-      <c r="B16">
-        <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>284</v>
-      </c>
-      <c r="B17">
-        <v>2000</v>
-      </c>
-      <c r="C17" t="s">
-        <v>288</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3870F7-A576-4BD3-9D23-1C9E10583711}">
   <dimension ref="A1:D8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed quar_eff to quar_factor
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwork/Documents/GitHub/covasim-australia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AC3342-B29A-C540-9CEB-1A1993E6E585}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9E778-1435-FC42-8326-CC3C73972327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6640" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="762" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact matrices-home" sheetId="2" r:id="rId1"/>
@@ -156,7 +156,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -165,12 +165,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-1 means that someone in quarantine is still in the network (completely ineffective, e.g. household), 0 means that someone who is quarantined is completely removed from network (perfect quarantine).</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>1 means that someone in quarantine is still in the network (completely ineffective, e.g. household), 0 means that someone who is quarantined is completely removed from network (perfect quarantine).</t>
         </r>
       </text>
     </comment>
@@ -277,7 +286,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -286,12 +295,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assume quarantine does not impact within-household transmission</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assume quarantine does not impact within-household transmission</t>
         </r>
       </text>
     </comment>
@@ -349,7 +367,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -358,12 +376,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Assume quarantine does not impact within-household transmission</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assume quarantine does not impact within-household transmission</t>
         </r>
       </text>
     </comment>
@@ -750,7 +777,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -759,12 +786,21 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-picnics, gatherings</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>picnics, gatherings</t>
         </r>
       </text>
     </comment>
@@ -1728,9 +1764,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>quar_eff</t>
-  </si>
-  <si>
     <t>proportion</t>
   </si>
   <si>
@@ -2179,6 +2212,9 @@
   </si>
   <si>
     <t>daily_imported_cases</t>
+  </si>
+  <si>
+    <t>quar_factor</t>
   </si>
 </sst>
 </file>
@@ -3123,10 +3159,10 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6880,10 +6916,10 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C33" sqref="C33"/>
-      <selection pane="bottomLeft" activeCell="A6" activeCellId="3" sqref="A19:XFD19 A17:XFD17 A8:XFD8 A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6906,7 +6942,7 @@
         <v>151</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>152</v>
@@ -6915,33 +6951,33 @@
         <v>153</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>158</v>
       </c>
-      <c r="H1" s="22" t="s">
-        <v>159</v>
-      </c>
       <c r="I1" s="22" t="s">
-        <v>155</v>
+        <v>305</v>
       </c>
       <c r="J1" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="K1" s="22" t="s">
-        <v>190</v>
-      </c>
       <c r="L1" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="B2" s="23" t="s">
         <v>160</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>161</v>
       </c>
       <c r="C2" s="72">
         <v>1</v>
@@ -6959,7 +6995,7 @@
         <v>110</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I2" s="23">
         <v>1</v>
@@ -6976,10 +7012,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>162</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>163</v>
       </c>
       <c r="C3" s="72">
         <v>1</v>
@@ -6997,7 +7033,7 @@
         <v>18</v>
       </c>
       <c r="H3" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I3" s="23">
         <v>0</v>
@@ -7014,10 +7050,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C4" s="72">
         <v>1</v>
@@ -7035,7 +7071,7 @@
         <v>65</v>
       </c>
       <c r="H4" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I4" s="23">
         <v>0</v>
@@ -7052,10 +7088,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="74">
         <v>1</v>
@@ -7073,7 +7109,7 @@
         <v>110</v>
       </c>
       <c r="H5" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I5" s="23">
         <v>0.1</v>
@@ -7090,10 +7126,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="B6" s="23" t="s">
         <v>165</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>166</v>
       </c>
       <c r="C6" s="74">
         <v>0.11</v>
@@ -7111,7 +7147,7 @@
         <v>110</v>
       </c>
       <c r="H6" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I6" s="23">
         <v>0.1</v>
@@ -7128,10 +7164,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B7" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>168</v>
       </c>
       <c r="C7" s="74">
         <v>5.9999999999999995E-4</v>
@@ -7149,7 +7185,7 @@
         <v>40</v>
       </c>
       <c r="H7" s="72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I7" s="23">
         <v>0</v>
@@ -7166,10 +7202,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>203</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>204</v>
       </c>
       <c r="C8" s="74">
         <v>0.34</v>
@@ -7187,7 +7223,7 @@
         <v>30</v>
       </c>
       <c r="H8" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I8" s="23">
         <v>0.1</v>
@@ -7204,10 +7240,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="74">
         <v>0.2</v>
@@ -7225,7 +7261,7 @@
         <v>80</v>
       </c>
       <c r="H9" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I9" s="23">
         <v>0.1</v>
@@ -7242,10 +7278,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C10" s="74">
         <v>0.3</v>
@@ -7263,7 +7299,7 @@
         <v>110</v>
       </c>
       <c r="H10" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I10" s="23">
         <v>0.1</v>
@@ -7280,10 +7316,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C11" s="74">
         <v>0.6</v>
@@ -7301,7 +7337,7 @@
         <v>110</v>
       </c>
       <c r="H11" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I11" s="23">
         <v>0.1</v>
@@ -7318,10 +7354,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>260</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>261</v>
       </c>
       <c r="C12" s="23">
         <v>0.4</v>
@@ -7339,7 +7375,7 @@
         <v>110</v>
       </c>
       <c r="H12" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I12" s="23">
         <v>0.1</v>
@@ -7356,10 +7392,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C13" s="23">
         <v>0.114</v>
@@ -7377,7 +7413,7 @@
         <v>110</v>
       </c>
       <c r="H13" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I13" s="23">
         <v>0.1</v>
@@ -7394,10 +7430,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="23" t="s">
         <v>198</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>199</v>
       </c>
       <c r="C14" s="23">
         <v>5.5E-2</v>
@@ -7415,7 +7451,7 @@
         <v>110</v>
       </c>
       <c r="H14" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I14" s="23">
         <v>0.1</v>
@@ -7432,10 +7468,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B15" s="23" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C15" s="23">
         <v>0.6</v>
@@ -7453,7 +7489,7 @@
         <v>110</v>
       </c>
       <c r="H15" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I15" s="23">
         <v>0.1</v>
@@ -7470,10 +7506,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B16" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C16" s="23">
         <v>0.2</v>
@@ -7492,7 +7528,7 @@
         <v>110</v>
       </c>
       <c r="H16" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I16" s="23">
         <v>0.1</v>
@@ -7509,10 +7545,10 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="B17" s="23" t="s">
         <v>251</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>252</v>
       </c>
       <c r="C17" s="23">
         <v>0.54500000000000004</v>
@@ -7530,7 +7566,7 @@
         <v>6</v>
       </c>
       <c r="H17" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I17" s="23">
         <v>0</v>
@@ -7547,10 +7583,10 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C18" s="23">
         <v>1</v>
@@ -7568,7 +7604,7 @@
         <v>110</v>
       </c>
       <c r="H18" s="72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I18" s="23">
         <v>0.1</v>
@@ -7585,10 +7621,10 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="B19" s="23" t="s">
         <v>277</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>278</v>
       </c>
       <c r="C19" s="23">
         <v>7.0000000000000007E-2</v>
@@ -7606,7 +7642,7 @@
         <v>110</v>
       </c>
       <c r="H19" s="72" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I19" s="23">
         <v>0</v>
@@ -7635,7 +7671,7 @@
   </sheetPr>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="109" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -7658,40 +7694,40 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="D1" s="81" t="s">
-        <v>246</v>
-      </c>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="83"/>
+        <v>245</v>
+      </c>
+      <c r="E1" s="83"/>
+      <c r="F1" s="83"/>
+      <c r="G1" s="83"/>
+      <c r="H1" s="83"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="82"/>
       <c r="V1" s="55"/>
       <c r="W1" s="81" t="s">
-        <v>228</v>
-      </c>
-      <c r="X1" s="83"/>
+        <v>227</v>
+      </c>
+      <c r="X1" s="82"/>
     </row>
     <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D2" s="51" t="str">
         <f ca="1">INDIRECT("layers!A"&amp;COLUMN() -2)</f>
@@ -7766,19 +7802,19 @@
         <v>aged_care</v>
       </c>
       <c r="V2" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="W2" s="57" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="X2" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="Y2" s="51" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="Z2" s="42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="AA2" s="41"/>
       <c r="AB2" s="40"/>
@@ -7786,10 +7822,10 @@
     </row>
     <row r="3" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C3" s="47">
         <v>0.14000000000000001</v>
@@ -7863,10 +7899,10 @@
     </row>
     <row r="4" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C4" s="48">
         <v>1</v>
@@ -7940,10 +7976,10 @@
     </row>
     <row r="5" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C5" s="48">
         <v>1</v>
@@ -8015,10 +8051,10 @@
     </row>
     <row r="6" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="33" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="48">
         <v>1</v>
@@ -8090,10 +8126,10 @@
     </row>
     <row r="7" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="48">
         <v>1</v>
@@ -8167,10 +8203,10 @@
     </row>
     <row r="8" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="33" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8" s="48">
         <v>1</v>
@@ -8244,10 +8280,10 @@
     </row>
     <row r="9" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9" s="48">
         <v>1</v>
@@ -8324,10 +8360,10 @@
     </row>
     <row r="10" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="33" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C10" s="48">
         <v>1</v>
@@ -8401,10 +8437,10 @@
     </row>
     <row r="11" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C11" s="48">
         <v>1</v>
@@ -8481,10 +8517,10 @@
     </row>
     <row r="12" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
+        <v>263</v>
+      </c>
+      <c r="B12" s="34" t="s">
         <v>264</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>265</v>
       </c>
       <c r="C12" s="48">
         <v>1</v>
@@ -8558,10 +8594,10 @@
     </row>
     <row r="13" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
+        <v>265</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>266</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>267</v>
       </c>
       <c r="C13" s="48">
         <v>1</v>
@@ -8638,10 +8674,10 @@
     </row>
     <row r="14" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C14" s="48">
         <v>1</v>
@@ -8715,10 +8751,10 @@
     </row>
     <row r="15" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C15" s="48">
         <v>1</v>
@@ -8790,10 +8826,10 @@
     </row>
     <row r="16" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C16" s="48">
         <v>1</v>
@@ -8870,10 +8906,10 @@
     </row>
     <row r="17" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C17" s="48">
         <v>1</v>
@@ -8947,10 +8983,10 @@
     </row>
     <row r="18" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C18" s="48">
         <v>1</v>
@@ -9024,10 +9060,10 @@
     </row>
     <row r="19" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C19" s="48">
         <v>1</v>
@@ -9099,10 +9135,10 @@
     </row>
     <row r="20" spans="1:29" s="35" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C20" s="48">
         <v>1</v>
@@ -9165,7 +9201,7 @@
         <v>0</v>
       </c>
       <c r="W20" s="63" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="X20" s="65">
         <v>0.1</v>
@@ -9180,10 +9216,10 @@
     </row>
     <row r="21" spans="1:29" s="21" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C21" s="48">
         <v>1</v>
@@ -9246,7 +9282,7 @@
         <v>0</v>
       </c>
       <c r="W21" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X21" s="64">
         <v>0.95</v>
@@ -9261,10 +9297,10 @@
     </row>
     <row r="22" spans="1:29" s="21" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C22" s="48">
         <v>1</v>
@@ -9338,10 +9374,10 @@
     </row>
     <row r="23" spans="1:29" s="21" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C23" s="48">
         <v>1</v>
@@ -9415,10 +9451,10 @@
     </row>
     <row r="24" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="30" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B24" s="30" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C24" s="48">
         <v>1</v>
@@ -9481,7 +9517,7 @@
         <v>0</v>
       </c>
       <c r="W24" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X24" s="64">
         <v>0.8</v>
@@ -9496,10 +9532,10 @@
     </row>
     <row r="25" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="30" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C25" s="48">
         <v>1</v>
@@ -9562,7 +9598,7 @@
         <v>0</v>
       </c>
       <c r="W25" s="63" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="X25" s="64">
         <v>0.95</v>
@@ -9577,10 +9613,10 @@
     </row>
     <row r="26" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C26" s="48">
         <v>1</v>
@@ -9654,10 +9690,10 @@
     </row>
     <row r="27" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="30" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C27" s="48">
         <v>1</v>
@@ -9731,10 +9767,10 @@
     </row>
     <row r="28" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B28" s="67" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C28" s="47">
         <v>0.8</v>
@@ -9806,10 +9842,10 @@
     </row>
     <row r="29" spans="1:29" s="20" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="B29" s="26" t="s">
         <v>279</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>280</v>
       </c>
       <c r="C29" s="48">
         <v>1</v>
@@ -10496,7 +10532,7 @@
         <v>154</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>151</v>
@@ -10504,29 +10540,29 @@
     </row>
     <row r="2" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="18">
         <v>43891</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="18">
         <v>44075</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="19">
         <v>10</v>
@@ -10534,30 +10570,30 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5">
         <v>20000</v>
       </c>
       <c r="C5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6">
         <f>6200000/B5</f>
         <v>310</v>
       </c>
       <c r="C6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -10565,18 +10601,18 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>0.2</v>
       </c>
       <c r="C8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B9">
         <v>1.2</v>
@@ -10584,18 +10620,18 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B10">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <v>0.17</v>
@@ -10603,68 +10639,68 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12">
         <v>0.6</v>
       </c>
       <c r="C12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>289</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
         <v>290</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B15">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16">
         <v>60</v>
       </c>
       <c r="C16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B17">
         <v>2000</v>
       </c>
       <c r="C17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -10687,40 +10723,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="77" t="s">
+        <v>293</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>295</v>
       </c>
-      <c r="C1" s="77" t="s">
+      <c r="D1" s="77" t="s">
         <v>296</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="E1" s="77" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="77" t="s">
+      <c r="F1" s="77" t="s">
         <v>298</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="G1" s="77" t="s">
         <v>299</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="H1" s="77" t="s">
         <v>300</v>
       </c>
-      <c r="H1" s="77" t="s">
+      <c r="I1" s="77" t="s">
         <v>301</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="J1" s="77" t="s">
         <v>302</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="K1" s="77" t="s">
         <v>303</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="L1" s="77" t="s">
         <v>304</v>
-      </c>
-      <c r="L1" s="77" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -12500,16 +12536,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1" t="s">
         <v>272</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>273</v>
-      </c>
-      <c r="D1" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -12604,7 +12640,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C8" s="70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D8" s="71">
         <f>SUM(B2:B7)/SUM(C2:C7)</f>

</xml_diff>

<commit_message>
Updated diag_factor to iso_factor
</commit_message>
<xml_diff>
--- a/data/vic-data.xlsx
+++ b/data/vic-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samwork/Documents/GitHub/covasim-australia/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE9E778-1435-FC42-8326-CC3C73972327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0335E8CD-A748-A248-A4FC-D3AF9069F813}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="762" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact matrices-home" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,7 @@
     <sheet name="layers" sheetId="5" r:id="rId4"/>
     <sheet name="policies" sheetId="7" r:id="rId5"/>
     <sheet name="other_par" sheetId="6" r:id="rId6"/>
-    <sheet name="epi_data" sheetId="11" r:id="rId7"/>
-    <sheet name="data" sheetId="8" r:id="rId8"/>
+    <sheet name="data" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1297,7 +1296,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="292">
   <si>
     <t>age</t>
   </si>
@@ -2166,52 +2165,10 @@
     <t>Physical distancing relaxed a bit (what do we go back to)</t>
   </si>
   <si>
-    <t>diag_factor</t>
-  </si>
-  <si>
-    <t>Proportion of cases that are asymptomatic (for estimate cumulative cases data)</t>
-  </si>
-  <si>
     <t>Proportion who are asymptomatic</t>
   </si>
   <si>
     <t>iso_factor</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>cum_infections</t>
-  </si>
-  <si>
-    <t>cum_deaths</t>
-  </si>
-  <si>
-    <t>cum_test</t>
-  </si>
-  <si>
-    <t>cum_neg</t>
-  </si>
-  <si>
-    <t>n_severe</t>
-  </si>
-  <si>
-    <t>n_critical</t>
-  </si>
-  <si>
-    <t>cum_recovered</t>
-  </si>
-  <si>
-    <t>new_diagnoses</t>
-  </si>
-  <si>
-    <t>new_deaths</t>
-  </si>
-  <si>
-    <t>new_tests</t>
-  </si>
-  <si>
-    <t>daily_imported_cases</t>
   </si>
   <si>
     <t>quar_factor</t>
@@ -2225,7 +2182,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2489,23 +2446,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="41">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2719,18 +2661,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -2982,7 +2912,7 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3152,10 +3082,6 @@
     <xf numFmtId="2" fontId="31" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="38" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6916,7 +6842,7 @@
   </sheetPr>
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C33" sqref="C33"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
@@ -6960,7 +6886,7 @@
         <v>158</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="J1" s="22" t="s">
         <v>188</v>
@@ -6969,7 +6895,7 @@
         <v>189</v>
       </c>
       <c r="L1" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -7693,31 +7619,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="77" t="s">
         <v>245</v>
       </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="82"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="78"/>
       <c r="V1" s="55"/>
-      <c r="W1" s="81" t="s">
+      <c r="W1" s="77" t="s">
         <v>227</v>
       </c>
-      <c r="X1" s="82"/>
+      <c r="X1" s="78"/>
     </row>
     <row r="2" spans="1:29" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
@@ -10517,8 +10443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BC351A-C64B-994E-8CEF-B4F269832CFD}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10645,18 +10571,15 @@
         <v>0.6</v>
       </c>
       <c r="C12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B13">
         <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -10709,1822 +10632,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3091FBE5-3E95-934F-B436-B236BC518E77}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:L53"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
-        <v>293</v>
-      </c>
-      <c r="B1" s="77" t="s">
-        <v>294</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>295</v>
-      </c>
-      <c r="D1" s="77" t="s">
-        <v>296</v>
-      </c>
-      <c r="E1" s="77" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" s="77" t="s">
-        <v>298</v>
-      </c>
-      <c r="G1" s="77" t="s">
-        <v>299</v>
-      </c>
-      <c r="H1" s="77" t="s">
-        <v>300</v>
-      </c>
-      <c r="I1" s="77" t="s">
-        <v>301</v>
-      </c>
-      <c r="J1" s="77" t="s">
-        <v>302</v>
-      </c>
-      <c r="K1" s="77" t="s">
-        <v>303</v>
-      </c>
-      <c r="L1" s="77" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="78">
-        <v>43891</v>
-      </c>
-      <c r="B2" s="79">
-        <v>9</v>
-      </c>
-      <c r="C2" s="79">
-        <v>0</v>
-      </c>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
-      <c r="I2" s="79">
-        <v>2</v>
-      </c>
-      <c r="J2" s="79">
-        <v>0</v>
-      </c>
-      <c r="K2" s="79">
-        <v>0</v>
-      </c>
-      <c r="L2" s="79">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="78">
-        <v>43892</v>
-      </c>
-      <c r="B3" s="79">
-        <v>9</v>
-      </c>
-      <c r="C3" s="79">
-        <v>0</v>
-      </c>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79">
-        <v>0</v>
-      </c>
-      <c r="J3" s="79">
-        <v>0</v>
-      </c>
-      <c r="K3" s="79">
-        <v>0</v>
-      </c>
-      <c r="L3" s="79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="78">
-        <v>43893</v>
-      </c>
-      <c r="B4" s="79">
-        <v>9</v>
-      </c>
-      <c r="C4" s="79">
-        <v>0</v>
-      </c>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79">
-        <v>0</v>
-      </c>
-      <c r="J4" s="79">
-        <v>0</v>
-      </c>
-      <c r="K4" s="79">
-        <v>0</v>
-      </c>
-      <c r="L4" s="79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="78">
-        <v>43894</v>
-      </c>
-      <c r="B5" s="79">
-        <v>10</v>
-      </c>
-      <c r="C5" s="79">
-        <v>0</v>
-      </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79">
-        <v>1</v>
-      </c>
-      <c r="J5" s="79">
-        <v>0</v>
-      </c>
-      <c r="K5" s="79">
-        <v>0</v>
-      </c>
-      <c r="L5" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="78">
-        <v>43895</v>
-      </c>
-      <c r="B6" s="79">
-        <v>10</v>
-      </c>
-      <c r="C6" s="79">
-        <v>0</v>
-      </c>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79">
-        <v>0</v>
-      </c>
-      <c r="J6" s="79">
-        <v>0</v>
-      </c>
-      <c r="K6" s="79">
-        <v>0</v>
-      </c>
-      <c r="L6" s="79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="78">
-        <v>43896</v>
-      </c>
-      <c r="B7" s="79">
-        <v>10</v>
-      </c>
-      <c r="C7" s="79">
-        <v>0</v>
-      </c>
-      <c r="D7" s="79"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="79"/>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79"/>
-      <c r="I7" s="79">
-        <v>0</v>
-      </c>
-      <c r="J7" s="79">
-        <v>0</v>
-      </c>
-      <c r="K7" s="79">
-        <v>0</v>
-      </c>
-      <c r="L7" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="78">
-        <v>43897</v>
-      </c>
-      <c r="B8" s="79">
-        <v>11</v>
-      </c>
-      <c r="C8" s="79">
-        <v>0</v>
-      </c>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="79">
-        <v>1</v>
-      </c>
-      <c r="J8" s="79">
-        <v>0</v>
-      </c>
-      <c r="K8" s="79">
-        <v>0</v>
-      </c>
-      <c r="L8" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="78">
-        <v>43898</v>
-      </c>
-      <c r="B9" s="79">
-        <v>12</v>
-      </c>
-      <c r="C9" s="79">
-        <v>0</v>
-      </c>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79">
-        <v>1</v>
-      </c>
-      <c r="J9" s="79">
-        <v>0</v>
-      </c>
-      <c r="K9" s="79">
-        <v>0</v>
-      </c>
-      <c r="L9" s="79">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="78">
-        <v>43899</v>
-      </c>
-      <c r="B10" s="79">
-        <v>15</v>
-      </c>
-      <c r="C10" s="79">
-        <v>0</v>
-      </c>
-      <c r="D10" s="79"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="79">
-        <v>3</v>
-      </c>
-      <c r="J10" s="79">
-        <v>0</v>
-      </c>
-      <c r="K10" s="79">
-        <v>0</v>
-      </c>
-      <c r="L10" s="79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="78">
-        <v>43900</v>
-      </c>
-      <c r="B11" s="79">
-        <v>18</v>
-      </c>
-      <c r="C11" s="79">
-        <v>0</v>
-      </c>
-      <c r="D11" s="79"/>
-      <c r="E11" s="79"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="79">
-        <v>3</v>
-      </c>
-      <c r="J11" s="79">
-        <v>0</v>
-      </c>
-      <c r="K11" s="79">
-        <v>0</v>
-      </c>
-      <c r="L11" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="78">
-        <v>43901</v>
-      </c>
-      <c r="B12" s="79">
-        <v>21</v>
-      </c>
-      <c r="C12" s="79">
-        <v>0</v>
-      </c>
-      <c r="D12" s="79"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79">
-        <v>3</v>
-      </c>
-      <c r="J12" s="79">
-        <v>0</v>
-      </c>
-      <c r="K12" s="79">
-        <v>0</v>
-      </c>
-      <c r="L12" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="78">
-        <v>43902</v>
-      </c>
-      <c r="B13" s="79">
-        <v>27</v>
-      </c>
-      <c r="C13" s="79">
-        <v>0</v>
-      </c>
-      <c r="D13" s="79"/>
-      <c r="E13" s="79"/>
-      <c r="F13" s="79"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="79">
-        <v>6</v>
-      </c>
-      <c r="J13" s="79">
-        <v>0</v>
-      </c>
-      <c r="K13" s="79">
-        <v>0</v>
-      </c>
-      <c r="L13" s="79">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="78">
-        <v>43903</v>
-      </c>
-      <c r="B14" s="79">
-        <v>36</v>
-      </c>
-      <c r="C14" s="79">
-        <v>0</v>
-      </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79">
-        <v>9</v>
-      </c>
-      <c r="J14" s="79">
-        <v>0</v>
-      </c>
-      <c r="K14" s="80">
-        <v>500</v>
-      </c>
-      <c r="L14" s="79">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="78">
-        <v>43904</v>
-      </c>
-      <c r="B15" s="79">
-        <v>49</v>
-      </c>
-      <c r="C15" s="79">
-        <v>0</v>
-      </c>
-      <c r="D15" s="79"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="79">
-        <v>13</v>
-      </c>
-      <c r="J15" s="79">
-        <v>0</v>
-      </c>
-      <c r="K15" s="80">
-        <v>500</v>
-      </c>
-      <c r="L15" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="78">
-        <v>43905</v>
-      </c>
-      <c r="B16" s="79">
-        <v>57</v>
-      </c>
-      <c r="C16" s="79">
-        <v>0</v>
-      </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="79">
-        <v>8</v>
-      </c>
-      <c r="J16" s="79">
-        <v>0</v>
-      </c>
-      <c r="K16" s="80">
-        <v>500</v>
-      </c>
-      <c r="L16" s="79">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="78">
-        <v>43906</v>
-      </c>
-      <c r="B17" s="79">
-        <v>71</v>
-      </c>
-      <c r="C17" s="79">
-        <v>0</v>
-      </c>
-      <c r="D17" s="79">
-        <v>11700</v>
-      </c>
-      <c r="E17" s="79">
-        <v>11629</v>
-      </c>
-      <c r="F17" s="79"/>
-      <c r="G17" s="79"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="79">
-        <v>14</v>
-      </c>
-      <c r="J17" s="79">
-        <v>0</v>
-      </c>
-      <c r="K17" s="80">
-        <v>500</v>
-      </c>
-      <c r="L17" s="79">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="78">
-        <v>43907</v>
-      </c>
-      <c r="B18" s="79">
-        <v>94</v>
-      </c>
-      <c r="C18" s="79">
-        <v>0</v>
-      </c>
-      <c r="D18" s="79">
-        <v>14200</v>
-      </c>
-      <c r="E18" s="79">
-        <v>14106</v>
-      </c>
-      <c r="F18" s="79"/>
-      <c r="G18" s="79"/>
-      <c r="H18" s="79"/>
-      <c r="I18" s="79">
-        <v>23</v>
-      </c>
-      <c r="J18" s="79">
-        <v>0</v>
-      </c>
-      <c r="K18" s="80">
-        <v>1000</v>
-      </c>
-      <c r="L18" s="79">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="78">
-        <v>43908</v>
-      </c>
-      <c r="B19" s="79">
-        <v>121</v>
-      </c>
-      <c r="C19" s="79">
-        <v>0</v>
-      </c>
-      <c r="D19" s="79">
-        <v>15200</v>
-      </c>
-      <c r="E19" s="79">
-        <v>15079</v>
-      </c>
-      <c r="F19" s="79"/>
-      <c r="G19" s="79"/>
-      <c r="H19" s="79"/>
-      <c r="I19" s="79">
-        <v>27</v>
-      </c>
-      <c r="J19" s="79">
-        <v>0</v>
-      </c>
-      <c r="K19" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L19" s="79">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="78">
-        <v>43909</v>
-      </c>
-      <c r="B20" s="79">
-        <v>150</v>
-      </c>
-      <c r="C20" s="79">
-        <v>0</v>
-      </c>
-      <c r="D20" s="79">
-        <v>17180</v>
-      </c>
-      <c r="E20" s="79">
-        <v>17030</v>
-      </c>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79"/>
-      <c r="H20" s="79"/>
-      <c r="I20" s="79">
-        <v>29</v>
-      </c>
-      <c r="J20" s="79">
-        <v>0</v>
-      </c>
-      <c r="K20" s="79">
-        <v>1980</v>
-      </c>
-      <c r="L20" s="79">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="78">
-        <v>43910</v>
-      </c>
-      <c r="B21" s="79">
-        <v>178</v>
-      </c>
-      <c r="C21" s="79">
-        <v>0</v>
-      </c>
-      <c r="D21" s="79">
-        <v>19337</v>
-      </c>
-      <c r="E21" s="79">
-        <v>19159</v>
-      </c>
-      <c r="F21" s="79"/>
-      <c r="G21" s="79"/>
-      <c r="H21" s="79"/>
-      <c r="I21" s="79">
-        <v>28</v>
-      </c>
-      <c r="J21" s="79">
-        <v>0</v>
-      </c>
-      <c r="K21" s="79">
-        <v>2157</v>
-      </c>
-      <c r="L21" s="79">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="78">
-        <v>43911</v>
-      </c>
-      <c r="B22" s="79">
-        <v>229</v>
-      </c>
-      <c r="C22" s="79">
-        <v>0</v>
-      </c>
-      <c r="D22" s="79">
-        <v>20500</v>
-      </c>
-      <c r="E22" s="79">
-        <v>20271</v>
-      </c>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79">
-        <v>51</v>
-      </c>
-      <c r="J22" s="79">
-        <v>0</v>
-      </c>
-      <c r="K22" s="79">
-        <v>1163</v>
-      </c>
-      <c r="L22" s="79">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="78">
-        <v>43912</v>
-      </c>
-      <c r="B23" s="79">
-        <v>296</v>
-      </c>
-      <c r="C23" s="79">
-        <v>0</v>
-      </c>
-      <c r="D23" s="79">
-        <v>22900</v>
-      </c>
-      <c r="E23" s="79">
-        <v>22604</v>
-      </c>
-      <c r="F23" s="79"/>
-      <c r="G23" s="79"/>
-      <c r="H23" s="79"/>
-      <c r="I23" s="79">
-        <v>67</v>
-      </c>
-      <c r="J23" s="79">
-        <v>0</v>
-      </c>
-      <c r="K23" s="79">
-        <v>2400</v>
-      </c>
-      <c r="L23" s="79">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="78">
-        <v>43913</v>
-      </c>
-      <c r="B24" s="79">
-        <v>355</v>
-      </c>
-      <c r="C24" s="79">
-        <v>0</v>
-      </c>
-      <c r="D24" s="79">
-        <v>23700</v>
-      </c>
-      <c r="E24" s="79">
-        <v>23345</v>
-      </c>
-      <c r="F24" s="79">
-        <v>6</v>
-      </c>
-      <c r="G24" s="79"/>
-      <c r="H24" s="79">
-        <v>96</v>
-      </c>
-      <c r="I24" s="79">
-        <v>59</v>
-      </c>
-      <c r="J24" s="79">
-        <v>0</v>
-      </c>
-      <c r="K24" s="79">
-        <v>800</v>
-      </c>
-      <c r="L24" s="79">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="78">
-        <v>43914</v>
-      </c>
-      <c r="B25" s="79">
-        <v>411</v>
-      </c>
-      <c r="C25" s="79">
-        <v>0</v>
-      </c>
-      <c r="D25" s="79">
-        <v>25000</v>
-      </c>
-      <c r="E25" s="79">
-        <v>24589</v>
-      </c>
-      <c r="F25" s="79"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79">
-        <v>113</v>
-      </c>
-      <c r="I25" s="79">
-        <v>56</v>
-      </c>
-      <c r="J25" s="79">
-        <v>0</v>
-      </c>
-      <c r="K25" s="79">
-        <v>1300</v>
-      </c>
-      <c r="L25" s="79">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="78">
-        <v>43915</v>
-      </c>
-      <c r="B26" s="79">
-        <v>466</v>
-      </c>
-      <c r="C26" s="79">
-        <v>0</v>
-      </c>
-      <c r="D26" s="79">
-        <v>25500</v>
-      </c>
-      <c r="E26" s="79">
-        <v>25034</v>
-      </c>
-      <c r="F26" s="79"/>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79">
-        <v>128</v>
-      </c>
-      <c r="I26" s="79">
-        <v>55</v>
-      </c>
-      <c r="J26" s="79">
-        <v>0</v>
-      </c>
-      <c r="K26" s="79">
-        <v>500</v>
-      </c>
-      <c r="L26" s="79">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="78">
-        <v>43916</v>
-      </c>
-      <c r="B27" s="79">
-        <v>520</v>
-      </c>
-      <c r="C27" s="79">
-        <v>2</v>
-      </c>
-      <c r="D27" s="79">
-        <v>26900</v>
-      </c>
-      <c r="E27" s="79">
-        <v>26380</v>
-      </c>
-      <c r="F27" s="79"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79">
-        <v>149</v>
-      </c>
-      <c r="I27" s="79">
-        <v>54</v>
-      </c>
-      <c r="J27" s="79">
-        <v>2</v>
-      </c>
-      <c r="K27" s="79">
-        <v>1400</v>
-      </c>
-      <c r="L27" s="79">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="78">
-        <v>43917</v>
-      </c>
-      <c r="B28" s="79">
-        <v>574</v>
-      </c>
-      <c r="C28" s="79">
-        <v>3</v>
-      </c>
-      <c r="D28" s="79">
-        <v>27800</v>
-      </c>
-      <c r="E28" s="79">
-        <v>27226</v>
-      </c>
-      <c r="F28" s="79"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79">
-        <v>172</v>
-      </c>
-      <c r="I28" s="79">
-        <v>54</v>
-      </c>
-      <c r="J28" s="79">
-        <v>1</v>
-      </c>
-      <c r="K28" s="79">
-        <v>900</v>
-      </c>
-      <c r="L28" s="79">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="78">
-        <v>43918</v>
-      </c>
-      <c r="B29" s="79">
-        <v>685</v>
-      </c>
-      <c r="C29" s="79">
-        <v>4</v>
-      </c>
-      <c r="D29" s="79">
-        <v>35000</v>
-      </c>
-      <c r="E29" s="79">
-        <v>34315</v>
-      </c>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79">
-        <v>191</v>
-      </c>
-      <c r="I29" s="79">
-        <v>111</v>
-      </c>
-      <c r="J29" s="79">
-        <v>1</v>
-      </c>
-      <c r="K29" s="79">
-        <v>7200</v>
-      </c>
-      <c r="L29" s="79">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="78">
-        <v>43919</v>
-      </c>
-      <c r="B30" s="79">
-        <v>769</v>
-      </c>
-      <c r="C30" s="79">
-        <v>4</v>
-      </c>
-      <c r="D30" s="79">
-        <v>39000</v>
-      </c>
-      <c r="E30" s="79">
-        <v>38231</v>
-      </c>
-      <c r="F30" s="79">
-        <v>26</v>
-      </c>
-      <c r="G30" s="79">
-        <v>4</v>
-      </c>
-      <c r="H30" s="79">
-        <v>193</v>
-      </c>
-      <c r="I30" s="79">
-        <v>84</v>
-      </c>
-      <c r="J30" s="79">
-        <v>0</v>
-      </c>
-      <c r="K30" s="79">
-        <v>4000</v>
-      </c>
-      <c r="L30" s="79">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="78">
-        <v>43920</v>
-      </c>
-      <c r="B31" s="79">
-        <v>821</v>
-      </c>
-      <c r="C31" s="79">
-        <v>4</v>
-      </c>
-      <c r="D31" s="79">
-        <v>42000</v>
-      </c>
-      <c r="E31" s="79">
-        <v>41179</v>
-      </c>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79">
-        <v>4</v>
-      </c>
-      <c r="H31" s="79">
-        <v>248</v>
-      </c>
-      <c r="I31" s="79">
-        <v>52</v>
-      </c>
-      <c r="J31" s="79">
-        <v>0</v>
-      </c>
-      <c r="K31" s="79">
-        <v>3000</v>
-      </c>
-      <c r="L31" s="79">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="78">
-        <v>43921</v>
-      </c>
-      <c r="B32" s="79">
-        <v>917</v>
-      </c>
-      <c r="C32" s="79">
-        <v>4</v>
-      </c>
-      <c r="D32" s="79">
-        <v>45000</v>
-      </c>
-      <c r="E32" s="79">
-        <v>44083</v>
-      </c>
-      <c r="F32" s="79">
-        <v>29</v>
-      </c>
-      <c r="G32" s="79">
-        <v>4</v>
-      </c>
-      <c r="H32" s="79">
-        <v>291</v>
-      </c>
-      <c r="I32" s="79">
-        <v>96</v>
-      </c>
-      <c r="J32" s="79">
-        <v>0</v>
-      </c>
-      <c r="K32" s="79">
-        <v>3000</v>
-      </c>
-      <c r="L32" s="79">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="78">
-        <v>43922</v>
-      </c>
-      <c r="B33" s="79">
-        <v>968</v>
-      </c>
-      <c r="C33" s="79">
-        <v>5</v>
-      </c>
-      <c r="D33" s="79">
-        <v>47000</v>
-      </c>
-      <c r="E33" s="79">
-        <v>46032</v>
-      </c>
-      <c r="F33" s="79">
-        <v>32</v>
-      </c>
-      <c r="G33" s="79">
-        <v>6</v>
-      </c>
-      <c r="H33" s="79">
-        <v>343</v>
-      </c>
-      <c r="I33" s="79">
-        <v>51</v>
-      </c>
-      <c r="J33" s="79">
-        <v>1</v>
-      </c>
-      <c r="K33" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L33" s="79">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="78">
-        <v>43923</v>
-      </c>
-      <c r="B34" s="79">
-        <v>1036</v>
-      </c>
-      <c r="C34" s="79">
-        <v>6</v>
-      </c>
-      <c r="D34" s="79">
-        <v>49000</v>
-      </c>
-      <c r="E34" s="79">
-        <v>47964</v>
-      </c>
-      <c r="F34" s="79">
-        <v>34</v>
-      </c>
-      <c r="G34" s="79">
-        <v>6</v>
-      </c>
-      <c r="H34" s="79">
-        <v>422</v>
-      </c>
-      <c r="I34" s="79">
-        <v>68</v>
-      </c>
-      <c r="J34" s="79">
-        <v>1</v>
-      </c>
-      <c r="K34" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L34" s="79">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="78">
-        <v>43924</v>
-      </c>
-      <c r="B35" s="79">
-        <v>1085</v>
-      </c>
-      <c r="C35" s="79">
-        <v>7</v>
-      </c>
-      <c r="D35" s="79">
-        <v>51000</v>
-      </c>
-      <c r="E35" s="79">
-        <v>49915</v>
-      </c>
-      <c r="F35" s="79">
-        <v>37</v>
-      </c>
-      <c r="G35" s="79">
-        <v>7</v>
-      </c>
-      <c r="H35" s="79">
-        <v>476</v>
-      </c>
-      <c r="I35" s="79">
-        <v>49</v>
-      </c>
-      <c r="J35" s="79">
-        <v>1</v>
-      </c>
-      <c r="K35" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L35" s="79">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="78">
-        <v>43925</v>
-      </c>
-      <c r="B36" s="79">
-        <v>1115</v>
-      </c>
-      <c r="C36" s="79">
-        <v>8</v>
-      </c>
-      <c r="D36" s="79">
-        <v>54000</v>
-      </c>
-      <c r="E36" s="79">
-        <v>52885</v>
-      </c>
-      <c r="F36" s="79">
-        <v>42</v>
-      </c>
-      <c r="G36" s="79">
-        <v>10</v>
-      </c>
-      <c r="H36" s="79">
-        <v>527</v>
-      </c>
-      <c r="I36" s="79">
-        <v>30</v>
-      </c>
-      <c r="J36" s="79">
-        <v>1</v>
-      </c>
-      <c r="K36" s="79">
-        <v>3000</v>
-      </c>
-      <c r="L36" s="79">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="78">
-        <v>43926</v>
-      </c>
-      <c r="B37" s="79">
-        <v>1135</v>
-      </c>
-      <c r="C37" s="79">
-        <v>8</v>
-      </c>
-      <c r="D37" s="79">
-        <v>56000</v>
-      </c>
-      <c r="E37" s="79">
-        <v>54865</v>
-      </c>
-      <c r="F37" s="79">
-        <v>47</v>
-      </c>
-      <c r="G37" s="79">
-        <v>11</v>
-      </c>
-      <c r="H37" s="79">
-        <v>573</v>
-      </c>
-      <c r="I37" s="79">
-        <v>20</v>
-      </c>
-      <c r="J37" s="79">
-        <v>0</v>
-      </c>
-      <c r="K37" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L37" s="79">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="78">
-        <v>43927</v>
-      </c>
-      <c r="B38" s="79">
-        <v>1158</v>
-      </c>
-      <c r="C38" s="79">
-        <v>10</v>
-      </c>
-      <c r="D38" s="79">
-        <v>57000</v>
-      </c>
-      <c r="E38" s="79">
-        <v>55842</v>
-      </c>
-      <c r="F38" s="79">
-        <v>45</v>
-      </c>
-      <c r="G38" s="79">
-        <v>11</v>
-      </c>
-      <c r="H38" s="79">
-        <v>620</v>
-      </c>
-      <c r="I38" s="79">
-        <v>23</v>
-      </c>
-      <c r="J38" s="79">
-        <v>2</v>
-      </c>
-      <c r="K38" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L38" s="79">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="78">
-        <v>43928</v>
-      </c>
-      <c r="B39" s="79">
-        <v>1191</v>
-      </c>
-      <c r="C39" s="79">
-        <v>11</v>
-      </c>
-      <c r="D39" s="79">
-        <v>58000</v>
-      </c>
-      <c r="E39" s="79">
-        <v>56809</v>
-      </c>
-      <c r="F39" s="79">
-        <v>47</v>
-      </c>
-      <c r="G39" s="79">
-        <v>13</v>
-      </c>
-      <c r="H39" s="79">
-        <v>686</v>
-      </c>
-      <c r="I39" s="79">
-        <v>33</v>
-      </c>
-      <c r="J39" s="79">
-        <v>1</v>
-      </c>
-      <c r="K39" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L39" s="79">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="78">
-        <v>43929</v>
-      </c>
-      <c r="B40" s="79">
-        <v>1212</v>
-      </c>
-      <c r="C40" s="79">
-        <v>12</v>
-      </c>
-      <c r="D40" s="79">
-        <v>60000</v>
-      </c>
-      <c r="E40" s="79">
-        <v>58788</v>
-      </c>
-      <c r="F40" s="79">
-        <v>45</v>
-      </c>
-      <c r="G40" s="79">
-        <v>12</v>
-      </c>
-      <c r="H40" s="79">
-        <v>736</v>
-      </c>
-      <c r="I40" s="79">
-        <v>21</v>
-      </c>
-      <c r="J40" s="79">
-        <v>1</v>
-      </c>
-      <c r="K40" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L40" s="79">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="78">
-        <v>43930</v>
-      </c>
-      <c r="B41" s="79">
-        <v>1228</v>
-      </c>
-      <c r="C41" s="79">
-        <v>12</v>
-      </c>
-      <c r="D41" s="79">
-        <v>62000</v>
-      </c>
-      <c r="E41" s="79">
-        <v>60772</v>
-      </c>
-      <c r="F41" s="79">
-        <v>50</v>
-      </c>
-      <c r="G41" s="79">
-        <v>13</v>
-      </c>
-      <c r="H41" s="79">
-        <v>806</v>
-      </c>
-      <c r="I41" s="79">
-        <v>16</v>
-      </c>
-      <c r="J41" s="79">
-        <v>0</v>
-      </c>
-      <c r="K41" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L41" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="78">
-        <v>43931</v>
-      </c>
-      <c r="B42" s="79">
-        <v>1241</v>
-      </c>
-      <c r="C42" s="79">
-        <v>13</v>
-      </c>
-      <c r="D42" s="79">
-        <v>65000</v>
-      </c>
-      <c r="E42" s="79">
-        <v>63759</v>
-      </c>
-      <c r="F42" s="79">
-        <v>43</v>
-      </c>
-      <c r="G42" s="79">
-        <v>13</v>
-      </c>
-      <c r="H42" s="79">
-        <v>926</v>
-      </c>
-      <c r="I42" s="79">
-        <v>13</v>
-      </c>
-      <c r="J42" s="79">
-        <v>1</v>
-      </c>
-      <c r="K42" s="79">
-        <v>3000</v>
-      </c>
-      <c r="L42" s="79">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="78">
-        <v>43932</v>
-      </c>
-      <c r="B43" s="79">
-        <v>1265</v>
-      </c>
-      <c r="C43" s="79">
-        <v>14</v>
-      </c>
-      <c r="D43" s="79">
-        <v>67000</v>
-      </c>
-      <c r="E43" s="79">
-        <v>65735</v>
-      </c>
-      <c r="F43" s="79">
-        <v>44</v>
-      </c>
-      <c r="G43" s="79">
-        <v>15</v>
-      </c>
-      <c r="H43" s="79">
-        <v>986</v>
-      </c>
-      <c r="I43" s="79">
-        <v>24</v>
-      </c>
-      <c r="J43" s="79">
-        <v>1</v>
-      </c>
-      <c r="K43" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L43" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="78">
-        <v>43933</v>
-      </c>
-      <c r="B44" s="79">
-        <v>1268</v>
-      </c>
-      <c r="C44" s="79">
-        <v>14</v>
-      </c>
-      <c r="D44" s="79">
-        <v>69000</v>
-      </c>
-      <c r="E44" s="79">
-        <v>67732</v>
-      </c>
-      <c r="F44" s="79">
-        <v>44</v>
-      </c>
-      <c r="G44" s="79">
-        <v>16</v>
-      </c>
-      <c r="H44" s="79">
-        <v>1015</v>
-      </c>
-      <c r="I44" s="79">
-        <v>3</v>
-      </c>
-      <c r="J44" s="79">
-        <v>0</v>
-      </c>
-      <c r="K44" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L44" s="79">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="78">
-        <v>43934</v>
-      </c>
-      <c r="B45" s="79">
-        <v>1281</v>
-      </c>
-      <c r="C45" s="79">
-        <v>14</v>
-      </c>
-      <c r="D45" s="79">
-        <v>70000</v>
-      </c>
-      <c r="E45" s="79">
-        <v>68719</v>
-      </c>
-      <c r="F45" s="79">
-        <v>40</v>
-      </c>
-      <c r="G45" s="79">
-        <v>14</v>
-      </c>
-      <c r="H45" s="79">
-        <v>1075</v>
-      </c>
-      <c r="I45" s="79">
-        <v>13</v>
-      </c>
-      <c r="J45" s="79">
-        <v>0</v>
-      </c>
-      <c r="K45" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L45" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="78">
-        <v>43935</v>
-      </c>
-      <c r="B46" s="79">
-        <v>1291</v>
-      </c>
-      <c r="C46" s="79">
-        <v>14</v>
-      </c>
-      <c r="D46" s="79">
-        <v>71000</v>
-      </c>
-      <c r="E46" s="79">
-        <v>69709</v>
-      </c>
-      <c r="F46" s="79">
-        <v>40</v>
-      </c>
-      <c r="G46" s="79">
-        <v>15</v>
-      </c>
-      <c r="H46" s="79">
-        <v>1118</v>
-      </c>
-      <c r="I46" s="79">
-        <v>10</v>
-      </c>
-      <c r="J46" s="79">
-        <v>0</v>
-      </c>
-      <c r="K46" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L46" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="78">
-        <v>43936</v>
-      </c>
-      <c r="B47" s="79">
-        <v>1299</v>
-      </c>
-      <c r="C47" s="79">
-        <v>14</v>
-      </c>
-      <c r="D47" s="79">
-        <v>72000</v>
-      </c>
-      <c r="E47" s="79">
-        <v>70701</v>
-      </c>
-      <c r="F47" s="79">
-        <v>39</v>
-      </c>
-      <c r="G47" s="79">
-        <v>18</v>
-      </c>
-      <c r="H47" s="79">
-        <v>1137</v>
-      </c>
-      <c r="I47" s="79">
-        <v>8</v>
-      </c>
-      <c r="J47" s="79">
-        <v>0</v>
-      </c>
-      <c r="K47" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L47" s="79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="78">
-        <v>43937</v>
-      </c>
-      <c r="B48" s="79">
-        <v>1301</v>
-      </c>
-      <c r="C48" s="79">
-        <v>14</v>
-      </c>
-      <c r="D48" s="79">
-        <v>73000</v>
-      </c>
-      <c r="E48" s="79">
-        <v>71699</v>
-      </c>
-      <c r="F48" s="79">
-        <v>39</v>
-      </c>
-      <c r="G48" s="79">
-        <v>18</v>
-      </c>
-      <c r="H48" s="79">
-        <v>1153</v>
-      </c>
-      <c r="I48" s="79">
-        <v>2</v>
-      </c>
-      <c r="J48" s="79">
-        <v>0</v>
-      </c>
-      <c r="K48" s="79">
-        <v>1000</v>
-      </c>
-      <c r="L48" s="79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="78">
-        <v>43938</v>
-      </c>
-      <c r="B49" s="79">
-        <v>1302</v>
-      </c>
-      <c r="C49" s="79">
-        <v>14</v>
-      </c>
-      <c r="D49" s="79">
-        <v>75000</v>
-      </c>
-      <c r="E49" s="79">
-        <v>73698</v>
-      </c>
-      <c r="F49" s="79">
-        <v>32</v>
-      </c>
-      <c r="G49" s="79">
-        <v>13</v>
-      </c>
-      <c r="H49" s="79">
-        <v>1159</v>
-      </c>
-      <c r="I49" s="79">
-        <v>1</v>
-      </c>
-      <c r="J49" s="79">
-        <v>0</v>
-      </c>
-      <c r="K49" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L49" s="79">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="78">
-        <v>43939</v>
-      </c>
-      <c r="B50" s="79">
-        <v>1319</v>
-      </c>
-      <c r="C50" s="79">
-        <v>14</v>
-      </c>
-      <c r="D50" s="79">
-        <v>79000</v>
-      </c>
-      <c r="E50" s="79">
-        <v>77681</v>
-      </c>
-      <c r="F50" s="79">
-        <v>30</v>
-      </c>
-      <c r="G50" s="79">
-        <v>12</v>
-      </c>
-      <c r="H50" s="79">
-        <v>1172</v>
-      </c>
-      <c r="I50" s="79">
-        <v>17</v>
-      </c>
-      <c r="J50" s="79">
-        <v>0</v>
-      </c>
-      <c r="K50" s="79">
-        <v>4000</v>
-      </c>
-      <c r="L50" s="79">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="78">
-        <v>43940</v>
-      </c>
-      <c r="B51" s="79">
-        <v>1328</v>
-      </c>
-      <c r="C51" s="79">
-        <v>15</v>
-      </c>
-      <c r="D51" s="79">
-        <v>82000</v>
-      </c>
-      <c r="E51" s="79">
-        <v>80672</v>
-      </c>
-      <c r="F51" s="79">
-        <v>29</v>
-      </c>
-      <c r="G51" s="79">
-        <v>10</v>
-      </c>
-      <c r="H51" s="79">
-        <v>1188</v>
-      </c>
-      <c r="I51" s="79">
-        <v>9</v>
-      </c>
-      <c r="J51" s="79">
-        <v>1</v>
-      </c>
-      <c r="K51" s="79">
-        <v>3000</v>
-      </c>
-      <c r="L51" s="79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="78">
-        <v>43941</v>
-      </c>
-      <c r="B52" s="79">
-        <v>1329</v>
-      </c>
-      <c r="C52" s="79">
-        <v>15</v>
-      </c>
-      <c r="D52" s="79">
-        <v>86000</v>
-      </c>
-      <c r="E52" s="79">
-        <v>84671</v>
-      </c>
-      <c r="F52" s="79">
-        <v>28</v>
-      </c>
-      <c r="G52" s="79">
-        <v>11</v>
-      </c>
-      <c r="H52" s="79">
-        <v>1196</v>
-      </c>
-      <c r="I52" s="79">
-        <v>1</v>
-      </c>
-      <c r="J52" s="79">
-        <v>0</v>
-      </c>
-      <c r="K52" s="79">
-        <v>4000</v>
-      </c>
-      <c r="L52" s="79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="78">
-        <v>43942</v>
-      </c>
-      <c r="B53" s="79">
-        <v>1336</v>
-      </c>
-      <c r="C53" s="79">
-        <v>15</v>
-      </c>
-      <c r="D53" s="79">
-        <v>88000</v>
-      </c>
-      <c r="E53" s="79">
-        <v>86664</v>
-      </c>
-      <c r="F53" s="79">
-        <v>28</v>
-      </c>
-      <c r="G53" s="79">
-        <v>12</v>
-      </c>
-      <c r="H53" s="79">
-        <v>1202</v>
-      </c>
-      <c r="I53" s="79">
-        <v>7</v>
-      </c>
-      <c r="J53" s="79">
-        <v>0</v>
-      </c>
-      <c r="K53" s="79">
-        <v>2000</v>
-      </c>
-      <c r="L53" s="79">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3870F7-A576-4BD3-9D23-1C9E10583711}">
   <dimension ref="A1:D8"/>
   <sheetViews>

</xml_diff>